<commit_message>
remade model. May need to reduce thresh_lower
</commit_message>
<xml_diff>
--- a/decision_data_new.xlsx
+++ b/decision_data_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/paul_kumar_mail_utoronto_ca/Documents/engineering_masters/thesis work/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="164" documentId="6_{F6B86153-F216-4926-93F2-3946DCDAA96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{91BC6516-32D4-4668-8BB0-A1AFE73EABBD}"/>
+  <xr:revisionPtr revIDLastSave="171" documentId="6_{F6B86153-F216-4926-93F2-3946DCDAA96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{921B34C7-CC24-4494-B553-1A937B87BEF0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wall_mounted_data" sheetId="12" r:id="rId1"/>
@@ -21,24 +21,21 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">wall_mounted_data!$B$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">wall_mounted_data!$E$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">wall_mounted_data!$E$2:$E$320</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">wall_mounted_data!$F$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">wall_mounted_data!$F$2:$F$320</definedName>
     <definedName name="_xlchart.v1.12" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">wall_mounted_data!$D$1</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">wall_mounted_data!$D$2:$D$320</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">wall_mounted_data!$E$1</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">wall_mounted_data!$E$2:$E$320</definedName>
     <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$A$2:$A$150</definedName>
     <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$B$1</definedName>
     <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$B$2:$B$150</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$A$2:$A$150</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$B$1</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">wall_mounted_data!$B$2:$B$320</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$B$2:$B$150</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">wall_mounted_data!$C$1</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">wall_mounted_data!$C$2:$C$320</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">wall_mounted_data!$F$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">wall_mounted_data!$F$2:$F$320</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">wall_mounted_data!$D$1</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">wall_mounted_data!$D$2:$D$320</definedName>
     <definedName name="_xlchart.v1.9" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -46,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="12">
   <si>
     <t>first_peak</t>
   </si>
@@ -82,12 +79,6 @@
   </si>
   <si>
     <t>1-hot_second_last</t>
-  </si>
-  <si>
-    <t>1-hot-first_2</t>
-  </si>
-  <si>
-    <t>1-hot_last_2</t>
   </si>
 </sst>
 </file>
@@ -778,10 +769,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.12</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.14</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -819,7 +810,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{2E007EC1-CE09-47B1-A3E4-A95E48D1BADB}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.13</cx:f>
+              <cx:f>_xlchart.v1.7</cx:f>
               <cx:v>second_last_peak</cx:v>
             </cx:txData>
           </cx:tx>
@@ -849,10 +840,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.12</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.11</cx:f>
+        <cx:f>_xlchart.v1.14</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -890,7 +881,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{28AFBDCB-EA5A-4D8B-B5F8-DF1924715131}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.10</cx:f>
+              <cx:f>_xlchart.v1.13</cx:f>
               <cx:v>last_peak</cx:v>
             </cx:txData>
           </cx:tx>
@@ -920,10 +911,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -961,7 +952,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{02F72712-9CA3-4436-A6ED-93C80B1901DF}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.7</cx:f>
+              <cx:f>_xlchart.v1.10</cx:f>
               <cx:v>Gradient_1</cx:v>
             </cx:txData>
           </cx:tx>
@@ -991,10 +982,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.18</cx:f>
+        <cx:f>_xlchart.v1.15</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.20</cx:f>
+        <cx:f>_xlchart.v1.17</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1005,7 +996,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{1ED9ED9D-8B6C-434A-9689-07BDF3F028CE}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.19</cx:f>
+              <cx:f>_xlchart.v1.16</cx:f>
               <cx:v>first_peak</cx:v>
             </cx:txData>
           </cx:tx>
@@ -17206,15 +17197,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A2C5052-2A6F-49B6-97B4-305C293E194C}">
-  <dimension ref="A1:H147"/>
+  <dimension ref="A1:F145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H38" sqref="H25:H38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -17225,22 +17220,16 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -17251,22 +17240,16 @@
         <v>0.118967393</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -17277,22 +17260,16 @@
         <v>0.145104488</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -17306,19 +17283,13 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -17329,22 +17300,16 @@
         <v>-0.33530743600000001</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -17358,19 +17323,13 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -17384,19 +17343,13 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -17407,22 +17360,16 @@
         <v>-0.34055490799999999</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -17433,22 +17380,16 @@
         <v>7.4506949000000003E-2</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -17462,19 +17403,13 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -17485,22 +17420,16 @@
         <v>0.25041475299999999</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -17514,19 +17443,13 @@
         <v>1</v>
       </c>
       <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -17537,22 +17460,16 @@
         <v>4.4362171999999998E-2</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -17566,19 +17483,13 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -17589,22 +17500,16 @@
         <v>0.250621759</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -17618,19 +17523,13 @@
         <v>1</v>
       </c>
       <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -17641,22 +17540,16 @@
         <v>0.14714822499999999</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -17672,17 +17565,11 @@
       <c r="E18">
         <v>0</v>
       </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -17693,22 +17580,16 @@
         <v>0.20586744900000001</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-      <c r="H19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0</v>
       </c>
@@ -17722,19 +17603,13 @@
         <v>1</v>
       </c>
       <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -17745,22 +17620,16 @@
         <v>-7.1472360000000004E-3</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-      <c r="H21" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -17771,22 +17640,16 @@
         <v>-0.39146710099999998</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -17797,22 +17660,16 @@
         <v>0.49096794599999999</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-      <c r="H23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -17823,22 +17680,16 @@
         <v>-0.401706695</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
@@ -17852,19 +17703,13 @@
         <v>1</v>
       </c>
       <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
-      <c r="H25" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -17875,22 +17720,16 @@
         <v>-0.31057901500000001</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -17904,19 +17743,13 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
-      <c r="H27" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0</v>
       </c>
@@ -17927,22 +17760,16 @@
         <v>-5.9575818000000003E-2</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28">
         <v>1</v>
       </c>
-      <c r="F28">
-        <v>1</v>
-      </c>
-      <c r="G28">
-        <v>1</v>
-      </c>
-      <c r="H28" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -17953,22 +17780,16 @@
         <v>0.42907381300000003</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>1</v>
-      </c>
-      <c r="H29" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0</v>
       </c>
@@ -17982,19 +17803,13 @@
         <v>1</v>
       </c>
       <c r="E30">
-        <v>1</v>
-      </c>
-      <c r="F30">
-        <v>1</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1</v>
       </c>
@@ -18005,22 +17820,16 @@
         <v>0.356441701</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
-      <c r="H31" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0</v>
       </c>
@@ -18031,22 +17840,16 @@
         <v>-0.36295447600000003</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32">
-        <v>1</v>
-      </c>
-      <c r="F32">
-        <v>1</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
@@ -18060,19 +17863,13 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-      <c r="G33">
-        <v>1</v>
-      </c>
-      <c r="H33" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0</v>
       </c>
@@ -18086,19 +17883,13 @@
         <v>1</v>
       </c>
       <c r="E34">
-        <v>1</v>
-      </c>
-      <c r="F34">
-        <v>1</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1</v>
       </c>
@@ -18114,17 +17905,11 @@
       <c r="E35">
         <v>1</v>
       </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-      <c r="G35">
-        <v>1</v>
-      </c>
-      <c r="H35" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0</v>
       </c>
@@ -18138,19 +17923,13 @@
         <v>1</v>
       </c>
       <c r="E36">
-        <v>1</v>
-      </c>
-      <c r="F36">
-        <v>1</v>
-      </c>
-      <c r="G36">
-        <v>0</v>
-      </c>
-      <c r="H36" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F36" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1</v>
       </c>
@@ -18161,22 +17940,16 @@
         <v>0.490613892</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E37">
         <v>0</v>
       </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-      <c r="H37" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>0</v>
       </c>
@@ -18187,22 +17960,16 @@
         <v>-0.21272780499999999</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38">
-        <v>1</v>
-      </c>
-      <c r="F38">
-        <v>1</v>
-      </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-      <c r="H38" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>0</v>
       </c>
@@ -18213,22 +17980,16 @@
         <v>-0.19471264799999999</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39">
-        <v>1</v>
-      </c>
-      <c r="F39">
-        <v>1</v>
-      </c>
-      <c r="G39">
-        <v>0</v>
-      </c>
-      <c r="H39" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>0</v>
       </c>
@@ -18239,22 +18000,16 @@
         <v>8.1387119999999993E-3</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40">
-        <v>1</v>
-      </c>
-      <c r="G40">
-        <v>1</v>
-      </c>
-      <c r="H40" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1</v>
       </c>
@@ -18268,19 +18023,13 @@
         <v>0</v>
       </c>
       <c r="E41">
-        <v>1</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="H41" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>0</v>
       </c>
@@ -18296,17 +18045,11 @@
       <c r="E42">
         <v>1</v>
       </c>
-      <c r="F42">
-        <v>1</v>
-      </c>
-      <c r="G42">
-        <v>1</v>
-      </c>
-      <c r="H42" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1</v>
       </c>
@@ -18320,19 +18063,13 @@
         <v>0</v>
       </c>
       <c r="E43">
-        <v>1</v>
-      </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
-      <c r="G43">
-        <v>0</v>
-      </c>
-      <c r="H43" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F43" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1</v>
       </c>
@@ -18348,17 +18085,11 @@
       <c r="E44">
         <v>1</v>
       </c>
-      <c r="F44">
-        <v>0</v>
-      </c>
-      <c r="G44">
-        <v>1</v>
-      </c>
-      <c r="H44" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F44" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1</v>
       </c>
@@ -18372,19 +18103,13 @@
         <v>0</v>
       </c>
       <c r="E45">
-        <v>1</v>
-      </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-      <c r="G45">
-        <v>0</v>
-      </c>
-      <c r="H45" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F45" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1</v>
       </c>
@@ -18395,22 +18120,16 @@
         <v>0.51047199600000004</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E46">
-        <v>0</v>
-      </c>
-      <c r="F46">
-        <v>0</v>
-      </c>
-      <c r="G46">
-        <v>1</v>
-      </c>
-      <c r="H46" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>0</v>
       </c>
@@ -18426,17 +18145,11 @@
       <c r="E47">
         <v>0</v>
       </c>
-      <c r="F47">
-        <v>1</v>
-      </c>
-      <c r="G47">
-        <v>0</v>
-      </c>
-      <c r="H47" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F47" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>0</v>
       </c>
@@ -18450,19 +18163,13 @@
         <v>1</v>
       </c>
       <c r="E48">
-        <v>0</v>
-      </c>
-      <c r="F48">
-        <v>1</v>
-      </c>
-      <c r="G48">
-        <v>1</v>
-      </c>
-      <c r="H48" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F48" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>0</v>
       </c>
@@ -18476,19 +18183,13 @@
         <v>1</v>
       </c>
       <c r="E49">
-        <v>1</v>
-      </c>
-      <c r="F49">
-        <v>1</v>
-      </c>
-      <c r="G49">
-        <v>0</v>
-      </c>
-      <c r="H49" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F49" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1</v>
       </c>
@@ -18502,19 +18203,13 @@
         <v>0</v>
       </c>
       <c r="E50">
-        <v>0</v>
-      </c>
-      <c r="F50">
-        <v>0</v>
-      </c>
-      <c r="G50">
-        <v>1</v>
-      </c>
-      <c r="H50" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F50" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>0</v>
       </c>
@@ -18525,22 +18220,16 @@
         <v>-0.15760224</v>
       </c>
       <c r="D51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E51">
         <v>0</v>
       </c>
-      <c r="F51">
-        <v>1</v>
-      </c>
-      <c r="G51">
-        <v>0</v>
-      </c>
-      <c r="H51" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F51" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1</v>
       </c>
@@ -18551,22 +18240,16 @@
         <v>-3.5866759999999998E-2</v>
       </c>
       <c r="D52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E52">
         <v>0</v>
       </c>
-      <c r="F52">
-        <v>0</v>
-      </c>
-      <c r="G52">
-        <v>0</v>
-      </c>
-      <c r="H52" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F52" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>0</v>
       </c>
@@ -18577,22 +18260,16 @@
         <v>-0.32771599400000001</v>
       </c>
       <c r="D53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E53">
-        <v>1</v>
-      </c>
-      <c r="F53">
-        <v>1</v>
-      </c>
-      <c r="G53">
-        <v>0</v>
-      </c>
-      <c r="H53" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F53" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1</v>
       </c>
@@ -18603,22 +18280,16 @@
         <v>0.15997613499999999</v>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E54">
-        <v>0</v>
-      </c>
-      <c r="F54">
-        <v>0</v>
-      </c>
-      <c r="G54">
-        <v>1</v>
-      </c>
-      <c r="H54" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F54" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>0</v>
       </c>
@@ -18632,19 +18303,13 @@
         <v>1</v>
       </c>
       <c r="E55">
-        <v>1</v>
-      </c>
-      <c r="F55">
-        <v>1</v>
-      </c>
-      <c r="G55">
-        <v>0</v>
-      </c>
-      <c r="H55" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F55" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1</v>
       </c>
@@ -18655,22 +18320,16 @@
         <v>0.39515518799999999</v>
       </c>
       <c r="D56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E56">
-        <v>0</v>
-      </c>
-      <c r="F56">
-        <v>0</v>
-      </c>
-      <c r="G56">
-        <v>1</v>
-      </c>
-      <c r="H56" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F56" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>0</v>
       </c>
@@ -18686,17 +18345,11 @@
       <c r="E57">
         <v>0</v>
       </c>
-      <c r="F57">
-        <v>1</v>
-      </c>
-      <c r="G57">
-        <v>0</v>
-      </c>
-      <c r="H57" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F57" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1</v>
       </c>
@@ -18707,22 +18360,16 @@
         <v>0.31894950100000002</v>
       </c>
       <c r="D58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E58">
-        <v>0</v>
-      </c>
-      <c r="F58">
-        <v>0</v>
-      </c>
-      <c r="G58">
-        <v>1</v>
-      </c>
-      <c r="H58" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F58" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1</v>
       </c>
@@ -18733,22 +18380,16 @@
         <v>-0.36195993799999998</v>
       </c>
       <c r="D59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E59">
-        <v>1</v>
-      </c>
-      <c r="F59">
-        <v>0</v>
-      </c>
-      <c r="G59">
-        <v>0</v>
-      </c>
-      <c r="H59" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>0</v>
       </c>
@@ -18764,17 +18405,11 @@
       <c r="E60">
         <v>1</v>
       </c>
-      <c r="F60">
-        <v>1</v>
-      </c>
-      <c r="G60">
-        <v>1</v>
-      </c>
-      <c r="H60" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F60" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>0</v>
       </c>
@@ -18788,19 +18423,13 @@
         <v>1</v>
       </c>
       <c r="E61">
-        <v>0</v>
-      </c>
-      <c r="F61">
-        <v>1</v>
-      </c>
-      <c r="G61">
-        <v>1</v>
-      </c>
-      <c r="H61" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F61" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>0</v>
       </c>
@@ -18811,22 +18440,16 @@
         <v>-0.312974209</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E62">
-        <v>1</v>
-      </c>
-      <c r="F62">
-        <v>1</v>
-      </c>
-      <c r="G62">
-        <v>0</v>
-      </c>
-      <c r="H62" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F62" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1</v>
       </c>
@@ -18840,19 +18463,13 @@
         <v>0</v>
       </c>
       <c r="E63">
-        <v>0</v>
-      </c>
-      <c r="F63">
-        <v>0</v>
-      </c>
-      <c r="G63">
-        <v>1</v>
-      </c>
-      <c r="H63" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F63" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>0</v>
       </c>
@@ -18863,22 +18480,16 @@
         <v>-0.28855860700000002</v>
       </c>
       <c r="D64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E64">
-        <v>1</v>
-      </c>
-      <c r="F64">
-        <v>1</v>
-      </c>
-      <c r="G64">
-        <v>0</v>
-      </c>
-      <c r="H64" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F64" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>0</v>
       </c>
@@ -18889,22 +18500,16 @@
         <v>7.4074856999999994E-2</v>
       </c>
       <c r="D65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E65">
-        <v>0</v>
-      </c>
-      <c r="F65">
-        <v>1</v>
-      </c>
-      <c r="G65">
-        <v>1</v>
-      </c>
-      <c r="H65" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F65" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>0</v>
       </c>
@@ -18920,17 +18525,11 @@
       <c r="E66">
         <v>0</v>
       </c>
-      <c r="F66">
-        <v>1</v>
-      </c>
-      <c r="G66">
-        <v>0</v>
-      </c>
-      <c r="H66" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F66" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>1</v>
       </c>
@@ -18944,19 +18543,13 @@
         <v>0</v>
       </c>
       <c r="E67">
-        <v>0</v>
-      </c>
-      <c r="F67">
-        <v>0</v>
-      </c>
-      <c r="G67">
-        <v>1</v>
-      </c>
-      <c r="H67" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F67" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>0</v>
       </c>
@@ -18970,19 +18563,13 @@
         <v>1</v>
       </c>
       <c r="E68">
-        <v>1</v>
-      </c>
-      <c r="F68">
-        <v>1</v>
-      </c>
-      <c r="G68">
-        <v>0</v>
-      </c>
-      <c r="H68" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F68" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>1</v>
       </c>
@@ -18993,22 +18580,16 @@
         <v>0.40055660599999998</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E69">
         <v>1</v>
       </c>
-      <c r="F69">
-        <v>0</v>
-      </c>
-      <c r="G69">
-        <v>1</v>
-      </c>
-      <c r="H69" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F69" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>1</v>
       </c>
@@ -19019,22 +18600,16 @@
         <v>2.5868637999999999E-2</v>
       </c>
       <c r="D70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E70">
-        <v>1</v>
-      </c>
-      <c r="F70">
-        <v>0</v>
-      </c>
-      <c r="G70">
-        <v>0</v>
-      </c>
-      <c r="H70" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F70" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>1</v>
       </c>
@@ -19048,19 +18623,13 @@
         <v>0</v>
       </c>
       <c r="E71">
-        <v>0</v>
-      </c>
-      <c r="F71">
-        <v>0</v>
-      </c>
-      <c r="G71">
-        <v>1</v>
-      </c>
-      <c r="H71" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F71" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>0</v>
       </c>
@@ -19076,17 +18645,11 @@
       <c r="E72">
         <v>0</v>
       </c>
-      <c r="F72">
-        <v>1</v>
-      </c>
-      <c r="G72">
-        <v>0</v>
-      </c>
-      <c r="H72" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F72" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>1</v>
       </c>
@@ -19102,17 +18665,11 @@
       <c r="E73">
         <v>1</v>
       </c>
-      <c r="F73">
-        <v>0</v>
-      </c>
-      <c r="G73">
-        <v>1</v>
-      </c>
-      <c r="H73" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F73" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>0</v>
       </c>
@@ -19126,19 +18683,13 @@
         <v>1</v>
       </c>
       <c r="E74">
-        <v>1</v>
-      </c>
-      <c r="F74">
-        <v>1</v>
-      </c>
-      <c r="G74">
-        <v>0</v>
-      </c>
-      <c r="H74" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F74" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>1</v>
       </c>
@@ -19149,22 +18700,16 @@
         <v>2.5794583999999999E-2</v>
       </c>
       <c r="D75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E75">
-        <v>1</v>
-      </c>
-      <c r="F75">
-        <v>0</v>
-      </c>
-      <c r="G75">
-        <v>0</v>
-      </c>
-      <c r="H75" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F75" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>0</v>
       </c>
@@ -19180,17 +18725,11 @@
       <c r="E76">
         <v>0</v>
       </c>
-      <c r="F76">
-        <v>1</v>
-      </c>
-      <c r="G76">
-        <v>0</v>
-      </c>
-      <c r="H76" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F76" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>1</v>
       </c>
@@ -19201,22 +18740,16 @@
         <v>0.21401905900000001</v>
       </c>
       <c r="D77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E77">
         <v>1</v>
       </c>
-      <c r="F77">
-        <v>0</v>
-      </c>
-      <c r="G77">
-        <v>1</v>
-      </c>
-      <c r="H77" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F77" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>0</v>
       </c>
@@ -19230,19 +18763,13 @@
         <v>1</v>
       </c>
       <c r="E78">
-        <v>1</v>
-      </c>
-      <c r="F78">
-        <v>1</v>
-      </c>
-      <c r="G78">
-        <v>0</v>
-      </c>
-      <c r="H78" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F78" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>1</v>
       </c>
@@ -19256,19 +18783,13 @@
         <v>0</v>
       </c>
       <c r="E79">
-        <v>0</v>
-      </c>
-      <c r="F79">
-        <v>0</v>
-      </c>
-      <c r="G79">
-        <v>1</v>
-      </c>
-      <c r="H79" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F79" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>0</v>
       </c>
@@ -19279,22 +18800,16 @@
         <v>-0.191685567</v>
       </c>
       <c r="D80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E80">
-        <v>1</v>
-      </c>
-      <c r="F80">
-        <v>1</v>
-      </c>
-      <c r="G80">
-        <v>0</v>
-      </c>
-      <c r="H80" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F80" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>1</v>
       </c>
@@ -19305,22 +18820,16 @@
         <v>0.32181554000000001</v>
       </c>
       <c r="D81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E81">
-        <v>0</v>
-      </c>
-      <c r="F81">
-        <v>0</v>
-      </c>
-      <c r="G81">
-        <v>1</v>
-      </c>
-      <c r="H81" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F81" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>0</v>
       </c>
@@ -19331,22 +18840,16 @@
         <v>-0.206106399</v>
       </c>
       <c r="D82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E82">
-        <v>1</v>
-      </c>
-      <c r="F82">
-        <v>1</v>
-      </c>
-      <c r="G82">
-        <v>0</v>
-      </c>
-      <c r="H82" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F82" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>1</v>
       </c>
@@ -19362,17 +18865,11 @@
       <c r="E83">
         <v>1</v>
       </c>
-      <c r="F83">
-        <v>0</v>
-      </c>
-      <c r="G83">
-        <v>1</v>
-      </c>
-      <c r="H83" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F83" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>0</v>
       </c>
@@ -19388,17 +18885,11 @@
       <c r="E84">
         <v>0</v>
       </c>
-      <c r="F84">
-        <v>1</v>
-      </c>
-      <c r="G84">
-        <v>0</v>
-      </c>
-      <c r="H84" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F84" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>0</v>
       </c>
@@ -19409,22 +18900,16 @@
         <v>-5.4029550000000003E-2</v>
       </c>
       <c r="D85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E85">
         <v>1</v>
       </c>
-      <c r="F85">
-        <v>1</v>
-      </c>
-      <c r="G85">
-        <v>1</v>
-      </c>
-      <c r="H85" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F85" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>1</v>
       </c>
@@ -19440,17 +18925,11 @@
       <c r="E86">
         <v>0</v>
       </c>
-      <c r="F86">
-        <v>0</v>
-      </c>
-      <c r="G86">
-        <v>0</v>
-      </c>
-      <c r="H86" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F86" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>0</v>
       </c>
@@ -19464,19 +18943,13 @@
         <v>1</v>
       </c>
       <c r="E87">
-        <v>1</v>
-      </c>
-      <c r="F87">
-        <v>1</v>
-      </c>
-      <c r="G87">
-        <v>0</v>
-      </c>
-      <c r="H87" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F87" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>1</v>
       </c>
@@ -19487,22 +18960,16 @@
         <v>0.48340467399999998</v>
       </c>
       <c r="D88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E88">
-        <v>0</v>
-      </c>
-      <c r="F88">
-        <v>0</v>
-      </c>
-      <c r="G88">
-        <v>1</v>
-      </c>
-      <c r="H88" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F88" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>0</v>
       </c>
@@ -19516,19 +18983,13 @@
         <v>1</v>
       </c>
       <c r="E89">
-        <v>1</v>
-      </c>
-      <c r="F89">
-        <v>1</v>
-      </c>
-      <c r="G89">
-        <v>0</v>
-      </c>
-      <c r="H89" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F89" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>0</v>
       </c>
@@ -19542,19 +19003,13 @@
         <v>1</v>
       </c>
       <c r="E90">
-        <v>0</v>
-      </c>
-      <c r="F90">
-        <v>1</v>
-      </c>
-      <c r="G90">
-        <v>1</v>
-      </c>
-      <c r="H90" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F90" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>0</v>
       </c>
@@ -19570,17 +19025,11 @@
       <c r="E91">
         <v>0</v>
       </c>
-      <c r="F91">
-        <v>1</v>
-      </c>
-      <c r="G91">
-        <v>0</v>
-      </c>
-      <c r="H91" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F91" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>1</v>
       </c>
@@ -19591,22 +19040,16 @@
         <v>0.17636068699999999</v>
       </c>
       <c r="D92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E92">
         <v>0</v>
       </c>
-      <c r="F92">
-        <v>0</v>
-      </c>
-      <c r="G92">
-        <v>0</v>
-      </c>
-      <c r="H92" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F92" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>0</v>
       </c>
@@ -19617,22 +19060,16 @@
         <v>-0.10293682799999999</v>
       </c>
       <c r="D93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E93">
-        <v>1</v>
-      </c>
-      <c r="F93">
-        <v>1</v>
-      </c>
-      <c r="G93">
-        <v>0</v>
-      </c>
-      <c r="H93" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F93" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>1</v>
       </c>
@@ -19643,22 +19080,16 @@
         <v>0.111470682</v>
       </c>
       <c r="D94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E94">
-        <v>0</v>
-      </c>
-      <c r="F94">
-        <v>0</v>
-      </c>
-      <c r="G94">
-        <v>1</v>
-      </c>
-      <c r="H94" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F94" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>0</v>
       </c>
@@ -19672,19 +19103,13 @@
         <v>1</v>
       </c>
       <c r="E95">
-        <v>1</v>
-      </c>
-      <c r="F95">
-        <v>1</v>
-      </c>
-      <c r="G95">
-        <v>0</v>
-      </c>
-      <c r="H95" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F95" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>1</v>
       </c>
@@ -19695,22 +19120,16 @@
         <v>0.37292665400000002</v>
       </c>
       <c r="D96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E96">
         <v>1</v>
       </c>
-      <c r="F96">
-        <v>0</v>
-      </c>
-      <c r="G96">
-        <v>1</v>
-      </c>
-      <c r="H96" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F96" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>0</v>
       </c>
@@ -19726,17 +19145,11 @@
       <c r="E97">
         <v>0</v>
       </c>
-      <c r="F97">
-        <v>1</v>
-      </c>
-      <c r="G97">
-        <v>0</v>
-      </c>
-      <c r="H97" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F97" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>1</v>
       </c>
@@ -19747,22 +19160,16 @@
         <v>0.293303698</v>
       </c>
       <c r="D98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E98">
         <v>1</v>
       </c>
-      <c r="F98">
-        <v>0</v>
-      </c>
-      <c r="G98">
-        <v>1</v>
-      </c>
-      <c r="H98" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F98" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>1</v>
       </c>
@@ -19773,22 +19180,16 @@
         <v>-7.4743730000000003E-3</v>
       </c>
       <c r="D99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E99">
         <v>0</v>
       </c>
-      <c r="F99">
-        <v>0</v>
-      </c>
-      <c r="G99">
-        <v>0</v>
-      </c>
-      <c r="H99" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F99" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>1</v>
       </c>
@@ -19804,17 +19205,11 @@
       <c r="E100">
         <v>1</v>
       </c>
-      <c r="F100">
-        <v>0</v>
-      </c>
-      <c r="G100">
-        <v>1</v>
-      </c>
-      <c r="H100" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F100" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>0</v>
       </c>
@@ -19828,19 +19223,13 @@
         <v>1</v>
       </c>
       <c r="E101">
-        <v>1</v>
-      </c>
-      <c r="F101">
-        <v>1</v>
-      </c>
-      <c r="G101">
-        <v>0</v>
-      </c>
-      <c r="H101" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F101" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>1</v>
       </c>
@@ -19851,22 +19240,16 @@
         <v>8.5473926000000006E-2</v>
       </c>
       <c r="D102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E102">
-        <v>0</v>
-      </c>
-      <c r="F102">
-        <v>0</v>
-      </c>
-      <c r="G102">
-        <v>1</v>
-      </c>
-      <c r="H102" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F102" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>0</v>
       </c>
@@ -19880,19 +19263,13 @@
         <v>1</v>
       </c>
       <c r="E103">
-        <v>1</v>
-      </c>
-      <c r="F103">
-        <v>1</v>
-      </c>
-      <c r="G103">
-        <v>0</v>
-      </c>
-      <c r="H103" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F103" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>1</v>
       </c>
@@ -19906,19 +19283,13 @@
         <v>0</v>
       </c>
       <c r="E104">
-        <v>0</v>
-      </c>
-      <c r="F104">
-        <v>0</v>
-      </c>
-      <c r="G104">
-        <v>1</v>
-      </c>
-      <c r="H104" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F104" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>0</v>
       </c>
@@ -19929,22 +19300,16 @@
         <v>-1.2134555999999999E-2</v>
       </c>
       <c r="D105">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E105">
-        <v>1</v>
-      </c>
-      <c r="F105">
-        <v>1</v>
-      </c>
-      <c r="G105">
-        <v>0</v>
-      </c>
-      <c r="H105" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F105" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>1</v>
       </c>
@@ -19955,22 +19320,16 @@
         <v>0.54402489799999998</v>
       </c>
       <c r="D106">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E106">
-        <v>0</v>
-      </c>
-      <c r="F106">
-        <v>0</v>
-      </c>
-      <c r="G106">
-        <v>1</v>
-      </c>
-      <c r="H106" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F106" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>1</v>
       </c>
@@ -19981,22 +19340,16 @@
         <v>-0.14358104999999999</v>
       </c>
       <c r="D107">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E107">
         <v>0</v>
       </c>
-      <c r="F107">
-        <v>0</v>
-      </c>
-      <c r="G107">
-        <v>0</v>
-      </c>
-      <c r="H107" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F107" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>0</v>
       </c>
@@ -20007,22 +19360,16 @@
         <v>-0.14221056500000001</v>
       </c>
       <c r="D108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E108">
-        <v>1</v>
-      </c>
-      <c r="F108">
-        <v>1</v>
-      </c>
-      <c r="G108">
-        <v>0</v>
-      </c>
-      <c r="H108" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F108" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>1</v>
       </c>
@@ -20033,22 +19380,16 @@
         <v>0.40059949500000003</v>
       </c>
       <c r="D109">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E109">
-        <v>0</v>
-      </c>
-      <c r="F109">
-        <v>0</v>
-      </c>
-      <c r="G109">
-        <v>1</v>
-      </c>
-      <c r="H109" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F109" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>0</v>
       </c>
@@ -20062,19 +19403,13 @@
         <v>1</v>
       </c>
       <c r="E110">
-        <v>1</v>
-      </c>
-      <c r="F110">
-        <v>1</v>
-      </c>
-      <c r="G110">
-        <v>0</v>
-      </c>
-      <c r="H110" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F110" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>1</v>
       </c>
@@ -20085,22 +19420,16 @@
         <v>0.67833785300000005</v>
       </c>
       <c r="D111">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E111">
-        <v>0</v>
-      </c>
-      <c r="F111">
-        <v>0</v>
-      </c>
-      <c r="G111">
-        <v>1</v>
-      </c>
-      <c r="H111" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F111" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>0</v>
       </c>
@@ -20111,22 +19440,16 @@
         <v>-0.25869156799999998</v>
       </c>
       <c r="D112">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E112">
-        <v>1</v>
-      </c>
-      <c r="F112">
-        <v>1</v>
-      </c>
-      <c r="G112">
-        <v>0</v>
-      </c>
-      <c r="H112" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F112" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>0</v>
       </c>
@@ -20142,17 +19465,11 @@
       <c r="E113">
         <v>0</v>
       </c>
-      <c r="F113">
-        <v>1</v>
-      </c>
-      <c r="G113">
-        <v>0</v>
-      </c>
-      <c r="H113" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F113" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>0</v>
       </c>
@@ -20166,19 +19483,13 @@
         <v>1</v>
       </c>
       <c r="E114">
-        <v>1</v>
-      </c>
-      <c r="F114">
-        <v>1</v>
-      </c>
-      <c r="G114">
-        <v>0</v>
-      </c>
-      <c r="H114" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F114" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>1</v>
       </c>
@@ -20189,22 +19500,16 @@
         <v>0.11296392099999999</v>
       </c>
       <c r="D115">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E115">
-        <v>0</v>
-      </c>
-      <c r="F115">
-        <v>0</v>
-      </c>
-      <c r="G115">
-        <v>1</v>
-      </c>
-      <c r="H115" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F115" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>0</v>
       </c>
@@ -20215,22 +19520,16 @@
         <v>-0.182749526</v>
       </c>
       <c r="D116">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E116">
-        <v>1</v>
-      </c>
-      <c r="F116">
-        <v>1</v>
-      </c>
-      <c r="G116">
-        <v>0</v>
-      </c>
-      <c r="H116" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F116" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>1</v>
       </c>
@@ -20241,22 +19540,16 @@
         <v>5.2005112999999999E-2</v>
       </c>
       <c r="D117">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E117">
-        <v>0</v>
-      </c>
-      <c r="F117">
-        <v>0</v>
-      </c>
-      <c r="G117">
-        <v>1</v>
-      </c>
-      <c r="H117" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F117" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>0</v>
       </c>
@@ -20272,17 +19565,11 @@
       <c r="E118">
         <v>0</v>
       </c>
-      <c r="F118">
-        <v>1</v>
-      </c>
-      <c r="G118">
-        <v>0</v>
-      </c>
-      <c r="H118" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F118" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>0</v>
       </c>
@@ -20293,22 +19580,16 @@
         <v>-7.6015137999999996E-2</v>
       </c>
       <c r="D119">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E119">
-        <v>0</v>
-      </c>
-      <c r="F119">
-        <v>1</v>
-      </c>
-      <c r="G119">
-        <v>1</v>
-      </c>
-      <c r="H119" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F119" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>0</v>
       </c>
@@ -20319,82 +19600,64 @@
         <v>-0.24200292800000001</v>
       </c>
       <c r="D120">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E120">
-        <v>1</v>
-      </c>
-      <c r="F120">
-        <v>1</v>
-      </c>
-      <c r="G120">
-        <v>0</v>
-      </c>
-      <c r="H120" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F120" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C121">
-        <v>-0.24721615499999999</v>
+        <v>2.4171567000000001E-2</v>
       </c>
       <c r="D121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E121">
-        <v>0</v>
-      </c>
-      <c r="F121">
-        <v>1</v>
-      </c>
-      <c r="G121">
-        <v>0</v>
-      </c>
-      <c r="H121" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F121" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>1</v>
       </c>
       <c r="B122">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C122">
-        <v>2.4171567000000001E-2</v>
+        <v>-7.2758334999999993E-2</v>
       </c>
       <c r="D122">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E122">
         <v>0</v>
       </c>
-      <c r="F122">
-        <v>0</v>
-      </c>
-      <c r="G122">
-        <v>1</v>
-      </c>
-      <c r="H122" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F122" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B123">
         <v>1</v>
       </c>
       <c r="C123">
-        <v>-7.2758334999999993E-2</v>
+        <v>-0.20443434799999999</v>
       </c>
       <c r="D123">
         <v>1</v>
@@ -20402,51 +19665,39 @@
       <c r="E123">
         <v>0</v>
       </c>
-      <c r="F123">
-        <v>0</v>
-      </c>
-      <c r="G123">
-        <v>0</v>
-      </c>
-      <c r="H123" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F123" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C124">
-        <v>-0.20443434799999999</v>
+        <v>0.238217712</v>
       </c>
       <c r="D124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E124">
         <v>1</v>
       </c>
-      <c r="F124">
-        <v>1</v>
-      </c>
-      <c r="G124">
-        <v>0</v>
-      </c>
-      <c r="H124" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F124" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C125">
-        <v>0.238217712</v>
+        <v>-0.18539619800000001</v>
       </c>
       <c r="D125">
         <v>1</v>
@@ -20454,103 +19705,79 @@
       <c r="E125">
         <v>0</v>
       </c>
-      <c r="F125">
-        <v>0</v>
-      </c>
-      <c r="G125">
-        <v>1</v>
-      </c>
-      <c r="H125" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F125" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B126">
         <v>1</v>
       </c>
       <c r="C126">
-        <v>-0.18539619800000001</v>
+        <v>3.3844991999999997E-2</v>
       </c>
       <c r="D126">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E126">
-        <v>1</v>
-      </c>
-      <c r="F126">
-        <v>1</v>
-      </c>
-      <c r="G126">
-        <v>0</v>
-      </c>
-      <c r="H126" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F126" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B127">
         <v>1</v>
       </c>
       <c r="C127">
-        <v>3.3844991999999997E-2</v>
+        <v>-0.209851657</v>
       </c>
       <c r="D127">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E127">
         <v>0</v>
       </c>
-      <c r="F127">
-        <v>0</v>
-      </c>
-      <c r="G127">
-        <v>0</v>
-      </c>
-      <c r="H127" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F127" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>0</v>
       </c>
       <c r="B128">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C128">
-        <v>-0.209851657</v>
+        <v>0.12006352300000001</v>
       </c>
       <c r="D128">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E128">
-        <v>0</v>
-      </c>
-      <c r="F128">
-        <v>1</v>
-      </c>
-      <c r="G128">
-        <v>0</v>
-      </c>
-      <c r="H128" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F128" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>0</v>
       </c>
       <c r="B129">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C129">
-        <v>0.12006352300000001</v>
+        <v>-0.28803014799999999</v>
       </c>
       <c r="D129">
         <v>1</v>
@@ -20558,17 +19785,11 @@
       <c r="E129">
         <v>0</v>
       </c>
-      <c r="F129">
-        <v>1</v>
-      </c>
-      <c r="G129">
-        <v>1</v>
-      </c>
-      <c r="H129" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F129" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>0</v>
       </c>
@@ -20576,33 +19797,27 @@
         <v>1</v>
       </c>
       <c r="C130">
-        <v>-0.28803014799999999</v>
+        <v>-0.19662292000000001</v>
       </c>
       <c r="D130">
         <v>1</v>
       </c>
       <c r="E130">
-        <v>1</v>
-      </c>
-      <c r="F130">
-        <v>1</v>
-      </c>
-      <c r="G130">
-        <v>0</v>
-      </c>
-      <c r="H130" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F130" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>0</v>
       </c>
       <c r="B131">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C131">
-        <v>-0.19662292000000001</v>
+        <v>0.31126057499999998</v>
       </c>
       <c r="D131">
         <v>1</v>
@@ -20610,25 +19825,19 @@
       <c r="E131">
         <v>1</v>
       </c>
-      <c r="F131">
-        <v>1</v>
-      </c>
-      <c r="G131">
-        <v>0</v>
-      </c>
-      <c r="H131" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F131" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>0</v>
       </c>
       <c r="B132">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C132">
-        <v>0.31126057499999998</v>
+        <v>-0.29285293200000001</v>
       </c>
       <c r="D132">
         <v>1</v>
@@ -20636,51 +19845,39 @@
       <c r="E132">
         <v>0</v>
       </c>
-      <c r="F132">
-        <v>1</v>
-      </c>
-      <c r="G132">
-        <v>1</v>
-      </c>
-      <c r="H132" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F132" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B133">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C133">
-        <v>-0.29285293200000001</v>
+        <v>0.18306831300000001</v>
       </c>
       <c r="D133">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E133">
         <v>1</v>
       </c>
-      <c r="F133">
-        <v>1</v>
-      </c>
-      <c r="G133">
-        <v>0</v>
-      </c>
-      <c r="H133" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F133" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B134">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C134">
-        <v>0.18306831300000001</v>
+        <v>-0.18999949499999999</v>
       </c>
       <c r="D134">
         <v>1</v>
@@ -20688,69 +19885,51 @@
       <c r="E134">
         <v>0</v>
       </c>
-      <c r="F134">
-        <v>0</v>
-      </c>
-      <c r="G134">
-        <v>1</v>
-      </c>
-      <c r="H134" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F134" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B135">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C135">
-        <v>-0.18999949499999999</v>
+        <v>0.56047754699999996</v>
       </c>
       <c r="D135">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E135">
         <v>1</v>
       </c>
-      <c r="F135">
-        <v>1</v>
-      </c>
-      <c r="G135">
-        <v>0</v>
-      </c>
-      <c r="H135" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F135" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B136">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C136">
-        <v>0.56047754699999996</v>
+        <v>-0.22781441199999999</v>
       </c>
       <c r="D136">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E136">
         <v>0</v>
       </c>
-      <c r="F136">
-        <v>0</v>
-      </c>
-      <c r="G136">
-        <v>1</v>
-      </c>
-      <c r="H136" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F136" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>0</v>
       </c>
@@ -20758,59 +19937,47 @@
         <v>1</v>
       </c>
       <c r="C137">
-        <v>-0.22781441199999999</v>
+        <v>-0.323345243</v>
       </c>
       <c r="D137">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E137">
-        <v>1</v>
-      </c>
-      <c r="F137">
-        <v>1</v>
-      </c>
-      <c r="G137">
-        <v>0</v>
-      </c>
-      <c r="H137" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F137" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B138">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C138">
-        <v>-0.323345243</v>
+        <v>0.14159177100000001</v>
       </c>
       <c r="D138">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E138">
         <v>1</v>
       </c>
-      <c r="F138">
-        <v>1</v>
-      </c>
-      <c r="G138">
-        <v>0</v>
-      </c>
-      <c r="H138" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F138" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B139">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C139">
-        <v>0.14159177100000001</v>
+        <v>-0.16209535899999999</v>
       </c>
       <c r="D139">
         <v>1</v>
@@ -20818,51 +19985,39 @@
       <c r="E139">
         <v>0</v>
       </c>
-      <c r="F139">
-        <v>0</v>
-      </c>
-      <c r="G139">
-        <v>1</v>
-      </c>
-      <c r="H139" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F139" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B140">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C140">
-        <v>-0.16209535899999999</v>
+        <v>0.231269799</v>
       </c>
       <c r="D140">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E140">
         <v>1</v>
       </c>
-      <c r="F140">
-        <v>1</v>
-      </c>
-      <c r="G140">
-        <v>0</v>
-      </c>
-      <c r="H140" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F140" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B141">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C141">
-        <v>0.231269799</v>
+        <v>-0.22116288100000001</v>
       </c>
       <c r="D141">
         <v>1</v>
@@ -20870,51 +20025,39 @@
       <c r="E141">
         <v>0</v>
       </c>
-      <c r="F141">
-        <v>0</v>
-      </c>
-      <c r="G141">
-        <v>1</v>
-      </c>
-      <c r="H141" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F141" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B142">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C142">
-        <v>-0.22116288100000001</v>
+        <v>0.25997959500000001</v>
       </c>
       <c r="D142">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E142">
         <v>1</v>
       </c>
-      <c r="F142">
-        <v>1</v>
-      </c>
-      <c r="G142">
-        <v>0</v>
-      </c>
-      <c r="H142" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F142" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B143">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C143">
-        <v>0.25997959500000001</v>
+        <v>-0.36746735899999999</v>
       </c>
       <c r="D143">
         <v>1</v>
@@ -20922,51 +20065,39 @@
       <c r="E143">
         <v>0</v>
       </c>
-      <c r="F143">
-        <v>0</v>
-      </c>
-      <c r="G143">
-        <v>1</v>
-      </c>
-      <c r="H143" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F143" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B144">
         <v>1</v>
       </c>
       <c r="C144">
-        <v>-0.36746735899999999</v>
+        <v>1.9163779999999998E-2</v>
       </c>
       <c r="D144">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E144">
-        <v>1</v>
-      </c>
-      <c r="F144">
-        <v>1</v>
-      </c>
-      <c r="G144">
-        <v>0</v>
-      </c>
-      <c r="H144" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F144" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>0</v>
       </c>
       <c r="B145">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C145">
-        <v>-5.4178346000000002E-2</v>
+        <v>-0.207731155</v>
       </c>
       <c r="D145">
         <v>1</v>
@@ -20974,65 +20105,7 @@
       <c r="E145">
         <v>0</v>
       </c>
-      <c r="F145">
-        <v>1</v>
-      </c>
-      <c r="G145">
-        <v>1</v>
-      </c>
-      <c r="H145" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A146">
-        <v>1</v>
-      </c>
-      <c r="B146">
-        <v>1</v>
-      </c>
-      <c r="C146">
-        <v>1.9163779999999998E-2</v>
-      </c>
-      <c r="D146">
-        <v>1</v>
-      </c>
-      <c r="E146">
-        <v>0</v>
-      </c>
-      <c r="F146">
-        <v>0</v>
-      </c>
-      <c r="G146">
-        <v>0</v>
-      </c>
-      <c r="H146" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A147">
-        <v>0</v>
-      </c>
-      <c r="B147">
-        <v>1</v>
-      </c>
-      <c r="C147">
-        <v>-0.207731155</v>
-      </c>
-      <c r="D147">
-        <v>0</v>
-      </c>
-      <c r="E147">
-        <v>1</v>
-      </c>
-      <c r="F147">
-        <v>1</v>
-      </c>
-      <c r="G147">
-        <v>0</v>
-      </c>
-      <c r="H147" t="s">
+      <c r="F145" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
committing new system code
</commit_message>
<xml_diff>
--- a/decision_data_new.xlsx
+++ b/decision_data_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/paul_kumar_mail_utoronto_ca/Documents/engineering_masters/thesis work/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="183" documentId="6_{F6B86153-F216-4926-93F2-3946DCDAA96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9EE60764-5A39-4AC9-BDBB-910EEAAA2E2B}"/>
+  <xr:revisionPtr revIDLastSave="184" documentId="6_{F6B86153-F216-4926-93F2-3946DCDAA96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B57D20DF-E045-4855-905E-86B16D48D1AE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,8 +22,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">wall_binary_2!$F$1:$F$182</definedName>
     <definedName name="_xlchart.v1.0" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">wall_mounted_data!$F$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">wall_mounted_data!$B$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">wall_mounted_data!$B$2:$B$320</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">wall_mounted_data!$E$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">wall_mounted_data!$E$2:$E$320</definedName>
     <definedName name="_xlchart.v1.12" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
     <definedName name="_xlchart.v1.13" hidden="1">wall_mounted_data!$D$1</definedName>
     <definedName name="_xlchart.v1.14" hidden="1">wall_mounted_data!$D$2:$D$320</definedName>
@@ -32,11 +32,11 @@
     <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$B$2:$B$150</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">wall_mounted_data!$F$2:$F$320</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">wall_mounted_data!$C$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">wall_mounted_data!$C$2:$C$320</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">wall_mounted_data!$B$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">wall_mounted_data!$B$2:$B$320</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">wall_mounted_data!$E$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">wall_mounted_data!$E$2:$E$320</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">wall_mounted_data!$C$1</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">wall_mounted_data!$C$2:$C$320</definedName>
     <definedName name="_xlchart.v1.9" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -628,10 +628,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.11</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -669,7 +669,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{24F89B28-D331-4BF4-97FC-98740A0DD325}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.10</cx:f>
+              <cx:f>_xlchart.v1.4</cx:f>
               <cx:v>first_peak</cx:v>
             </cx:txData>
           </cx:tx>
@@ -699,10 +699,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -740,7 +740,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{5A2C1765-A6AF-400C-A8FA-AC7260F1E1FC}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:f>_xlchart.v1.7</cx:f>
               <cx:v>second_peak</cx:v>
             </cx:txData>
           </cx:tx>
@@ -841,10 +841,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -882,7 +882,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{28AFBDCB-EA5A-4D8B-B5F8-DF1924715131}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.7</cx:f>
+              <cx:f>_xlchart.v1.10</cx:f>
               <cx:v>last_peak</cx:v>
             </cx:txData>
           </cx:tx>
@@ -17198,11 +17198,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A2C5052-2A6F-49B6-97B4-305C293E194C}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:F182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="A167" sqref="A167:XFD167"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17251,7 +17250,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -17291,7 +17290,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -17311,7 +17310,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -17331,7 +17330,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -17351,7 +17350,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -17391,7 +17390,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -17431,7 +17430,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -17471,7 +17470,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -17511,7 +17510,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -17551,7 +17550,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -17591,7 +17590,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0</v>
       </c>
@@ -17611,7 +17610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -17631,7 +17630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -17671,7 +17670,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -17711,7 +17710,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -17751,7 +17750,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0</v>
       </c>
@@ -17791,7 +17790,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0</v>
       </c>
@@ -17831,7 +17830,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0</v>
       </c>
@@ -17871,7 +17870,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0</v>
       </c>
@@ -17911,7 +17910,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0</v>
       </c>
@@ -17951,7 +17950,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>0</v>
       </c>
@@ -17971,7 +17970,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>0</v>
       </c>
@@ -18011,7 +18010,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1</v>
       </c>
@@ -18051,7 +18050,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1</v>
       </c>
@@ -18091,7 +18090,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1</v>
       </c>
@@ -18131,7 +18130,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>0</v>
       </c>
@@ -18171,7 +18170,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>0</v>
       </c>
@@ -18211,7 +18210,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>0</v>
       </c>
@@ -18251,7 +18250,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>0</v>
       </c>
@@ -18291,7 +18290,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>0</v>
       </c>
@@ -18331,7 +18330,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>0</v>
       </c>
@@ -18371,7 +18370,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1</v>
       </c>
@@ -18411,7 +18410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>0</v>
       </c>
@@ -18451,7 +18450,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>0</v>
       </c>
@@ -18491,7 +18490,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>0</v>
       </c>
@@ -18531,7 +18530,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>0</v>
       </c>
@@ -18571,7 +18570,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>1</v>
       </c>
@@ -18611,7 +18610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>0</v>
       </c>
@@ -18651,7 +18650,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>0</v>
       </c>
@@ -18691,7 +18690,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>0</v>
       </c>
@@ -18731,7 +18730,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>0</v>
       </c>
@@ -18771,7 +18770,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>0</v>
       </c>
@@ -18811,7 +18810,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>0</v>
       </c>
@@ -18851,7 +18850,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>0</v>
       </c>
@@ -18871,7 +18870,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>0</v>
       </c>
@@ -18911,7 +18910,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>0</v>
       </c>
@@ -18951,7 +18950,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>0</v>
       </c>
@@ -18991,7 +18990,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>0</v>
       </c>
@@ -19031,7 +19030,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>0</v>
       </c>
@@ -19071,7 +19070,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>0</v>
       </c>
@@ -19111,7 +19110,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>0</v>
       </c>
@@ -19191,7 +19190,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>0</v>
       </c>
@@ -19231,7 +19230,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>0</v>
       </c>
@@ -19271,7 +19270,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>0</v>
       </c>
@@ -19331,7 +19330,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>0</v>
       </c>
@@ -19371,7 +19370,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>0</v>
       </c>
@@ -19411,7 +19410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>0</v>
       </c>
@@ -19431,7 +19430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>0</v>
       </c>
@@ -19471,7 +19470,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>0</v>
       </c>
@@ -19511,7 +19510,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>0</v>
       </c>
@@ -19531,7 +19530,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>0</v>
       </c>
@@ -19551,7 +19550,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>1</v>
       </c>
@@ -19591,7 +19590,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>0</v>
       </c>
@@ -19631,7 +19630,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>0</v>
       </c>
@@ -19671,7 +19670,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>0</v>
       </c>
@@ -19711,7 +19710,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>0</v>
       </c>
@@ -19731,7 +19730,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>0</v>
       </c>
@@ -19771,7 +19770,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>0</v>
       </c>
@@ -19811,7 +19810,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>0</v>
       </c>
@@ -19851,7 +19850,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>0</v>
       </c>
@@ -19871,7 +19870,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>0</v>
       </c>
@@ -19911,7 +19910,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>0</v>
       </c>
@@ -19951,7 +19950,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>0</v>
       </c>
@@ -19991,7 +19990,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="140" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>0</v>
       </c>
@@ -20011,7 +20010,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="141" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>1</v>
       </c>
@@ -20031,7 +20030,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="142" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>0</v>
       </c>
@@ -20071,7 +20070,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="144" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>0</v>
       </c>
@@ -20091,7 +20090,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>0</v>
       </c>
@@ -20131,7 +20130,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>0</v>
       </c>
@@ -20171,7 +20170,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>0</v>
       </c>
@@ -20211,7 +20210,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>0</v>
       </c>
@@ -20251,7 +20250,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>0</v>
       </c>
@@ -20271,7 +20270,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>0</v>
       </c>
@@ -20311,7 +20310,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>0</v>
       </c>
@@ -20351,7 +20350,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>0</v>
       </c>
@@ -20371,7 +20370,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>0</v>
       </c>
@@ -20411,7 +20410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>1</v>
       </c>
@@ -20431,7 +20430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>0</v>
       </c>
@@ -20471,7 +20470,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>0</v>
       </c>
@@ -20511,7 +20510,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>0</v>
       </c>
@@ -20551,7 +20550,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>0</v>
       </c>
@@ -20591,7 +20590,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>0</v>
       </c>
@@ -20631,7 +20630,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>0</v>
       </c>
@@ -20671,7 +20670,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>0</v>
       </c>
@@ -20711,7 +20710,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>0</v>
       </c>
@@ -20751,7 +20750,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>0</v>
       </c>
@@ -20791,7 +20790,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>0</v>
       </c>
@@ -20831,7 +20830,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>0</v>
       </c>
@@ -20852,13 +20851,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="F1:F182" xr:uid="{A6C5FCF7-5A38-4CF2-9668-F9E38AD993C1}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="right"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="F1:F182" xr:uid="{A6C5FCF7-5A38-4CF2-9668-F9E38AD993C1}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
there was a data conflict
</commit_message>
<xml_diff>
--- a/decision_data_new.xlsx
+++ b/decision_data_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/paul_kumar_mail_utoronto_ca/Documents/engineering_masters/thesis work/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="188" documentId="6_{F6B86153-F216-4926-93F2-3946DCDAA96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D9B69976-3AE8-4EB8-94F8-39DD6DEB2C4E}"/>
+  <xr:revisionPtr revIDLastSave="196" documentId="6_{F6B86153-F216-4926-93F2-3946DCDAA96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A5D2AB1D-4887-4F46-B42A-BFB94648FCDB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,21 +23,36 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">wall_binary_2!$F$1:$F$182</definedName>
     <definedName name="_xlchart.v1.0" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">wall_mounted_data!$B$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">wall_mounted_data!$D$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">wall_mounted_data!$D$2:$D$320</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">wall_mounted_data!$E$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">wall_mounted_data!$E$2:$E$320</definedName>
     <definedName name="_xlchart.v1.12" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
     <definedName name="_xlchart.v1.13" hidden="1">wall_mounted_data!$F$1</definedName>
     <definedName name="_xlchart.v1.14" hidden="1">wall_mounted_data!$F$2:$F$320</definedName>
     <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$A$2:$A$150</definedName>
     <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$B$1</definedName>
     <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$B$2:$B$150</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">adjusted_lens!$A$2:$A$41</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">adjusted_lens!$K$1</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">wall_mounted_data!$B$2:$B$320</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">adjusted_lens!$K$2:$K$41</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">adjusted_lens!$A$2:$A$41</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">adjusted_lens!$D$1</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">adjusted_lens!$D$2:$D$41</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">adjusted_lens!$A$2:$A$41</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">adjusted_lens!$K$1</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">adjusted_lens!$K$2:$K$41</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">adjusted_lens!$A$2:$A$41</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">adjusted_lens!$G$1</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">adjusted_lens!$G$2:$G$41</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">adjusted_lens!$A$2:$A$41</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">adjusted_lens!$D$1</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">adjusted_lens!$D$2:$D$41</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">wall_mounted_data!$C$1</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">wall_mounted_data!$C$2:$C$320</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">wall_mounted_data!$E$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">wall_mounted_data!$E$2:$E$320</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">wall_mounted_data!$D$1</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">wall_mounted_data!$D$2:$D$320</definedName>
     <definedName name="_xlchart.v1.9" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -45,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="17">
   <si>
     <t>first_peak</t>
   </si>
@@ -786,10 +801,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.11</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -827,7 +842,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{2E007EC1-CE09-47B1-A3E4-A95E48D1BADB}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.10</cx:f>
+              <cx:f>_xlchart.v1.7</cx:f>
               <cx:v>second_last_peak</cx:v>
             </cx:txData>
           </cx:tx>
@@ -857,10 +872,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -898,7 +913,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{28AFBDCB-EA5A-4D8B-B5F8-DF1924715131}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.7</cx:f>
+              <cx:f>_xlchart.v1.10</cx:f>
               <cx:v>last_peak</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1015,6 +1030,148 @@
             <cx:txData>
               <cx:f>_xlchart.v1.16</cx:f>
               <cx:v>first_peak</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx7.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.21</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.23</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Gradient_1</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Gradient_1</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{F817657A-853F-485F-B1CA-8304AC66361E}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.22</cx:f>
+              <cx:v>Gradient_1</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx8.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.27</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.29</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Gradient_2</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Gradient_2</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{54F07B9F-F54F-47A3-8629-153198983661}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.28</cx:f>
+              <cx:v>Gradient_2</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:dataId val="0"/>
@@ -1239,6 +1396,86 @@
 </file>
 
 <file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4368,6 +4605,1036 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -4846,6 +6113,167 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Chart 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{364B3107-6430-4C55-A828-CCA82ADF84BC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9191625" y="1681162"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Chart 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72F1E82D-F310-4EEF-9546-72D192F08AA6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9163050" y="4462462"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -23890,70 +25318,73 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81501096-BB37-47DA-850A-215A7DDA06CF}">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
         <v>-9.7222440687221995E-2</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
         <v>9.9780925968464995E-2</v>
       </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
       <c r="H2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -23961,139 +25392,151 @@
       <c r="J2">
         <v>1</v>
       </c>
-      <c r="K2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0</v>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
         <v>0.183824563229637</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
         <v>-0.177715589829256</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3">
         <v>1</v>
       </c>
-      <c r="K3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
         <v>0.54352392285351903</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
         <v>0.32347375165776199</v>
       </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
         <v>0.157219715113944</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
         <v>-0.16176035670568201</v>
       </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
       <c r="H5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5">
         <v>1</v>
       </c>
-      <c r="K5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1</v>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
         <v>0.20647414902335001</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
         <v>0.134448283084972</v>
       </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
       <c r="H6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -24101,69 +25544,75 @@
       <c r="J6">
         <v>1</v>
       </c>
-      <c r="K6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>0</v>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
         <v>0.120529458892708</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
         <v>-0.142246478513016</v>
       </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
       <c r="H7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <v>1</v>
       </c>
-      <c r="K7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1</v>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
         <v>0.59316373511953402</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
         <v>0.109570523292914</v>
       </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
       <c r="H8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -24171,139 +25620,151 @@
       <c r="J8">
         <v>1</v>
       </c>
-      <c r="K8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>0</v>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
         <v>0.13440447450485399</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
         <v>-3.2054623626681003E-2</v>
       </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
       <c r="H9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9">
         <v>1</v>
       </c>
-      <c r="K9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1</v>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
         <v>0.45632605552963101</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
       <c r="E10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
         <v>0.34324701540717401</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
       <c r="H10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
         <v>-0.12025403559534401</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
         <v>-0.28386496837812503</v>
       </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
       <c r="H11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11">
-        <v>1</v>
-      </c>
-      <c r="K11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
         <v>2.5541348684520002E-2</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
       <c r="E12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
         <v>0.34027667763569702</v>
       </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
       <c r="H12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -24311,67 +25772,73 @@
       <c r="J12">
         <v>1</v>
       </c>
-      <c r="K12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>0</v>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
         <v>-0.44405454770090902</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
       <c r="E13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
         <v>-0.24110457160360199</v>
       </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
       <c r="H13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13">
         <v>0</v>
       </c>
       <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="K13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
         <v>-0.16350563865235901</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
       <c r="E14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
         <v>0.32267041964137999</v>
       </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
       <c r="H14">
         <v>1</v>
       </c>
@@ -24379,211 +25846,229 @@
         <v>1</v>
       </c>
       <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>3</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
         <v>-0.15503514849518199</v>
       </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
       <c r="E15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
         <v>-0.214858493838432</v>
       </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
       <c r="H15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15">
         <v>0</v>
       </c>
       <c r="J15">
-        <v>1</v>
-      </c>
-      <c r="K15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>4</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
         <v>0.469802697459133</v>
       </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
       <c r="E16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
         <v>0.346843746384352</v>
       </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
       <c r="H16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16">
         <v>1</v>
       </c>
       <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>3</v>
       </c>
       <c r="B17">
         <v>0</v>
       </c>
       <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
         <v>0.14596493616042899</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
       <c r="E17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
         <v>-0.148111479339259</v>
       </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
       <c r="H17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17">
         <v>1</v>
       </c>
-      <c r="K17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1</v>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>4</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
         <v>0.48415725316850899</v>
       </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
       <c r="E18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
         <v>0.367704272999478</v>
       </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
       <c r="H18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18">
         <v>1</v>
       </c>
       <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>3</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
       <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
         <v>6.5654857789326004E-2</v>
       </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
       <c r="E19">
         <v>1</v>
       </c>
       <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
         <v>-7.5503086457723995E-2</v>
       </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
       <c r="H19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>4</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
         <v>0.37463135710877798</v>
       </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
         <v>6.0194467526992E-2</v>
       </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
       <c r="H20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20">
         <v>1</v>
@@ -24591,69 +26076,75 @@
       <c r="J20">
         <v>1</v>
       </c>
-      <c r="K20" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>0</v>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>3</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
         <v>1.0144342173684999E-2</v>
       </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
       <c r="E21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
         <v>-0.111587763910532</v>
       </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
       <c r="H21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21">
         <v>1</v>
       </c>
-      <c r="K21" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>1</v>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>4</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
         <v>0.23889148164950399</v>
       </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
       <c r="E22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
         <v>0.42770605477454199</v>
       </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
       <c r="H22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22">
         <v>1</v>
@@ -24661,419 +26152,455 @@
       <c r="J22">
         <v>1</v>
       </c>
-      <c r="K22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>0</v>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>3</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
       <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
         <v>4.1324889625494E-2</v>
       </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
       <c r="E23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
         <v>-0.16825133633236999</v>
       </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
       <c r="H23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23">
         <v>1</v>
       </c>
-      <c r="K23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>1</v>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>4</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
         <v>0.20209992085684</v>
       </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
       <c r="E24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
         <v>0.37850917380814902</v>
       </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
       <c r="H24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24">
         <v>1</v>
       </c>
       <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>3</v>
       </c>
       <c r="B25">
         <v>0</v>
       </c>
       <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
         <v>-3.2643356713877997E-2</v>
       </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
       <c r="E25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
         <v>-0.19819180861997299</v>
       </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
       <c r="H25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25">
         <v>1</v>
       </c>
-      <c r="K25" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>1</v>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>4</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
         <v>4.0439892667097001E-2</v>
       </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
       <c r="E26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
         <v>0.386161328017185</v>
       </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
       <c r="H26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26">
         <v>1</v>
       </c>
       <c r="J26">
-        <v>0</v>
-      </c>
-      <c r="K26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>3</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
       <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
         <v>4.2314749951295E-2</v>
       </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
       <c r="E27">
         <v>1</v>
       </c>
       <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
         <v>-7.7294943244365005E-2</v>
       </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
       <c r="H27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27">
-        <v>0</v>
-      </c>
-      <c r="K27" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>4</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
         <v>4.0103044087160004E-3</v>
       </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
       <c r="E28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
         <v>0.33766763121391602</v>
       </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
       <c r="H28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28">
         <v>1</v>
       </c>
       <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="K28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>3</v>
       </c>
       <c r="B29">
         <v>0</v>
       </c>
       <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
         <v>1.3208043346287999E-2</v>
       </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
       <c r="E29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
         <v>-0.186061132356409</v>
       </c>
-      <c r="G29">
-        <v>1</v>
-      </c>
       <c r="H29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29">
         <v>1</v>
       </c>
-      <c r="K29" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>1</v>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>4</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
         <v>0.17978501603942501</v>
       </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
       <c r="E30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
         <v>0.37138688759317801</v>
       </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
       <c r="H30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30">
         <v>1</v>
       </c>
       <c r="J30">
-        <v>0</v>
-      </c>
-      <c r="K30" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>3</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
         <v>-2.4824999104198001E-2</v>
       </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
       <c r="E31">
         <v>1</v>
       </c>
       <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
         <v>-0.100901609262224</v>
       </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
       <c r="H31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31">
         <v>0</v>
       </c>
       <c r="J31">
-        <v>1</v>
-      </c>
-      <c r="K31" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>4</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
         <v>-1.6907893292898001E-2</v>
       </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
       <c r="E32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
         <v>0.36505678700574601</v>
       </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
       <c r="H32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I32">
         <v>1</v>
       </c>
       <c r="J32">
-        <v>0</v>
-      </c>
-      <c r="K32" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>3</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
         <v>-0.19917151879705999</v>
       </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
       <c r="E33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
         <v>-0.22683422974109599</v>
       </c>
-      <c r="G33">
-        <v>1</v>
-      </c>
       <c r="H33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33">
         <v>0</v>
       </c>
       <c r="J33">
-        <v>1</v>
-      </c>
-      <c r="K33" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="L33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>4</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
         <v>0.32705448221799399</v>
       </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
         <v>0.109288007671854</v>
       </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
       <c r="H34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34">
         <v>1</v>
@@ -25081,209 +26608,227 @@
       <c r="J34">
         <v>1</v>
       </c>
-      <c r="K34" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>0</v>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>3</v>
       </c>
       <c r="B35">
         <v>0</v>
       </c>
       <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
         <v>0.11657989053918601</v>
       </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
       <c r="E35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
         <v>-0.18979431454930201</v>
       </c>
-      <c r="G35">
-        <v>1</v>
-      </c>
       <c r="H35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J35">
         <v>1</v>
       </c>
-      <c r="K35" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>1</v>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>4</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
         <v>0.16369792033425301</v>
       </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
       <c r="E36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
         <v>0.32136486465619202</v>
       </c>
-      <c r="G36">
-        <v>0</v>
-      </c>
       <c r="H36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I36">
         <v>1</v>
       </c>
       <c r="J36">
-        <v>0</v>
-      </c>
-      <c r="K36" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>3</v>
       </c>
       <c r="B37">
         <v>0</v>
       </c>
       <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
         <v>0.10927124441678</v>
       </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
       <c r="E37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
         <v>-0.19050955178423001</v>
       </c>
-      <c r="G37">
-        <v>1</v>
-      </c>
       <c r="H37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37">
         <v>1</v>
       </c>
-      <c r="K37" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>1</v>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>4</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
       <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
         <v>-8.1501594296909993E-2</v>
       </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
       <c r="E38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
         <v>0.26159382685621202</v>
       </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
       <c r="H38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38">
         <v>0</v>
       </c>
-      <c r="K38" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>0</v>
+      <c r="K38">
+        <v>0</v>
+      </c>
+      <c r="L38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>3</v>
       </c>
       <c r="B39">
         <v>0</v>
       </c>
       <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
         <v>0.143387814552872</v>
       </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
       <c r="E39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
         <v>-0.19118375273716201</v>
       </c>
-      <c r="G39">
-        <v>1</v>
-      </c>
       <c r="H39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J39">
         <v>1</v>
       </c>
-      <c r="K39" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>1</v>
+      <c r="K39">
+        <v>1</v>
+      </c>
+      <c r="L39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>4</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
         <v>0.29628855256645897</v>
       </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
       <c r="E40">
         <v>0</v>
       </c>
       <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
         <v>0.11615858026753199</v>
       </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
       <c r="H40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I40">
         <v>1</v>
@@ -25291,46 +26836,53 @@
       <c r="J40">
         <v>1</v>
       </c>
-      <c r="K40" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>0</v>
+      <c r="K40">
+        <v>1</v>
+      </c>
+      <c r="L40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>3</v>
       </c>
       <c r="B41">
         <v>0</v>
       </c>
       <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
         <v>0.14364183675300499</v>
       </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
       <c r="E41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
         <v>-0.18690745023282601</v>
       </c>
-      <c r="G41">
-        <v>1</v>
-      </c>
       <c r="H41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J41">
         <v>1</v>
       </c>
-      <c r="K41" t="s">
+      <c r="K41">
+        <v>1</v>
+      </c>
+      <c r="L41" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
quick test of model
</commit_message>
<xml_diff>
--- a/decision_data_new.xlsx
+++ b/decision_data_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/paul_kumar_mail_utoronto_ca/Documents/engineering_masters/thesis work/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="205" documentId="6_{F6B86153-F216-4926-93F2-3946DCDAA96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{EFD9D949-3520-4A0D-BFD3-60492CD2049A}"/>
+  <xr:revisionPtr revIDLastSave="207" documentId="6_{F6B86153-F216-4926-93F2-3946DCDAA96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2B5CAC63-57CF-4522-9145-5026292BE9A6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,28 +23,28 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">wall_binary_2!$F$1:$F$182</definedName>
     <definedName name="_xlchart.v1.0" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">wall_mounted_data!$B$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">wall_mounted_data!$E$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">wall_mounted_data!$E$2:$E$320</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">wall_mounted_data!$E$1</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">wall_mounted_data!$C$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">wall_mounted_data!$C$2:$C$320</definedName>
     <definedName name="_xlchart.v1.12" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">wall_mounted_data!$C$1</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">wall_mounted_data!$C$2:$C$320</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">wall_mounted_data!$D$1</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">wall_mounted_data!$D$2:$D$320</definedName>
     <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$A$2:$A$150</definedName>
     <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$B$1</definedName>
     <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$B$2:$B$150</definedName>
     <definedName name="_xlchart.v1.18" hidden="1">adjusted_lens!$A$2:$A$41</definedName>
     <definedName name="_xlchart.v1.19" hidden="1">adjusted_lens!$D$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">wall_mounted_data!$B$2:$B$320</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">wall_mounted_data!$E$2:$E$320</definedName>
     <definedName name="_xlchart.v1.20" hidden="1">adjusted_lens!$D$2:$D$41</definedName>
     <definedName name="_xlchart.v1.21" hidden="1">adjusted_lens!$A$2:$A$41</definedName>
     <definedName name="_xlchart.v1.22" hidden="1">adjusted_lens!$G$1</definedName>
     <definedName name="_xlchart.v1.23" hidden="1">adjusted_lens!$G$2:$G$41</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">wall_mounted_data!$D$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">wall_mounted_data!$D$2:$D$320</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">wall_mounted_data!$F$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">wall_mounted_data!$F$2:$F$320</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">wall_mounted_data!$F$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">wall_mounted_data!$F$2:$F$320</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">wall_mounted_data!$B$1</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">wall_mounted_data!$B$2:$B$320</definedName>
     <definedName name="_xlchart.v1.9" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="21">
   <si>
     <t>first_peak</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>second_peak_differential</t>
+  </si>
+  <si>
+    <t>No-left</t>
+  </si>
+  <si>
+    <t>No-right</t>
   </si>
 </sst>
 </file>
@@ -657,10 +663,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -698,7 +704,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{24F89B28-D331-4BF4-97FC-98740A0DD325}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.1</cx:f>
+              <cx:f>_xlchart.v1.7</cx:f>
               <cx:v>first_peak</cx:v>
             </cx:txData>
           </cx:tx>
@@ -728,10 +734,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.12</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.14</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -769,7 +775,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{5A2C1765-A6AF-400C-A8FA-AC7260F1E1FC}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.13</cx:f>
+              <cx:f>_xlchart.v1.10</cx:f>
               <cx:v>second_peak</cx:v>
             </cx:txData>
           </cx:tx>
@@ -799,10 +805,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.12</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.14</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -840,7 +846,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{2E007EC1-CE09-47B1-A3E4-A95E48D1BADB}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:f>_xlchart.v1.13</cx:f>
               <cx:v>second_last_peak</cx:v>
             </cx:txData>
           </cx:tx>
@@ -870,10 +876,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.11</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -911,7 +917,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{28AFBDCB-EA5A-4D8B-B5F8-DF1924715131}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.10</cx:f>
+              <cx:f>_xlchart.v1.1</cx:f>
               <cx:v>last_peak</cx:v>
             </cx:txData>
           </cx:tx>
@@ -941,10 +947,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -982,7 +988,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{02F72712-9CA3-4436-A6ED-93C80B1901DF}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.7</cx:f>
+              <cx:f>_xlchart.v1.4</cx:f>
               <cx:v>Gradient_1</cx:v>
             </cx:txData>
           </cx:tx>
@@ -26887,10 +26893,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83B5E27E-8A64-4193-B44D-44B5D7422D12}">
-  <dimension ref="A1:M78"/>
+  <dimension ref="A1:M153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S27" sqref="S27"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:M153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26944,7 +26950,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.46237764428278999</v>
+        <v>0.46237764399999998</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -26953,7 +26959,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>0.48553496982828798</v>
+        <v>0.48553497000000001</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -26985,7 +26991,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>3.2487123304024E-2</v>
+        <v>3.2487123E-2</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -26994,7 +27000,7 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>-0.26295871622557998</v>
+        <v>-0.26295871599999998</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -27026,7 +27032,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0.48332211479584902</v>
+        <v>0.483322115</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -27035,7 +27041,7 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>0.59189806596845596</v>
+        <v>0.59189806599999994</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -27067,7 +27073,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>7.4755007392371994E-2</v>
+        <v>7.4755006999999998E-2</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -27076,7 +27082,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>-0.26452790211303101</v>
+        <v>-0.26452790199999998</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -27108,7 +27114,7 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>8.2453698588590002E-3</v>
+        <v>8.2453700000000001E-3</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -27117,7 +27123,7 @@
         <v>1</v>
       </c>
       <c r="F6">
-        <v>0.55928057029437295</v>
+        <v>0.55928056999999998</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -27149,7 +27155,7 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>0.13773424250917499</v>
+        <v>0.13773424300000001</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -27158,7 +27164,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>-0.263849399832635</v>
+        <v>-0.26384940000000001</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -27190,7 +27196,7 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>0.101163204745533</v>
+        <v>0.10116320500000001</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -27199,7 +27205,7 @@
         <v>1</v>
       </c>
       <c r="F8">
-        <v>0.585097785889099</v>
+        <v>0.58509778599999995</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -27231,7 +27237,7 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>2.4834238055423001E-2</v>
+        <v>2.4834238000000002E-2</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -27240,7 +27246,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>-0.257632659818818</v>
+        <v>-0.25763266000000001</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -27272,7 +27278,7 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>2.2749926401826E-2</v>
+        <v>2.2749926E-2</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -27281,7 +27287,7 @@
         <v>1</v>
       </c>
       <c r="F10">
-        <v>0.52957422285526101</v>
+        <v>0.52957422300000001</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -27313,7 +27319,7 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>3.1615940033929001E-2</v>
+        <v>3.1615940000000002E-2</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -27322,7 +27328,7 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>-0.39997344382484701</v>
+        <v>-0.39997344400000001</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -27354,7 +27360,7 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>2.3419404547463E-2</v>
+        <v>2.3419405000000001E-2</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -27363,7 +27369,7 @@
         <v>1</v>
       </c>
       <c r="F12">
-        <v>0.39784260078364603</v>
+        <v>0.39784260100000002</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -27395,7 +27401,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>0.19019937299734699</v>
+        <v>0.190199373</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -27404,7 +27410,7 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>-0.54382606224156405</v>
+        <v>-0.54382606200000005</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -27436,7 +27442,7 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <v>0.32164400407920402</v>
+        <v>0.32164400399999998</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -27445,7 +27451,7 @@
         <v>1</v>
       </c>
       <c r="F14">
-        <v>0.52509492867770502</v>
+        <v>0.52509492899999999</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -27477,7 +27483,7 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>0.21154298322096399</v>
+        <v>0.21154298299999999</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -27486,7 +27492,7 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>-0.24873264552055099</v>
+        <v>-0.248732646</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -27518,7 +27524,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>0.334838997906726</v>
+        <v>0.334838998</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -27527,7 +27533,7 @@
         <v>1</v>
       </c>
       <c r="F16">
-        <v>0.77710598213305604</v>
+        <v>0.77710598200000003</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -27559,7 +27565,7 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <v>2.6711404121207E-2</v>
+        <v>2.6711404000000001E-2</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -27568,7 +27574,7 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>-0.23561320719846901</v>
+        <v>-0.23561320699999999</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -27600,7 +27606,7 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <v>3.3341804868201999E-2</v>
+        <v>3.3341805000000002E-2</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -27609,7 +27615,7 @@
         <v>1</v>
       </c>
       <c r="F18">
-        <v>0.57495923399395299</v>
+        <v>0.57495923400000004</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -27641,7 +27647,7 @@
         <v>1</v>
       </c>
       <c r="C19">
-        <v>-0.29930330457475202</v>
+        <v>-0.29930330500000002</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -27650,7 +27656,7 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>-0.246315660349013</v>
+        <v>-0.24631565999999999</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -27682,7 +27688,7 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <v>7.6869773726399998E-3</v>
+        <v>7.6869770000000002E-3</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -27691,7 +27697,7 @@
         <v>1</v>
       </c>
       <c r="F20">
-        <v>0.65294938764271904</v>
+        <v>0.65294938800000002</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -27723,7 +27729,7 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <v>8.9543751850176004E-2</v>
+        <v>8.9543752000000004E-2</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -27732,7 +27738,7 @@
         <v>0</v>
       </c>
       <c r="F21">
-        <v>-0.70760382672601696</v>
+        <v>-0.70760382700000002</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -27764,7 +27770,7 @@
         <v>1</v>
       </c>
       <c r="C22">
-        <v>8.2802964704987006E-2</v>
+        <v>8.2802965000000006E-2</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -27773,7 +27779,7 @@
         <v>1</v>
       </c>
       <c r="F22">
-        <v>0.43945351697298402</v>
+        <v>0.43945351700000002</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -27805,7 +27811,7 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <v>2.1855256486542001E-2</v>
+        <v>2.1855256E-2</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -27814,7 +27820,7 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>-0.58339282913067803</v>
+        <v>-0.583392829</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -27846,7 +27852,7 @@
         <v>1</v>
       </c>
       <c r="C24">
-        <v>2.8461417073469999E-3</v>
+        <v>2.8461419999999999E-3</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -27855,7 +27861,7 @@
         <v>1</v>
       </c>
       <c r="F24">
-        <v>0.64281356451688898</v>
+        <v>0.64281356499999998</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -27887,7 +27893,7 @@
         <v>1</v>
       </c>
       <c r="C25">
-        <v>-9.7958621901139999E-3</v>
+        <v>-9.7958620000000007E-3</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -27896,7 +27902,7 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <v>-0.28105814989509997</v>
+        <v>-0.28105815000000001</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -27928,7 +27934,7 @@
         <v>1</v>
       </c>
       <c r="C26">
-        <v>-0.17687879570635001</v>
+        <v>-0.176878796</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -27937,7 +27943,7 @@
         <v>0</v>
       </c>
       <c r="F26">
-        <v>-0.25292944381403998</v>
+        <v>-0.252929444</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -27969,7 +27975,7 @@
         <v>1</v>
       </c>
       <c r="C27">
-        <v>-8.4982604470549995E-3</v>
+        <v>-8.4982600000000005E-3</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -27978,7 +27984,7 @@
         <v>0</v>
       </c>
       <c r="F27">
-        <v>-0.32920466999224202</v>
+        <v>-0.32920466999999998</v>
       </c>
       <c r="G27">
         <v>1</v>
@@ -28010,7 +28016,7 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <v>0.47277740065775298</v>
+        <v>0.47277740099999999</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -28019,7 +28025,7 @@
         <v>1</v>
       </c>
       <c r="F28">
-        <v>0.581939801224586</v>
+        <v>0.58193980099999998</v>
       </c>
       <c r="G28">
         <v>0</v>
@@ -28051,7 +28057,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <v>0.12908444405988401</v>
+        <v>0.12908444399999999</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -28060,7 +28066,7 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <v>-0.69052433075366804</v>
+        <v>-0.69052433099999999</v>
       </c>
       <c r="G29">
         <v>1</v>
@@ -28092,7 +28098,7 @@
         <v>1</v>
       </c>
       <c r="C30">
-        <v>7.9290605260821004E-2</v>
+        <v>7.9290605E-2</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -28101,7 +28107,7 @@
         <v>1</v>
       </c>
       <c r="F30">
-        <v>0.52423770450120599</v>
+        <v>0.524237705</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -28133,7 +28139,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <v>7.0537199833530004E-2</v>
+        <v>7.0537199999999994E-2</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -28142,7 +28148,7 @@
         <v>0</v>
       </c>
       <c r="F31">
-        <v>-0.63216547386463695</v>
+        <v>-0.63216547400000001</v>
       </c>
       <c r="G31">
         <v>1</v>
@@ -28174,7 +28180,7 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <v>0.492341444055022</v>
+        <v>0.49234144400000002</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -28183,7 +28189,7 @@
         <v>1</v>
       </c>
       <c r="F32">
-        <v>0.52167053967242805</v>
+        <v>0.52167054000000002</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -28215,7 +28221,7 @@
         <v>1</v>
       </c>
       <c r="C33">
-        <v>-7.5152429923721994E-2</v>
+        <v>-7.5152430000000006E-2</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -28224,7 +28230,7 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <v>-0.65716942403742296</v>
+        <v>-0.657169424</v>
       </c>
       <c r="G33">
         <v>1</v>
@@ -28256,7 +28262,7 @@
         <v>1</v>
       </c>
       <c r="C34">
-        <v>3.2068119097959001E-2</v>
+        <v>3.2068118999999999E-2</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -28265,7 +28271,7 @@
         <v>1</v>
       </c>
       <c r="F34">
-        <v>0.57070710757004794</v>
+        <v>0.57070710800000002</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -28297,7 +28303,7 @@
         <v>1</v>
       </c>
       <c r="C35">
-        <v>-9.9977260085198E-2</v>
+        <v>-9.9977259999999998E-2</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -28306,7 +28312,7 @@
         <v>0</v>
       </c>
       <c r="F35">
-        <v>-0.61369842585733703</v>
+        <v>-0.61369842600000002</v>
       </c>
       <c r="G35">
         <v>1</v>
@@ -28338,7 +28344,7 @@
         <v>1</v>
       </c>
       <c r="C36">
-        <v>0.10835291133882299</v>
+        <v>0.108352911</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -28347,7 +28353,7 @@
         <v>1</v>
       </c>
       <c r="F36">
-        <v>0.48880930554615099</v>
+        <v>0.488809306</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -28379,7 +28385,7 @@
         <v>1</v>
       </c>
       <c r="C37">
-        <v>-1.506461850187E-3</v>
+        <v>-1.5064620000000001E-3</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -28388,7 +28394,7 @@
         <v>0</v>
       </c>
       <c r="F37">
-        <v>-0.60530397556426996</v>
+        <v>-0.60530397599999997</v>
       </c>
       <c r="G37">
         <v>1</v>
@@ -28420,7 +28426,7 @@
         <v>1</v>
       </c>
       <c r="C38">
-        <v>5.9334340375382003E-2</v>
+        <v>5.9334339999999999E-2</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -28429,7 +28435,7 @@
         <v>1</v>
       </c>
       <c r="F38">
-        <v>0.44004808159970099</v>
+        <v>0.44004808200000001</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -28461,7 +28467,7 @@
         <v>1</v>
       </c>
       <c r="C39">
-        <v>-9.8881511067288E-2</v>
+        <v>-9.8881511000000005E-2</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -28470,7 +28476,7 @@
         <v>0</v>
       </c>
       <c r="F39">
-        <v>-0.36471970162155298</v>
+        <v>-0.36471970199999998</v>
       </c>
       <c r="G39">
         <v>1</v>
@@ -28502,7 +28508,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <v>0.33534731235713999</v>
+        <v>0.33534731200000001</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -28511,7 +28517,7 @@
         <v>1</v>
       </c>
       <c r="F40">
-        <v>0.59199411023752402</v>
+        <v>0.59199411000000002</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -28543,7 +28549,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <v>0.13645540458574301</v>
+        <v>0.136455405</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -28552,7 +28558,7 @@
         <v>0</v>
       </c>
       <c r="F41">
-        <v>-0.68504690480628105</v>
+        <v>-0.68504690499999998</v>
       </c>
       <c r="G41">
         <v>1</v>
@@ -28584,7 +28590,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <v>0.44326043848744601</v>
+        <v>0.44326043799999998</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -28593,7 +28599,7 @@
         <v>1</v>
       </c>
       <c r="F42">
-        <v>0.65758856888532902</v>
+        <v>0.65758856899999996</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -28625,7 +28631,7 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <v>0.10971689480496701</v>
+        <v>0.10971689499999999</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -28634,7 +28640,7 @@
         <v>0</v>
       </c>
       <c r="F43">
-        <v>-0.51261522988174402</v>
+        <v>-0.51261522999999998</v>
       </c>
       <c r="G43">
         <v>1</v>
@@ -28666,7 +28672,7 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <v>0.47133082487060601</v>
+        <v>0.47133082500000001</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -28675,7 +28681,7 @@
         <v>1</v>
       </c>
       <c r="F44">
-        <v>0.56713372087712399</v>
+        <v>0.56713372100000004</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -28707,7 +28713,7 @@
         <v>1</v>
       </c>
       <c r="C45">
-        <v>-0.17232263692830699</v>
+        <v>-0.172322637</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -28716,7 +28722,7 @@
         <v>0</v>
       </c>
       <c r="F45">
-        <v>-0.73780606056938902</v>
+        <v>-0.73780606100000001</v>
       </c>
       <c r="G45">
         <v>1</v>
@@ -28748,7 +28754,7 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <v>6.7052350206337999E-2</v>
+        <v>6.7052349999999997E-2</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -28757,7 +28763,7 @@
         <v>1</v>
       </c>
       <c r="F46">
-        <v>0.54084378609968198</v>
+        <v>0.54084378600000005</v>
       </c>
       <c r="G46">
         <v>1</v>
@@ -28789,7 +28795,7 @@
         <v>1</v>
       </c>
       <c r="C47">
-        <v>-2.8229287152470001E-2</v>
+        <v>-2.8229286999999999E-2</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -28798,7 +28804,7 @@
         <v>0</v>
       </c>
       <c r="F47">
-        <v>-0.498293317120444</v>
+        <v>-0.49829331700000001</v>
       </c>
       <c r="G47">
         <v>1</v>
@@ -28830,7 +28836,7 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <v>0.48800354651351102</v>
+        <v>0.48800354699999998</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -28839,7 +28845,7 @@
         <v>1</v>
       </c>
       <c r="F48">
-        <v>0.59517965505583803</v>
+        <v>0.59517965500000003</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -28871,7 +28877,7 @@
         <v>1</v>
       </c>
       <c r="C49">
-        <v>-3.2486351723890999E-2</v>
+        <v>-3.2486352000000003E-2</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -28880,7 +28886,7 @@
         <v>0</v>
       </c>
       <c r="F49">
-        <v>-0.337580289736301</v>
+        <v>-0.33758029000000001</v>
       </c>
       <c r="G49">
         <v>1</v>
@@ -28912,7 +28918,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <v>0.34051284385952502</v>
+        <v>0.34051284399999998</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -28921,7 +28927,7 @@
         <v>1</v>
       </c>
       <c r="F50">
-        <v>0.57981319769000805</v>
+        <v>0.57981319799999997</v>
       </c>
       <c r="G50">
         <v>0</v>
@@ -28953,7 +28959,7 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <v>0.110157437030219</v>
+        <v>0.110157437</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -28962,7 +28968,7 @@
         <v>0</v>
       </c>
       <c r="F51">
-        <v>-0.53111511281350998</v>
+        <v>-0.53111511300000003</v>
       </c>
       <c r="G51">
         <v>1</v>
@@ -28994,7 +29000,7 @@
         <v>0</v>
       </c>
       <c r="C52">
-        <v>0.45812111278931</v>
+        <v>0.45812111300000002</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -29003,7 +29009,7 @@
         <v>1</v>
       </c>
       <c r="F52">
-        <v>0.58399384368297103</v>
+        <v>0.58399384399999998</v>
       </c>
       <c r="G52">
         <v>0</v>
@@ -29035,7 +29041,7 @@
         <v>1</v>
       </c>
       <c r="C53">
-        <v>1.899992011104E-2</v>
+        <v>1.899992E-2</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -29044,7 +29050,7 @@
         <v>0</v>
       </c>
       <c r="F53">
-        <v>-0.27940595395393503</v>
+        <v>-0.27940595400000001</v>
       </c>
       <c r="G53">
         <v>1</v>
@@ -29076,7 +29082,7 @@
         <v>1</v>
       </c>
       <c r="C54">
-        <v>4.4248003968582E-2</v>
+        <v>4.4248004000000001E-2</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -29085,7 +29091,7 @@
         <v>1</v>
       </c>
       <c r="F54">
-        <v>0.48273626996883201</v>
+        <v>0.48273627000000002</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -29117,7 +29123,7 @@
         <v>1</v>
       </c>
       <c r="C55">
-        <v>-1.8174668045384999E-2</v>
+        <v>-1.8174668000000001E-2</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -29126,7 +29132,7 @@
         <v>0</v>
       </c>
       <c r="F55">
-        <v>-0.236403433962421</v>
+        <v>-0.236403434</v>
       </c>
       <c r="G55">
         <v>1</v>
@@ -29158,7 +29164,7 @@
         <v>1</v>
       </c>
       <c r="C56">
-        <v>9.2433198633265004E-2</v>
+        <v>9.2433198999999994E-2</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -29167,7 +29173,7 @@
         <v>1</v>
       </c>
       <c r="F56">
-        <v>0.54008894407095298</v>
+        <v>0.54008894399999996</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -29199,7 +29205,7 @@
         <v>1</v>
       </c>
       <c r="C57">
-        <v>-0.16662893182305</v>
+        <v>-0.16662893200000001</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -29208,7 +29214,7 @@
         <v>0</v>
       </c>
       <c r="F57">
-        <v>-0.22545016547390301</v>
+        <v>-0.22545016500000001</v>
       </c>
       <c r="G57">
         <v>1</v>
@@ -29240,7 +29246,7 @@
         <v>1</v>
       </c>
       <c r="C58">
-        <v>2.6224456630580002E-2</v>
+        <v>2.6224457E-2</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -29249,7 +29255,7 @@
         <v>1</v>
       </c>
       <c r="F58">
-        <v>0.49938149843583102</v>
+        <v>0.49938149799999998</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -29281,7 +29287,7 @@
         <v>0</v>
       </c>
       <c r="C59">
-        <v>6.3658486452398994E-2</v>
+        <v>6.3658486E-2</v>
       </c>
       <c r="D59">
         <v>1</v>
@@ -29290,7 +29296,7 @@
         <v>0</v>
       </c>
       <c r="F59">
-        <v>-0.72193099633695701</v>
+        <v>-0.72193099599999999</v>
       </c>
       <c r="G59">
         <v>1</v>
@@ -29322,7 +29328,7 @@
         <v>1</v>
       </c>
       <c r="C60">
-        <v>7.6014157234084001E-2</v>
+        <v>7.6014156999999999E-2</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -29331,7 +29337,7 @@
         <v>1</v>
       </c>
       <c r="F60">
-        <v>0.49001357307642701</v>
+        <v>0.49001357299999998</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -29363,7 +29369,7 @@
         <v>1</v>
       </c>
       <c r="C61">
-        <v>-0.20851452714150201</v>
+        <v>-0.20851452700000001</v>
       </c>
       <c r="D61">
         <v>1</v>
@@ -29372,7 +29378,7 @@
         <v>0</v>
       </c>
       <c r="F61">
-        <v>-0.64824535428251295</v>
+        <v>-0.64824535400000005</v>
       </c>
       <c r="G61">
         <v>1</v>
@@ -29404,7 +29410,7 @@
         <v>1</v>
       </c>
       <c r="C62">
-        <v>-0.19197068422500499</v>
+        <v>-0.191970684</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -29413,7 +29419,7 @@
         <v>1</v>
       </c>
       <c r="F62">
-        <v>0.68860402023746103</v>
+        <v>0.68860401999999998</v>
       </c>
       <c r="G62">
         <v>1</v>
@@ -29445,7 +29451,7 @@
         <v>0</v>
       </c>
       <c r="C63">
-        <v>0.114873384995059</v>
+        <v>0.11487338499999999</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -29454,7 +29460,7 @@
         <v>0</v>
       </c>
       <c r="F63">
-        <v>-0.66522050108992004</v>
+        <v>-0.66522050099999996</v>
       </c>
       <c r="G63">
         <v>1</v>
@@ -29486,7 +29492,7 @@
         <v>1</v>
       </c>
       <c r="C64">
-        <v>0.102156726960592</v>
+        <v>0.102156727</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -29495,7 +29501,7 @@
         <v>1</v>
       </c>
       <c r="F64">
-        <v>0.59389878864909496</v>
+        <v>0.59389878900000004</v>
       </c>
       <c r="G64">
         <v>0</v>
@@ -29527,7 +29533,7 @@
         <v>1</v>
       </c>
       <c r="C65">
-        <v>-0.163821289302854</v>
+        <v>-0.16382128900000001</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -29536,7 +29542,7 @@
         <v>0</v>
       </c>
       <c r="F65">
-        <v>-0.25057920768546998</v>
+        <v>-0.250579208</v>
       </c>
       <c r="G65">
         <v>1</v>
@@ -29568,7 +29574,7 @@
         <v>1</v>
       </c>
       <c r="C66">
-        <v>1.8012636745644E-2</v>
+        <v>1.8012637000000001E-2</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -29577,7 +29583,7 @@
         <v>0</v>
       </c>
       <c r="F66">
-        <v>0.50867482851178802</v>
+        <v>0.50867482900000005</v>
       </c>
       <c r="G66">
         <v>0</v>
@@ -29609,7 +29615,7 @@
         <v>1</v>
       </c>
       <c r="C67">
-        <v>7.7302106232700002E-3</v>
+        <v>7.7302109999999999E-3</v>
       </c>
       <c r="D67">
         <v>1</v>
@@ -29618,7 +29624,7 @@
         <v>0</v>
       </c>
       <c r="F67">
-        <v>-0.27521645118065402</v>
+        <v>-0.27521645099999997</v>
       </c>
       <c r="G67">
         <v>1</v>
@@ -29650,7 +29656,7 @@
         <v>1</v>
       </c>
       <c r="C68">
-        <v>8.3518704610953995E-2</v>
+        <v>8.3518704999999999E-2</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -29659,7 +29665,7 @@
         <v>1</v>
       </c>
       <c r="F68">
-        <v>0.43817043923342203</v>
+        <v>0.43817043900000002</v>
       </c>
       <c r="G68">
         <v>0</v>
@@ -29691,7 +29697,7 @@
         <v>1</v>
       </c>
       <c r="C69">
-        <v>5.7588948256059999E-3</v>
+        <v>5.758895E-3</v>
       </c>
       <c r="D69">
         <v>1</v>
@@ -29700,7 +29706,7 @@
         <v>0</v>
       </c>
       <c r="F69">
-        <v>-0.48141434651533499</v>
+        <v>-0.48141434700000002</v>
       </c>
       <c r="G69">
         <v>1</v>
@@ -29732,7 +29738,7 @@
         <v>1</v>
       </c>
       <c r="C70">
-        <v>9.2971927240985006E-2</v>
+        <v>9.2971926999999996E-2</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -29741,7 +29747,7 @@
         <v>1</v>
       </c>
       <c r="F70">
-        <v>0.52864016763000399</v>
+        <v>0.52864016800000002</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -29773,7 +29779,7 @@
         <v>1</v>
       </c>
       <c r="C71">
-        <v>-0.19426371105149601</v>
+        <v>-0.19426371100000001</v>
       </c>
       <c r="D71">
         <v>1</v>
@@ -29782,7 +29788,7 @@
         <v>0</v>
       </c>
       <c r="F71">
-        <v>-0.22774501285720999</v>
+        <v>-0.227745013</v>
       </c>
       <c r="G71">
         <v>1</v>
@@ -29814,7 +29820,7 @@
         <v>0</v>
       </c>
       <c r="C72">
-        <v>0.17510563496516399</v>
+        <v>0.17510563500000001</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -29823,7 +29829,7 @@
         <v>1</v>
       </c>
       <c r="F72">
-        <v>0.57711084344086905</v>
+        <v>0.57711084300000004</v>
       </c>
       <c r="G72">
         <v>0</v>
@@ -29855,7 +29861,7 @@
         <v>1</v>
       </c>
       <c r="C73">
-        <v>-3.3469332732789001E-2</v>
+        <v>-3.3469332999999997E-2</v>
       </c>
       <c r="D73">
         <v>1</v>
@@ -29864,7 +29870,7 @@
         <v>0</v>
       </c>
       <c r="F73">
-        <v>-0.26497035825277099</v>
+        <v>-0.26497035800000002</v>
       </c>
       <c r="G73">
         <v>1</v>
@@ -29896,7 +29902,7 @@
         <v>1</v>
       </c>
       <c r="C74">
-        <v>0.101351145262318</v>
+        <v>0.101351145</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -29905,7 +29911,7 @@
         <v>1</v>
       </c>
       <c r="F74">
-        <v>0.52054022386780896</v>
+        <v>0.520540224</v>
       </c>
       <c r="G74">
         <v>0</v>
@@ -29937,7 +29943,7 @@
         <v>1</v>
       </c>
       <c r="C75">
-        <v>-0.325827184414274</v>
+        <v>-0.32582718399999999</v>
       </c>
       <c r="D75">
         <v>1</v>
@@ -29946,7 +29952,7 @@
         <v>0</v>
       </c>
       <c r="F75">
-        <v>-0.23304887381152301</v>
+        <v>-0.23304887399999999</v>
       </c>
       <c r="G75">
         <v>1</v>
@@ -29978,7 +29984,7 @@
         <v>1</v>
       </c>
       <c r="C76">
-        <v>0.111405686173977</v>
+        <v>0.111405686</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -29987,7 +29993,7 @@
         <v>1</v>
       </c>
       <c r="F76">
-        <v>0.57016350118719905</v>
+        <v>0.57016350100000002</v>
       </c>
       <c r="G76">
         <v>0</v>
@@ -30019,7 +30025,7 @@
         <v>1</v>
       </c>
       <c r="C77">
-        <v>-0.363155614651678</v>
+        <v>-0.36315561499999999</v>
       </c>
       <c r="D77">
         <v>1</v>
@@ -30028,7 +30034,7 @@
         <v>0</v>
       </c>
       <c r="F77">
-        <v>-0.67531836187886796</v>
+        <v>-0.67531836199999995</v>
       </c>
       <c r="G77">
         <v>1</v>
@@ -30060,7 +30066,7 @@
         <v>1</v>
       </c>
       <c r="C78">
-        <v>6.1148605352854997E-2</v>
+        <v>6.1148605000000002E-2</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -30069,7 +30075,7 @@
         <v>1</v>
       </c>
       <c r="F78">
-        <v>0.59187962259127502</v>
+        <v>0.59187962299999997</v>
       </c>
       <c r="G78">
         <v>0</v>
@@ -30091,6 +30097,3081 @@
       </c>
       <c r="M78" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>1</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="C79">
+        <v>-4.8390724921654998E-2</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
+      <c r="F79">
+        <v>0.79830392341942902</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>1</v>
+      </c>
+      <c r="I79">
+        <v>0</v>
+      </c>
+      <c r="J79">
+        <v>0</v>
+      </c>
+      <c r="K79">
+        <v>0</v>
+      </c>
+      <c r="L79">
+        <v>0</v>
+      </c>
+      <c r="M79" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>0</v>
+      </c>
+      <c r="B80">
+        <v>1</v>
+      </c>
+      <c r="C80">
+        <v>-9.0588012546996E-2</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <v>-0.297942574923588</v>
+      </c>
+      <c r="G80">
+        <v>1</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+      <c r="I80">
+        <v>0</v>
+      </c>
+      <c r="J80">
+        <v>1</v>
+      </c>
+      <c r="K80">
+        <v>1</v>
+      </c>
+      <c r="L80">
+        <v>1</v>
+      </c>
+      <c r="M80" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>1</v>
+      </c>
+      <c r="B81">
+        <v>1</v>
+      </c>
+      <c r="C81">
+        <v>2.4298209553787999E-2</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <v>1</v>
+      </c>
+      <c r="F81">
+        <v>0.62109448152191604</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>1</v>
+      </c>
+      <c r="I81">
+        <v>0</v>
+      </c>
+      <c r="J81">
+        <v>1</v>
+      </c>
+      <c r="K81">
+        <v>0</v>
+      </c>
+      <c r="L81">
+        <v>0</v>
+      </c>
+      <c r="M81" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>-1</v>
+      </c>
+      <c r="B82">
+        <v>-1</v>
+      </c>
+      <c r="C82">
+        <v>9999</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <v>0.21777957011789401</v>
+      </c>
+      <c r="G82">
+        <v>-1</v>
+      </c>
+      <c r="H82">
+        <v>1</v>
+      </c>
+      <c r="I82">
+        <v>-1</v>
+      </c>
+      <c r="J82">
+        <v>1</v>
+      </c>
+      <c r="K82">
+        <v>1</v>
+      </c>
+      <c r="L82">
+        <v>1</v>
+      </c>
+      <c r="M82" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>-1</v>
+      </c>
+      <c r="B83">
+        <v>-1</v>
+      </c>
+      <c r="C83">
+        <v>9999</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <v>0.24114133934283599</v>
+      </c>
+      <c r="G83">
+        <v>-1</v>
+      </c>
+      <c r="H83">
+        <v>1</v>
+      </c>
+      <c r="I83">
+        <v>-1</v>
+      </c>
+      <c r="J83">
+        <v>1</v>
+      </c>
+      <c r="K83">
+        <v>1</v>
+      </c>
+      <c r="L83">
+        <v>1</v>
+      </c>
+      <c r="M83" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>0</v>
+      </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
+      <c r="C84">
+        <v>-0.22823217614830299</v>
+      </c>
+      <c r="D84">
+        <v>-1</v>
+      </c>
+      <c r="E84">
+        <v>-1</v>
+      </c>
+      <c r="F84">
+        <v>9999</v>
+      </c>
+      <c r="G84">
+        <v>1</v>
+      </c>
+      <c r="H84">
+        <v>-1</v>
+      </c>
+      <c r="I84">
+        <v>0</v>
+      </c>
+      <c r="J84">
+        <v>-1</v>
+      </c>
+      <c r="K84">
+        <v>0</v>
+      </c>
+      <c r="L84">
+        <v>0</v>
+      </c>
+      <c r="M84" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>0</v>
+      </c>
+      <c r="B85">
+        <v>1</v>
+      </c>
+      <c r="C85">
+        <v>-0.19127303976882801</v>
+      </c>
+      <c r="D85">
+        <v>-1</v>
+      </c>
+      <c r="E85">
+        <v>-1</v>
+      </c>
+      <c r="F85">
+        <v>9999</v>
+      </c>
+      <c r="G85">
+        <v>1</v>
+      </c>
+      <c r="H85">
+        <v>-1</v>
+      </c>
+      <c r="I85">
+        <v>0</v>
+      </c>
+      <c r="J85">
+        <v>-1</v>
+      </c>
+      <c r="K85">
+        <v>0</v>
+      </c>
+      <c r="L85">
+        <v>0</v>
+      </c>
+      <c r="M85" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>0</v>
+      </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
+      <c r="C86">
+        <v>-9.1523057241878994E-2</v>
+      </c>
+      <c r="D86">
+        <v>-1</v>
+      </c>
+      <c r="E86">
+        <v>-1</v>
+      </c>
+      <c r="F86">
+        <v>9999</v>
+      </c>
+      <c r="G86">
+        <v>1</v>
+      </c>
+      <c r="H86">
+        <v>-1</v>
+      </c>
+      <c r="I86">
+        <v>1</v>
+      </c>
+      <c r="J86">
+        <v>-1</v>
+      </c>
+      <c r="K86">
+        <v>0</v>
+      </c>
+      <c r="L86">
+        <v>0</v>
+      </c>
+      <c r="M86" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>1</v>
+      </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
+      <c r="C87">
+        <v>0.214546084942005</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87">
+        <v>0.140604524086405</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+      <c r="H87">
+        <v>1</v>
+      </c>
+      <c r="I87">
+        <v>1</v>
+      </c>
+      <c r="J87">
+        <v>1</v>
+      </c>
+      <c r="K87">
+        <v>0</v>
+      </c>
+      <c r="L87">
+        <v>0</v>
+      </c>
+      <c r="M87" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>1</v>
+      </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
+      <c r="C88">
+        <v>0.435457492069807</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>0.143082757373026</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+      <c r="H88">
+        <v>1</v>
+      </c>
+      <c r="I88">
+        <v>1</v>
+      </c>
+      <c r="J88">
+        <v>1</v>
+      </c>
+      <c r="K88">
+        <v>0</v>
+      </c>
+      <c r="L88">
+        <v>1</v>
+      </c>
+      <c r="M88" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>1</v>
+      </c>
+      <c r="B89">
+        <v>1</v>
+      </c>
+      <c r="C89">
+        <v>3.3456615904143998E-2</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+      <c r="F89">
+        <v>0.14548961100737001</v>
+      </c>
+      <c r="G89">
+        <v>0</v>
+      </c>
+      <c r="H89">
+        <v>1</v>
+      </c>
+      <c r="I89">
+        <v>0</v>
+      </c>
+      <c r="J89">
+        <v>1</v>
+      </c>
+      <c r="K89">
+        <v>0</v>
+      </c>
+      <c r="L89">
+        <v>1</v>
+      </c>
+      <c r="M89" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>0</v>
+      </c>
+      <c r="B90">
+        <v>1</v>
+      </c>
+      <c r="C90">
+        <v>-0.1619655959138</v>
+      </c>
+      <c r="D90">
+        <v>1</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="F90">
+        <v>-0.22789976772628301</v>
+      </c>
+      <c r="G90">
+        <v>1</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
+      <c r="I90">
+        <v>0</v>
+      </c>
+      <c r="J90">
+        <v>1</v>
+      </c>
+      <c r="K90">
+        <v>1</v>
+      </c>
+      <c r="L90">
+        <v>0</v>
+      </c>
+      <c r="M90" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>0</v>
+      </c>
+      <c r="B91">
+        <v>1</v>
+      </c>
+      <c r="C91">
+        <v>-8.6153390892600004E-2</v>
+      </c>
+      <c r="D91">
+        <v>1</v>
+      </c>
+      <c r="E91">
+        <v>1</v>
+      </c>
+      <c r="F91">
+        <v>-0.16174377165311099</v>
+      </c>
+      <c r="G91">
+        <v>1</v>
+      </c>
+      <c r="H91">
+        <v>0</v>
+      </c>
+      <c r="I91">
+        <v>0</v>
+      </c>
+      <c r="J91">
+        <v>0</v>
+      </c>
+      <c r="K91">
+        <v>1</v>
+      </c>
+      <c r="L91">
+        <v>0</v>
+      </c>
+      <c r="M91" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>0</v>
+      </c>
+      <c r="B92">
+        <v>1</v>
+      </c>
+      <c r="C92">
+        <v>-7.1849696506743999E-2</v>
+      </c>
+      <c r="D92">
+        <v>1</v>
+      </c>
+      <c r="E92">
+        <v>1</v>
+      </c>
+      <c r="F92">
+        <v>-7.1062629913349997E-3</v>
+      </c>
+      <c r="G92">
+        <v>1</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
+      <c r="I92">
+        <v>0</v>
+      </c>
+      <c r="J92">
+        <v>0</v>
+      </c>
+      <c r="K92">
+        <v>1</v>
+      </c>
+      <c r="L92">
+        <v>0</v>
+      </c>
+      <c r="M92" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>-1</v>
+      </c>
+      <c r="B93">
+        <v>-1</v>
+      </c>
+      <c r="C93">
+        <v>9999</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>1</v>
+      </c>
+      <c r="F93">
+        <v>0.34635957262378803</v>
+      </c>
+      <c r="G93">
+        <v>-1</v>
+      </c>
+      <c r="H93">
+        <v>1</v>
+      </c>
+      <c r="I93">
+        <v>-1</v>
+      </c>
+      <c r="J93">
+        <v>0</v>
+      </c>
+      <c r="K93">
+        <v>1</v>
+      </c>
+      <c r="L93">
+        <v>1</v>
+      </c>
+      <c r="M93" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>-1</v>
+      </c>
+      <c r="B94">
+        <v>-1</v>
+      </c>
+      <c r="C94">
+        <v>9999</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="F94">
+        <v>0.19380027731271601</v>
+      </c>
+      <c r="G94">
+        <v>-1</v>
+      </c>
+      <c r="H94">
+        <v>1</v>
+      </c>
+      <c r="I94">
+        <v>-1</v>
+      </c>
+      <c r="J94">
+        <v>1</v>
+      </c>
+      <c r="K94">
+        <v>1</v>
+      </c>
+      <c r="L94">
+        <v>1</v>
+      </c>
+      <c r="M94" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>-1</v>
+      </c>
+      <c r="B95">
+        <v>-1</v>
+      </c>
+      <c r="C95">
+        <v>9999</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="F95">
+        <v>0.23249113953737899</v>
+      </c>
+      <c r="G95">
+        <v>-1</v>
+      </c>
+      <c r="H95">
+        <v>1</v>
+      </c>
+      <c r="I95">
+        <v>-1</v>
+      </c>
+      <c r="J95">
+        <v>1</v>
+      </c>
+      <c r="K95">
+        <v>1</v>
+      </c>
+      <c r="L95">
+        <v>1</v>
+      </c>
+      <c r="M95" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>-1</v>
+      </c>
+      <c r="B96">
+        <v>-1</v>
+      </c>
+      <c r="C96">
+        <v>9999</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+      <c r="F96">
+        <v>0.25209712876497797</v>
+      </c>
+      <c r="G96">
+        <v>-1</v>
+      </c>
+      <c r="H96">
+        <v>1</v>
+      </c>
+      <c r="I96">
+        <v>-1</v>
+      </c>
+      <c r="J96">
+        <v>1</v>
+      </c>
+      <c r="K96">
+        <v>1</v>
+      </c>
+      <c r="L96">
+        <v>1</v>
+      </c>
+      <c r="M96" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>-1</v>
+      </c>
+      <c r="B97">
+        <v>-1</v>
+      </c>
+      <c r="C97">
+        <v>9999</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97">
+        <v>0.21968410053660201</v>
+      </c>
+      <c r="G97">
+        <v>-1</v>
+      </c>
+      <c r="H97">
+        <v>1</v>
+      </c>
+      <c r="I97">
+        <v>-1</v>
+      </c>
+      <c r="J97">
+        <v>1</v>
+      </c>
+      <c r="K97">
+        <v>1</v>
+      </c>
+      <c r="L97">
+        <v>1</v>
+      </c>
+      <c r="M97" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>-1</v>
+      </c>
+      <c r="B98">
+        <v>-1</v>
+      </c>
+      <c r="C98">
+        <v>9999</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="E98">
+        <v>1</v>
+      </c>
+      <c r="F98">
+        <v>0.34479692348551699</v>
+      </c>
+      <c r="G98">
+        <v>-1</v>
+      </c>
+      <c r="H98">
+        <v>1</v>
+      </c>
+      <c r="I98">
+        <v>-1</v>
+      </c>
+      <c r="J98">
+        <v>1</v>
+      </c>
+      <c r="K98">
+        <v>1</v>
+      </c>
+      <c r="L98">
+        <v>1</v>
+      </c>
+      <c r="M98" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>-1</v>
+      </c>
+      <c r="B99">
+        <v>-1</v>
+      </c>
+      <c r="C99">
+        <v>9999</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
+      <c r="F99">
+        <v>0.17847131010133199</v>
+      </c>
+      <c r="G99">
+        <v>-1</v>
+      </c>
+      <c r="H99">
+        <v>1</v>
+      </c>
+      <c r="I99">
+        <v>-1</v>
+      </c>
+      <c r="J99">
+        <v>1</v>
+      </c>
+      <c r="K99">
+        <v>1</v>
+      </c>
+      <c r="L99">
+        <v>1</v>
+      </c>
+      <c r="M99" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>1</v>
+      </c>
+      <c r="B100">
+        <v>1</v>
+      </c>
+      <c r="C100">
+        <v>-0.21616755523782699</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="E100">
+        <v>0</v>
+      </c>
+      <c r="F100">
+        <v>0.126489949231534</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+      <c r="H100">
+        <v>1</v>
+      </c>
+      <c r="I100">
+        <v>0</v>
+      </c>
+      <c r="J100">
+        <v>1</v>
+      </c>
+      <c r="K100">
+        <v>0</v>
+      </c>
+      <c r="L100">
+        <v>1</v>
+      </c>
+      <c r="M100" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>0</v>
+      </c>
+      <c r="B101">
+        <v>1</v>
+      </c>
+      <c r="C101">
+        <v>3.2944876452639998E-3</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="E101">
+        <v>1</v>
+      </c>
+      <c r="F101">
+        <v>0.49256363023820299</v>
+      </c>
+      <c r="G101">
+        <v>1</v>
+      </c>
+      <c r="H101">
+        <v>1</v>
+      </c>
+      <c r="I101">
+        <v>0</v>
+      </c>
+      <c r="J101">
+        <v>0</v>
+      </c>
+      <c r="K101">
+        <v>0</v>
+      </c>
+      <c r="L101">
+        <v>1</v>
+      </c>
+      <c r="M101" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>0</v>
+      </c>
+      <c r="B102">
+        <v>1</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="D102">
+        <v>0</v>
+      </c>
+      <c r="E102">
+        <v>0</v>
+      </c>
+      <c r="F102">
+        <v>8.5771433502186994E-2</v>
+      </c>
+      <c r="G102">
+        <v>1</v>
+      </c>
+      <c r="H102">
+        <v>1</v>
+      </c>
+      <c r="I102">
+        <v>0</v>
+      </c>
+      <c r="J102">
+        <v>1</v>
+      </c>
+      <c r="K102">
+        <v>0</v>
+      </c>
+      <c r="L102">
+        <v>1</v>
+      </c>
+      <c r="M102" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>1</v>
+      </c>
+      <c r="B103">
+        <v>0</v>
+      </c>
+      <c r="C103">
+        <v>0.35641256994522003</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+      <c r="E103">
+        <v>0</v>
+      </c>
+      <c r="F103">
+        <v>0.15626136847323099</v>
+      </c>
+      <c r="G103">
+        <v>0</v>
+      </c>
+      <c r="H103">
+        <v>1</v>
+      </c>
+      <c r="I103">
+        <v>1</v>
+      </c>
+      <c r="J103">
+        <v>1</v>
+      </c>
+      <c r="K103">
+        <v>0</v>
+      </c>
+      <c r="L103">
+        <v>1</v>
+      </c>
+      <c r="M103" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>1</v>
+      </c>
+      <c r="B104">
+        <v>0</v>
+      </c>
+      <c r="C104">
+        <v>0.45268065136277102</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+      <c r="E104">
+        <v>0</v>
+      </c>
+      <c r="F104">
+        <v>0.14577277402934</v>
+      </c>
+      <c r="G104">
+        <v>0</v>
+      </c>
+      <c r="H104">
+        <v>1</v>
+      </c>
+      <c r="I104">
+        <v>1</v>
+      </c>
+      <c r="J104">
+        <v>1</v>
+      </c>
+      <c r="K104">
+        <v>0</v>
+      </c>
+      <c r="L104">
+        <v>1</v>
+      </c>
+      <c r="M104" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>1</v>
+      </c>
+      <c r="B105">
+        <v>1</v>
+      </c>
+      <c r="C105">
+        <v>-0.213885922374975</v>
+      </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
+      <c r="E105">
+        <v>0</v>
+      </c>
+      <c r="F105">
+        <v>0.12671252083067899</v>
+      </c>
+      <c r="G105">
+        <v>0</v>
+      </c>
+      <c r="H105">
+        <v>1</v>
+      </c>
+      <c r="I105">
+        <v>0</v>
+      </c>
+      <c r="J105">
+        <v>1</v>
+      </c>
+      <c r="K105">
+        <v>0</v>
+      </c>
+      <c r="L105">
+        <v>1</v>
+      </c>
+      <c r="M105" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>1</v>
+      </c>
+      <c r="B106">
+        <v>0</v>
+      </c>
+      <c r="C106">
+        <v>0.43104723922028598</v>
+      </c>
+      <c r="D106">
+        <v>0</v>
+      </c>
+      <c r="E106">
+        <v>0</v>
+      </c>
+      <c r="F106">
+        <v>0.123666137450304</v>
+      </c>
+      <c r="G106">
+        <v>0</v>
+      </c>
+      <c r="H106">
+        <v>1</v>
+      </c>
+      <c r="I106">
+        <v>1</v>
+      </c>
+      <c r="J106">
+        <v>1</v>
+      </c>
+      <c r="K106">
+        <v>0</v>
+      </c>
+      <c r="L106">
+        <v>1</v>
+      </c>
+      <c r="M106" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>1</v>
+      </c>
+      <c r="B107">
+        <v>0</v>
+      </c>
+      <c r="C107">
+        <v>0.40220715202038998</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+      <c r="E107">
+        <v>0</v>
+      </c>
+      <c r="F107">
+        <v>6.6046248681994005E-2</v>
+      </c>
+      <c r="G107">
+        <v>0</v>
+      </c>
+      <c r="H107">
+        <v>1</v>
+      </c>
+      <c r="I107">
+        <v>1</v>
+      </c>
+      <c r="J107">
+        <v>1</v>
+      </c>
+      <c r="K107">
+        <v>0</v>
+      </c>
+      <c r="L107">
+        <v>1</v>
+      </c>
+      <c r="M107" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>1</v>
+      </c>
+      <c r="B108">
+        <v>1</v>
+      </c>
+      <c r="C108">
+        <v>2.3064783018181999E-2</v>
+      </c>
+      <c r="D108">
+        <v>0</v>
+      </c>
+      <c r="E108">
+        <v>0</v>
+      </c>
+      <c r="F108">
+        <v>7.9451324694038997E-2</v>
+      </c>
+      <c r="G108">
+        <v>0</v>
+      </c>
+      <c r="H108">
+        <v>1</v>
+      </c>
+      <c r="I108">
+        <v>0</v>
+      </c>
+      <c r="J108">
+        <v>1</v>
+      </c>
+      <c r="K108">
+        <v>0</v>
+      </c>
+      <c r="L108">
+        <v>1</v>
+      </c>
+      <c r="M108" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>1</v>
+      </c>
+      <c r="B109">
+        <v>1</v>
+      </c>
+      <c r="C109">
+        <v>-0.124447598444288</v>
+      </c>
+      <c r="D109">
+        <v>0</v>
+      </c>
+      <c r="E109">
+        <v>0</v>
+      </c>
+      <c r="F109">
+        <v>0.132286934047294</v>
+      </c>
+      <c r="G109">
+        <v>0</v>
+      </c>
+      <c r="H109">
+        <v>1</v>
+      </c>
+      <c r="I109">
+        <v>0</v>
+      </c>
+      <c r="J109">
+        <v>1</v>
+      </c>
+      <c r="K109">
+        <v>0</v>
+      </c>
+      <c r="L109">
+        <v>1</v>
+      </c>
+      <c r="M109" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>1</v>
+      </c>
+      <c r="B110">
+        <v>1</v>
+      </c>
+      <c r="C110">
+        <v>0.15549177801609401</v>
+      </c>
+      <c r="D110">
+        <v>0</v>
+      </c>
+      <c r="E110">
+        <v>0</v>
+      </c>
+      <c r="F110">
+        <v>0.10244917903400499</v>
+      </c>
+      <c r="G110">
+        <v>0</v>
+      </c>
+      <c r="H110">
+        <v>1</v>
+      </c>
+      <c r="I110">
+        <v>0</v>
+      </c>
+      <c r="J110">
+        <v>1</v>
+      </c>
+      <c r="K110">
+        <v>0</v>
+      </c>
+      <c r="L110">
+        <v>1</v>
+      </c>
+      <c r="M110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>1</v>
+      </c>
+      <c r="B111">
+        <v>1</v>
+      </c>
+      <c r="C111">
+        <v>-2.2149307283435001E-2</v>
+      </c>
+      <c r="D111">
+        <v>0</v>
+      </c>
+      <c r="E111">
+        <v>0</v>
+      </c>
+      <c r="F111">
+        <v>0.14333364220759601</v>
+      </c>
+      <c r="G111">
+        <v>0</v>
+      </c>
+      <c r="H111">
+        <v>1</v>
+      </c>
+      <c r="I111">
+        <v>0</v>
+      </c>
+      <c r="J111">
+        <v>1</v>
+      </c>
+      <c r="K111">
+        <v>0</v>
+      </c>
+      <c r="L111">
+        <v>1</v>
+      </c>
+      <c r="M111" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>1</v>
+      </c>
+      <c r="B112">
+        <v>1</v>
+      </c>
+      <c r="C112">
+        <v>8.8801719935087994E-2</v>
+      </c>
+      <c r="D112">
+        <v>0</v>
+      </c>
+      <c r="E112">
+        <v>0</v>
+      </c>
+      <c r="F112">
+        <v>0.13546227647707099</v>
+      </c>
+      <c r="G112">
+        <v>0</v>
+      </c>
+      <c r="H112">
+        <v>1</v>
+      </c>
+      <c r="I112">
+        <v>0</v>
+      </c>
+      <c r="J112">
+        <v>1</v>
+      </c>
+      <c r="K112">
+        <v>0</v>
+      </c>
+      <c r="L112">
+        <v>1</v>
+      </c>
+      <c r="M112" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>1</v>
+      </c>
+      <c r="B113">
+        <v>0</v>
+      </c>
+      <c r="C113">
+        <v>0.39329211599951402</v>
+      </c>
+      <c r="D113">
+        <v>0</v>
+      </c>
+      <c r="E113">
+        <v>0</v>
+      </c>
+      <c r="F113">
+        <v>0.119987028129158</v>
+      </c>
+      <c r="G113">
+        <v>0</v>
+      </c>
+      <c r="H113">
+        <v>1</v>
+      </c>
+      <c r="I113">
+        <v>1</v>
+      </c>
+      <c r="J113">
+        <v>1</v>
+      </c>
+      <c r="K113">
+        <v>0</v>
+      </c>
+      <c r="L113">
+        <v>1</v>
+      </c>
+      <c r="M113" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>1</v>
+      </c>
+      <c r="B114">
+        <v>0</v>
+      </c>
+      <c r="C114">
+        <v>0.42201647236594703</v>
+      </c>
+      <c r="D114">
+        <v>0</v>
+      </c>
+      <c r="E114">
+        <v>0</v>
+      </c>
+      <c r="F114">
+        <v>0.114442603580084</v>
+      </c>
+      <c r="G114">
+        <v>0</v>
+      </c>
+      <c r="H114">
+        <v>1</v>
+      </c>
+      <c r="I114">
+        <v>1</v>
+      </c>
+      <c r="J114">
+        <v>1</v>
+      </c>
+      <c r="K114">
+        <v>0</v>
+      </c>
+      <c r="L114">
+        <v>1</v>
+      </c>
+      <c r="M114" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>1</v>
+      </c>
+      <c r="B115">
+        <v>1</v>
+      </c>
+      <c r="C115">
+        <v>-3.3639129227659999E-2</v>
+      </c>
+      <c r="D115">
+        <v>0</v>
+      </c>
+      <c r="E115">
+        <v>0</v>
+      </c>
+      <c r="F115">
+        <v>0.18275060627811199</v>
+      </c>
+      <c r="G115">
+        <v>0</v>
+      </c>
+      <c r="H115">
+        <v>1</v>
+      </c>
+      <c r="I115">
+        <v>0</v>
+      </c>
+      <c r="J115">
+        <v>1</v>
+      </c>
+      <c r="K115">
+        <v>0</v>
+      </c>
+      <c r="L115">
+        <v>1</v>
+      </c>
+      <c r="M115" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>1</v>
+      </c>
+      <c r="B116">
+        <v>0</v>
+      </c>
+      <c r="C116">
+        <v>0.131653626716561</v>
+      </c>
+      <c r="D116">
+        <v>0</v>
+      </c>
+      <c r="E116">
+        <v>0</v>
+      </c>
+      <c r="F116">
+        <v>0.16532338057325199</v>
+      </c>
+      <c r="G116">
+        <v>0</v>
+      </c>
+      <c r="H116">
+        <v>1</v>
+      </c>
+      <c r="I116">
+        <v>1</v>
+      </c>
+      <c r="J116">
+        <v>1</v>
+      </c>
+      <c r="K116">
+        <v>0</v>
+      </c>
+      <c r="L116">
+        <v>1</v>
+      </c>
+      <c r="M116" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>1</v>
+      </c>
+      <c r="B117">
+        <v>1</v>
+      </c>
+      <c r="C117">
+        <v>-7.3632328642180001E-2</v>
+      </c>
+      <c r="D117">
+        <v>0</v>
+      </c>
+      <c r="E117">
+        <v>0</v>
+      </c>
+      <c r="F117">
+        <v>0.15086154497582299</v>
+      </c>
+      <c r="G117">
+        <v>0</v>
+      </c>
+      <c r="H117">
+        <v>1</v>
+      </c>
+      <c r="I117">
+        <v>0</v>
+      </c>
+      <c r="J117">
+        <v>1</v>
+      </c>
+      <c r="K117">
+        <v>0</v>
+      </c>
+      <c r="L117">
+        <v>1</v>
+      </c>
+      <c r="M117" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>1</v>
+      </c>
+      <c r="B118">
+        <v>1</v>
+      </c>
+      <c r="C118">
+        <v>-8.6574032390032002E-2</v>
+      </c>
+      <c r="D118">
+        <v>0</v>
+      </c>
+      <c r="E118">
+        <v>0</v>
+      </c>
+      <c r="F118">
+        <v>0.161972763526362</v>
+      </c>
+      <c r="G118">
+        <v>0</v>
+      </c>
+      <c r="H118">
+        <v>1</v>
+      </c>
+      <c r="I118">
+        <v>0</v>
+      </c>
+      <c r="J118">
+        <v>1</v>
+      </c>
+      <c r="K118">
+        <v>0</v>
+      </c>
+      <c r="L118">
+        <v>1</v>
+      </c>
+      <c r="M118" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>1</v>
+      </c>
+      <c r="B119">
+        <v>1</v>
+      </c>
+      <c r="C119">
+        <v>0.188882448309273</v>
+      </c>
+      <c r="D119">
+        <v>0</v>
+      </c>
+      <c r="E119">
+        <v>0</v>
+      </c>
+      <c r="F119">
+        <v>0.16612496939403401</v>
+      </c>
+      <c r="G119">
+        <v>0</v>
+      </c>
+      <c r="H119">
+        <v>1</v>
+      </c>
+      <c r="I119">
+        <v>0</v>
+      </c>
+      <c r="J119">
+        <v>1</v>
+      </c>
+      <c r="K119">
+        <v>0</v>
+      </c>
+      <c r="L119">
+        <v>1</v>
+      </c>
+      <c r="M119" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>0</v>
+      </c>
+      <c r="B120">
+        <v>1</v>
+      </c>
+      <c r="C120">
+        <v>-0.28646902907161098</v>
+      </c>
+      <c r="D120">
+        <v>-1</v>
+      </c>
+      <c r="E120">
+        <v>-1</v>
+      </c>
+      <c r="F120">
+        <v>9999</v>
+      </c>
+      <c r="G120">
+        <v>1</v>
+      </c>
+      <c r="H120">
+        <v>-1</v>
+      </c>
+      <c r="I120">
+        <v>0</v>
+      </c>
+      <c r="J120">
+        <v>-1</v>
+      </c>
+      <c r="K120">
+        <v>0</v>
+      </c>
+      <c r="L120">
+        <v>0</v>
+      </c>
+      <c r="M120" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>0</v>
+      </c>
+      <c r="B121">
+        <v>0</v>
+      </c>
+      <c r="C121">
+        <v>-5.3396161354493002E-2</v>
+      </c>
+      <c r="D121">
+        <v>-1</v>
+      </c>
+      <c r="E121">
+        <v>-1</v>
+      </c>
+      <c r="F121">
+        <v>9999</v>
+      </c>
+      <c r="G121">
+        <v>1</v>
+      </c>
+      <c r="H121">
+        <v>-1</v>
+      </c>
+      <c r="I121">
+        <v>1</v>
+      </c>
+      <c r="J121">
+        <v>-1</v>
+      </c>
+      <c r="K121">
+        <v>0</v>
+      </c>
+      <c r="L121">
+        <v>0</v>
+      </c>
+      <c r="M121" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>0</v>
+      </c>
+      <c r="B122">
+        <v>0</v>
+      </c>
+      <c r="C122">
+        <v>4.9238234964948002E-2</v>
+      </c>
+      <c r="D122">
+        <v>-1</v>
+      </c>
+      <c r="E122">
+        <v>-1</v>
+      </c>
+      <c r="F122">
+        <v>9999</v>
+      </c>
+      <c r="G122">
+        <v>1</v>
+      </c>
+      <c r="H122">
+        <v>-1</v>
+      </c>
+      <c r="I122">
+        <v>1</v>
+      </c>
+      <c r="J122">
+        <v>-1</v>
+      </c>
+      <c r="K122">
+        <v>0</v>
+      </c>
+      <c r="L122">
+        <v>0</v>
+      </c>
+      <c r="M122" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>0</v>
+      </c>
+      <c r="B123">
+        <v>1</v>
+      </c>
+      <c r="C123">
+        <v>-0.113948053967053</v>
+      </c>
+      <c r="D123">
+        <v>-1</v>
+      </c>
+      <c r="E123">
+        <v>-1</v>
+      </c>
+      <c r="F123">
+        <v>9999</v>
+      </c>
+      <c r="G123">
+        <v>1</v>
+      </c>
+      <c r="H123">
+        <v>-1</v>
+      </c>
+      <c r="I123">
+        <v>0</v>
+      </c>
+      <c r="J123">
+        <v>-1</v>
+      </c>
+      <c r="K123">
+        <v>0</v>
+      </c>
+      <c r="L123">
+        <v>0</v>
+      </c>
+      <c r="M123" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>0</v>
+      </c>
+      <c r="B124">
+        <v>0</v>
+      </c>
+      <c r="C124">
+        <v>-2.2827199501822999E-2</v>
+      </c>
+      <c r="D124">
+        <v>-1</v>
+      </c>
+      <c r="E124">
+        <v>-1</v>
+      </c>
+      <c r="F124">
+        <v>9999</v>
+      </c>
+      <c r="G124">
+        <v>1</v>
+      </c>
+      <c r="H124">
+        <v>-1</v>
+      </c>
+      <c r="I124">
+        <v>1</v>
+      </c>
+      <c r="J124">
+        <v>-1</v>
+      </c>
+      <c r="K124">
+        <v>0</v>
+      </c>
+      <c r="L124">
+        <v>0</v>
+      </c>
+      <c r="M124" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>0</v>
+      </c>
+      <c r="B125">
+        <v>0</v>
+      </c>
+      <c r="C125">
+        <v>-7.1778042812712994E-2</v>
+      </c>
+      <c r="D125">
+        <v>-1</v>
+      </c>
+      <c r="E125">
+        <v>-1</v>
+      </c>
+      <c r="F125">
+        <v>9999</v>
+      </c>
+      <c r="G125">
+        <v>1</v>
+      </c>
+      <c r="H125">
+        <v>-1</v>
+      </c>
+      <c r="I125">
+        <v>1</v>
+      </c>
+      <c r="J125">
+        <v>-1</v>
+      </c>
+      <c r="K125">
+        <v>0</v>
+      </c>
+      <c r="L125">
+        <v>0</v>
+      </c>
+      <c r="M125" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>1</v>
+      </c>
+      <c r="B126">
+        <v>0</v>
+      </c>
+      <c r="C126">
+        <v>0.29731312823550199</v>
+      </c>
+      <c r="D126">
+        <v>-1</v>
+      </c>
+      <c r="E126">
+        <v>-1</v>
+      </c>
+      <c r="F126">
+        <v>9999</v>
+      </c>
+      <c r="G126">
+        <v>0</v>
+      </c>
+      <c r="H126">
+        <v>-1</v>
+      </c>
+      <c r="I126">
+        <v>1</v>
+      </c>
+      <c r="J126">
+        <v>-1</v>
+      </c>
+      <c r="K126">
+        <v>0</v>
+      </c>
+      <c r="L126">
+        <v>0</v>
+      </c>
+      <c r="M126" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>0</v>
+      </c>
+      <c r="B127">
+        <v>0</v>
+      </c>
+      <c r="C127">
+        <v>-4.0799206432488001E-2</v>
+      </c>
+      <c r="D127">
+        <v>-1</v>
+      </c>
+      <c r="E127">
+        <v>-1</v>
+      </c>
+      <c r="F127">
+        <v>9999</v>
+      </c>
+      <c r="G127">
+        <v>1</v>
+      </c>
+      <c r="H127">
+        <v>-1</v>
+      </c>
+      <c r="I127">
+        <v>1</v>
+      </c>
+      <c r="J127">
+        <v>-1</v>
+      </c>
+      <c r="K127">
+        <v>0</v>
+      </c>
+      <c r="L127">
+        <v>0</v>
+      </c>
+      <c r="M127" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>1</v>
+      </c>
+      <c r="B128">
+        <v>1</v>
+      </c>
+      <c r="C128">
+        <v>9.7118117295805995E-2</v>
+      </c>
+      <c r="D128">
+        <v>-1</v>
+      </c>
+      <c r="E128">
+        <v>-1</v>
+      </c>
+      <c r="F128">
+        <v>9999</v>
+      </c>
+      <c r="G128">
+        <v>0</v>
+      </c>
+      <c r="H128">
+        <v>-1</v>
+      </c>
+      <c r="I128">
+        <v>0</v>
+      </c>
+      <c r="J128">
+        <v>-1</v>
+      </c>
+      <c r="K128">
+        <v>0</v>
+      </c>
+      <c r="L128">
+        <v>0</v>
+      </c>
+      <c r="M128" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>0</v>
+      </c>
+      <c r="B129">
+        <v>1</v>
+      </c>
+      <c r="C129">
+        <v>-0.132014525659778</v>
+      </c>
+      <c r="D129">
+        <v>-1</v>
+      </c>
+      <c r="E129">
+        <v>-1</v>
+      </c>
+      <c r="F129">
+        <v>9999</v>
+      </c>
+      <c r="G129">
+        <v>1</v>
+      </c>
+      <c r="H129">
+        <v>-1</v>
+      </c>
+      <c r="I129">
+        <v>0</v>
+      </c>
+      <c r="J129">
+        <v>-1</v>
+      </c>
+      <c r="K129">
+        <v>0</v>
+      </c>
+      <c r="L129">
+        <v>0</v>
+      </c>
+      <c r="M129" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>1</v>
+      </c>
+      <c r="B130">
+        <v>0</v>
+      </c>
+      <c r="C130">
+        <v>9.8328866748121996E-2</v>
+      </c>
+      <c r="D130">
+        <v>-1</v>
+      </c>
+      <c r="E130">
+        <v>-1</v>
+      </c>
+      <c r="F130">
+        <v>9999</v>
+      </c>
+      <c r="G130">
+        <v>0</v>
+      </c>
+      <c r="H130">
+        <v>-1</v>
+      </c>
+      <c r="I130">
+        <v>1</v>
+      </c>
+      <c r="J130">
+        <v>-1</v>
+      </c>
+      <c r="K130">
+        <v>0</v>
+      </c>
+      <c r="L130">
+        <v>0</v>
+      </c>
+      <c r="M130" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>1</v>
+      </c>
+      <c r="B131">
+        <v>1</v>
+      </c>
+      <c r="C131">
+        <v>-3.1606544845466003E-2</v>
+      </c>
+      <c r="D131">
+        <v>-1</v>
+      </c>
+      <c r="E131">
+        <v>-1</v>
+      </c>
+      <c r="F131">
+        <v>9999</v>
+      </c>
+      <c r="G131">
+        <v>0</v>
+      </c>
+      <c r="H131">
+        <v>-1</v>
+      </c>
+      <c r="I131">
+        <v>0</v>
+      </c>
+      <c r="J131">
+        <v>-1</v>
+      </c>
+      <c r="K131">
+        <v>0</v>
+      </c>
+      <c r="L131">
+        <v>0</v>
+      </c>
+      <c r="M131" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>0</v>
+      </c>
+      <c r="B132">
+        <v>1</v>
+      </c>
+      <c r="C132">
+        <v>-0.14052126810558199</v>
+      </c>
+      <c r="D132">
+        <v>-1</v>
+      </c>
+      <c r="E132">
+        <v>-1</v>
+      </c>
+      <c r="F132">
+        <v>9999</v>
+      </c>
+      <c r="G132">
+        <v>1</v>
+      </c>
+      <c r="H132">
+        <v>-1</v>
+      </c>
+      <c r="I132">
+        <v>0</v>
+      </c>
+      <c r="J132">
+        <v>-1</v>
+      </c>
+      <c r="K132">
+        <v>0</v>
+      </c>
+      <c r="L132">
+        <v>0</v>
+      </c>
+      <c r="M132" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>1</v>
+      </c>
+      <c r="B133">
+        <v>1</v>
+      </c>
+      <c r="C133">
+        <v>9.3867991827300008E-3</v>
+      </c>
+      <c r="D133">
+        <v>-1</v>
+      </c>
+      <c r="E133">
+        <v>-1</v>
+      </c>
+      <c r="F133">
+        <v>9999</v>
+      </c>
+      <c r="G133">
+        <v>0</v>
+      </c>
+      <c r="H133">
+        <v>-1</v>
+      </c>
+      <c r="I133">
+        <v>0</v>
+      </c>
+      <c r="J133">
+        <v>-1</v>
+      </c>
+      <c r="K133">
+        <v>0</v>
+      </c>
+      <c r="L133">
+        <v>0</v>
+      </c>
+      <c r="M133" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>0</v>
+      </c>
+      <c r="B134">
+        <v>1</v>
+      </c>
+      <c r="C134">
+        <v>-6.2611224796609993E-2</v>
+      </c>
+      <c r="D134">
+        <v>-1</v>
+      </c>
+      <c r="E134">
+        <v>-1</v>
+      </c>
+      <c r="F134">
+        <v>9999</v>
+      </c>
+      <c r="G134">
+        <v>1</v>
+      </c>
+      <c r="H134">
+        <v>-1</v>
+      </c>
+      <c r="I134">
+        <v>0</v>
+      </c>
+      <c r="J134">
+        <v>-1</v>
+      </c>
+      <c r="K134">
+        <v>0</v>
+      </c>
+      <c r="L134">
+        <v>0</v>
+      </c>
+      <c r="M134" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>0</v>
+      </c>
+      <c r="B135">
+        <v>0</v>
+      </c>
+      <c r="C135">
+        <v>-9.4273370104755005E-2</v>
+      </c>
+      <c r="D135">
+        <v>-1</v>
+      </c>
+      <c r="E135">
+        <v>-1</v>
+      </c>
+      <c r="F135">
+        <v>9999</v>
+      </c>
+      <c r="G135">
+        <v>1</v>
+      </c>
+      <c r="H135">
+        <v>-1</v>
+      </c>
+      <c r="I135">
+        <v>1</v>
+      </c>
+      <c r="J135">
+        <v>-1</v>
+      </c>
+      <c r="K135">
+        <v>0</v>
+      </c>
+      <c r="L135">
+        <v>0</v>
+      </c>
+      <c r="M135" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>0</v>
+      </c>
+      <c r="B136">
+        <v>0</v>
+      </c>
+      <c r="C136">
+        <v>-4.1352144715240999E-2</v>
+      </c>
+      <c r="D136">
+        <v>-1</v>
+      </c>
+      <c r="E136">
+        <v>-1</v>
+      </c>
+      <c r="F136">
+        <v>9999</v>
+      </c>
+      <c r="G136">
+        <v>1</v>
+      </c>
+      <c r="H136">
+        <v>-1</v>
+      </c>
+      <c r="I136">
+        <v>1</v>
+      </c>
+      <c r="J136">
+        <v>-1</v>
+      </c>
+      <c r="K136">
+        <v>0</v>
+      </c>
+      <c r="L136">
+        <v>0</v>
+      </c>
+      <c r="M136" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>0</v>
+      </c>
+      <c r="B137">
+        <v>1</v>
+      </c>
+      <c r="C137">
+        <v>-0.170955061667106</v>
+      </c>
+      <c r="D137">
+        <v>-1</v>
+      </c>
+      <c r="E137">
+        <v>-1</v>
+      </c>
+      <c r="F137">
+        <v>9999</v>
+      </c>
+      <c r="G137">
+        <v>1</v>
+      </c>
+      <c r="H137">
+        <v>-1</v>
+      </c>
+      <c r="I137">
+        <v>0</v>
+      </c>
+      <c r="J137">
+        <v>-1</v>
+      </c>
+      <c r="K137">
+        <v>0</v>
+      </c>
+      <c r="L137">
+        <v>0</v>
+      </c>
+      <c r="M137" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>0</v>
+      </c>
+      <c r="B138">
+        <v>0</v>
+      </c>
+      <c r="C138">
+        <v>3.2297194598762E-2</v>
+      </c>
+      <c r="D138">
+        <v>-1</v>
+      </c>
+      <c r="E138">
+        <v>-1</v>
+      </c>
+      <c r="F138">
+        <v>9999</v>
+      </c>
+      <c r="G138">
+        <v>1</v>
+      </c>
+      <c r="H138">
+        <v>-1</v>
+      </c>
+      <c r="I138">
+        <v>1</v>
+      </c>
+      <c r="J138">
+        <v>-1</v>
+      </c>
+      <c r="K138">
+        <v>0</v>
+      </c>
+      <c r="L138">
+        <v>0</v>
+      </c>
+      <c r="M138" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>0</v>
+      </c>
+      <c r="B139">
+        <v>1</v>
+      </c>
+      <c r="C139">
+        <v>-0.12580392401559901</v>
+      </c>
+      <c r="D139">
+        <v>-1</v>
+      </c>
+      <c r="E139">
+        <v>-1</v>
+      </c>
+      <c r="F139">
+        <v>9999</v>
+      </c>
+      <c r="G139">
+        <v>1</v>
+      </c>
+      <c r="H139">
+        <v>-1</v>
+      </c>
+      <c r="I139">
+        <v>0</v>
+      </c>
+      <c r="J139">
+        <v>-1</v>
+      </c>
+      <c r="K139">
+        <v>0</v>
+      </c>
+      <c r="L139">
+        <v>0</v>
+      </c>
+      <c r="M139" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>0</v>
+      </c>
+      <c r="B140">
+        <v>1</v>
+      </c>
+      <c r="C140">
+        <v>-0.14516699160466701</v>
+      </c>
+      <c r="D140">
+        <v>1</v>
+      </c>
+      <c r="E140">
+        <v>1</v>
+      </c>
+      <c r="F140">
+        <v>-1.2909921561119E-2</v>
+      </c>
+      <c r="G140">
+        <v>1</v>
+      </c>
+      <c r="H140">
+        <v>0</v>
+      </c>
+      <c r="I140">
+        <v>0</v>
+      </c>
+      <c r="J140">
+        <v>1</v>
+      </c>
+      <c r="K140">
+        <v>1</v>
+      </c>
+      <c r="L140">
+        <v>0</v>
+      </c>
+      <c r="M140" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>0</v>
+      </c>
+      <c r="B141">
+        <v>1</v>
+      </c>
+      <c r="C141">
+        <v>-0.108710773130929</v>
+      </c>
+      <c r="D141">
+        <v>1</v>
+      </c>
+      <c r="E141">
+        <v>1</v>
+      </c>
+      <c r="F141">
+        <v>-0.151044665300369</v>
+      </c>
+      <c r="G141">
+        <v>1</v>
+      </c>
+      <c r="H141">
+        <v>0</v>
+      </c>
+      <c r="I141">
+        <v>0</v>
+      </c>
+      <c r="J141">
+        <v>0</v>
+      </c>
+      <c r="K141">
+        <v>1</v>
+      </c>
+      <c r="L141">
+        <v>0</v>
+      </c>
+      <c r="M141" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>0</v>
+      </c>
+      <c r="B142">
+        <v>0</v>
+      </c>
+      <c r="C142">
+        <v>-4.1415580338342001E-2</v>
+      </c>
+      <c r="D142">
+        <v>1</v>
+      </c>
+      <c r="E142">
+        <v>1</v>
+      </c>
+      <c r="F142">
+        <v>1.9807086544693001E-2</v>
+      </c>
+      <c r="G142">
+        <v>1</v>
+      </c>
+      <c r="H142">
+        <v>0</v>
+      </c>
+      <c r="I142">
+        <v>1</v>
+      </c>
+      <c r="J142">
+        <v>0</v>
+      </c>
+      <c r="K142">
+        <v>1</v>
+      </c>
+      <c r="L142">
+        <v>0</v>
+      </c>
+      <c r="M142" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>0</v>
+      </c>
+      <c r="B143">
+        <v>0</v>
+      </c>
+      <c r="C143">
+        <v>-5.5503613794818003E-2</v>
+      </c>
+      <c r="D143">
+        <v>1</v>
+      </c>
+      <c r="E143">
+        <v>1</v>
+      </c>
+      <c r="F143">
+        <v>-0.15675117462867499</v>
+      </c>
+      <c r="G143">
+        <v>1</v>
+      </c>
+      <c r="H143">
+        <v>0</v>
+      </c>
+      <c r="I143">
+        <v>1</v>
+      </c>
+      <c r="J143">
+        <v>1</v>
+      </c>
+      <c r="K143">
+        <v>1</v>
+      </c>
+      <c r="L143">
+        <v>0</v>
+      </c>
+      <c r="M143" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>0</v>
+      </c>
+      <c r="B144">
+        <v>0</v>
+      </c>
+      <c r="C144">
+        <v>-1.0334987043833E-2</v>
+      </c>
+      <c r="D144">
+        <v>1</v>
+      </c>
+      <c r="E144">
+        <v>1</v>
+      </c>
+      <c r="F144">
+        <v>0.112194885565971</v>
+      </c>
+      <c r="G144">
+        <v>1</v>
+      </c>
+      <c r="H144">
+        <v>0</v>
+      </c>
+      <c r="I144">
+        <v>1</v>
+      </c>
+      <c r="J144">
+        <v>0</v>
+      </c>
+      <c r="K144">
+        <v>1</v>
+      </c>
+      <c r="L144">
+        <v>0</v>
+      </c>
+      <c r="M144" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>0</v>
+      </c>
+      <c r="B145">
+        <v>0</v>
+      </c>
+      <c r="C145">
+        <v>3.1400923151384999E-2</v>
+      </c>
+      <c r="D145">
+        <v>1</v>
+      </c>
+      <c r="E145">
+        <v>1</v>
+      </c>
+      <c r="F145">
+        <v>-1.8148774905254999E-2</v>
+      </c>
+      <c r="G145">
+        <v>1</v>
+      </c>
+      <c r="H145">
+        <v>0</v>
+      </c>
+      <c r="I145">
+        <v>1</v>
+      </c>
+      <c r="J145">
+        <v>0</v>
+      </c>
+      <c r="K145">
+        <v>1</v>
+      </c>
+      <c r="L145">
+        <v>0</v>
+      </c>
+      <c r="M145" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>0</v>
+      </c>
+      <c r="B146">
+        <v>0</v>
+      </c>
+      <c r="C146">
+        <v>-2.3514409078402999E-2</v>
+      </c>
+      <c r="D146">
+        <v>1</v>
+      </c>
+      <c r="E146">
+        <v>1</v>
+      </c>
+      <c r="F146">
+        <v>2.8996786616317001E-2</v>
+      </c>
+      <c r="G146">
+        <v>1</v>
+      </c>
+      <c r="H146">
+        <v>0</v>
+      </c>
+      <c r="I146">
+        <v>1</v>
+      </c>
+      <c r="J146">
+        <v>0</v>
+      </c>
+      <c r="K146">
+        <v>1</v>
+      </c>
+      <c r="L146">
+        <v>0</v>
+      </c>
+      <c r="M146" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>1</v>
+      </c>
+      <c r="B147">
+        <v>0</v>
+      </c>
+      <c r="C147">
+        <v>0.14703262466672701</v>
+      </c>
+      <c r="D147">
+        <v>1</v>
+      </c>
+      <c r="E147">
+        <v>1</v>
+      </c>
+      <c r="F147">
+        <v>-1.7277327348650999E-2</v>
+      </c>
+      <c r="G147">
+        <v>0</v>
+      </c>
+      <c r="H147">
+        <v>0</v>
+      </c>
+      <c r="I147">
+        <v>1</v>
+      </c>
+      <c r="J147">
+        <v>0</v>
+      </c>
+      <c r="K147">
+        <v>1</v>
+      </c>
+      <c r="L147">
+        <v>0</v>
+      </c>
+      <c r="M147" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>1</v>
+      </c>
+      <c r="B148">
+        <v>0</v>
+      </c>
+      <c r="C148">
+        <v>-2.3343019326896999E-2</v>
+      </c>
+      <c r="D148">
+        <v>1</v>
+      </c>
+      <c r="E148">
+        <v>1</v>
+      </c>
+      <c r="F148">
+        <v>-2.1842091869254999E-2</v>
+      </c>
+      <c r="G148">
+        <v>0</v>
+      </c>
+      <c r="H148">
+        <v>0</v>
+      </c>
+      <c r="I148">
+        <v>1</v>
+      </c>
+      <c r="J148">
+        <v>1</v>
+      </c>
+      <c r="K148">
+        <v>1</v>
+      </c>
+      <c r="L148">
+        <v>0</v>
+      </c>
+      <c r="M148" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>1</v>
+      </c>
+      <c r="B149">
+        <v>0</v>
+      </c>
+      <c r="C149">
+        <v>0.12217737825048</v>
+      </c>
+      <c r="D149">
+        <v>1</v>
+      </c>
+      <c r="E149">
+        <v>1</v>
+      </c>
+      <c r="F149">
+        <v>2.6307797052957001E-2</v>
+      </c>
+      <c r="G149">
+        <v>0</v>
+      </c>
+      <c r="H149">
+        <v>0</v>
+      </c>
+      <c r="I149">
+        <v>1</v>
+      </c>
+      <c r="J149">
+        <v>0</v>
+      </c>
+      <c r="K149">
+        <v>1</v>
+      </c>
+      <c r="L149">
+        <v>0</v>
+      </c>
+      <c r="M149" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>0</v>
+      </c>
+      <c r="B150">
+        <v>0</v>
+      </c>
+      <c r="C150">
+        <v>-6.2141980074562002E-2</v>
+      </c>
+      <c r="D150">
+        <v>1</v>
+      </c>
+      <c r="E150">
+        <v>1</v>
+      </c>
+      <c r="F150">
+        <v>5.4960375667185001E-2</v>
+      </c>
+      <c r="G150">
+        <v>1</v>
+      </c>
+      <c r="H150">
+        <v>0</v>
+      </c>
+      <c r="I150">
+        <v>1</v>
+      </c>
+      <c r="J150">
+        <v>0</v>
+      </c>
+      <c r="K150">
+        <v>1</v>
+      </c>
+      <c r="L150">
+        <v>0</v>
+      </c>
+      <c r="M150" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>0</v>
+      </c>
+      <c r="B151">
+        <v>1</v>
+      </c>
+      <c r="C151">
+        <v>-9.4121294891075E-2</v>
+      </c>
+      <c r="D151">
+        <v>1</v>
+      </c>
+      <c r="E151">
+        <v>1</v>
+      </c>
+      <c r="F151">
+        <v>-1.449203249514E-3</v>
+      </c>
+      <c r="G151">
+        <v>1</v>
+      </c>
+      <c r="H151">
+        <v>0</v>
+      </c>
+      <c r="I151">
+        <v>0</v>
+      </c>
+      <c r="J151">
+        <v>1</v>
+      </c>
+      <c r="K151">
+        <v>1</v>
+      </c>
+      <c r="L151">
+        <v>0</v>
+      </c>
+      <c r="M151" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>0</v>
+      </c>
+      <c r="B152">
+        <v>0</v>
+      </c>
+      <c r="C152">
+        <v>-1.9769064243341E-2</v>
+      </c>
+      <c r="D152">
+        <v>1</v>
+      </c>
+      <c r="E152">
+        <v>1</v>
+      </c>
+      <c r="F152">
+        <v>-2.0380217196938E-2</v>
+      </c>
+      <c r="G152">
+        <v>1</v>
+      </c>
+      <c r="H152">
+        <v>0</v>
+      </c>
+      <c r="I152">
+        <v>1</v>
+      </c>
+      <c r="J152">
+        <v>0</v>
+      </c>
+      <c r="K152">
+        <v>1</v>
+      </c>
+      <c r="L152">
+        <v>0</v>
+      </c>
+      <c r="M152" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>0</v>
+      </c>
+      <c r="B153">
+        <v>1</v>
+      </c>
+      <c r="C153">
+        <v>-0.11479066302487199</v>
+      </c>
+      <c r="D153">
+        <v>1</v>
+      </c>
+      <c r="E153">
+        <v>1</v>
+      </c>
+      <c r="F153">
+        <v>5.2269292512020001E-3</v>
+      </c>
+      <c r="G153">
+        <v>1</v>
+      </c>
+      <c r="H153">
+        <v>0</v>
+      </c>
+      <c r="I153">
+        <v>0</v>
+      </c>
+      <c r="J153">
+        <v>0</v>
+      </c>
+      <c r="K153">
+        <v>1</v>
+      </c>
+      <c r="L153">
+        <v>0</v>
+      </c>
+      <c r="M153" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testing the newest batch of data
</commit_message>
<xml_diff>
--- a/decision_data_new.xlsx
+++ b/decision_data_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/paul_kumar_mail_utoronto_ca/Documents/engineering_masters/thesis work/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="211" documentId="6_{F6B86153-F216-4926-93F2-3946DCDAA96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{62190587-51DB-4BC1-8FD8-19ECEA351592}"/>
+  <xr:revisionPtr revIDLastSave="215" documentId="6_{F6B86153-F216-4926-93F2-3946DCDAA96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{DB3DC674-4E5F-407F-AFB9-77F28321B448}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,8 +25,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">wall_binary_2!$F$1:$F$182</definedName>
     <definedName name="_xlchart.v1.0" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">wall_mounted_data!$B$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">wall_mounted_data!$D$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">wall_mounted_data!$D$2:$D$320</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">wall_mounted_data!$E$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">wall_mounted_data!$E$2:$E$320</definedName>
     <definedName name="_xlchart.v1.12" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
     <definedName name="_xlchart.v1.13" hidden="1">wall_mounted_data!$F$1</definedName>
     <definedName name="_xlchart.v1.14" hidden="1">wall_mounted_data!$F$2:$F$320</definedName>
@@ -44,8 +44,8 @@
     <definedName name="_xlchart.v1.4" hidden="1">wall_mounted_data!$C$1</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">wall_mounted_data!$C$2:$C$320</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">wall_mounted_data!$E$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">wall_mounted_data!$E$2:$E$320</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">wall_mounted_data!$D$1</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">wall_mounted_data!$D$2:$D$320</definedName>
     <definedName name="_xlchart.v1.9" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1315" uniqueCount="21">
   <si>
     <t>first_peak</t>
   </si>
@@ -806,10 +806,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.11</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -847,7 +847,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{2E007EC1-CE09-47B1-A3E4-A95E48D1BADB}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.10</cx:f>
+              <cx:f>_xlchart.v1.7</cx:f>
               <cx:v>second_last_peak</cx:v>
             </cx:txData>
           </cx:tx>
@@ -877,10 +877,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -918,7 +918,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{28AFBDCB-EA5A-4D8B-B5F8-DF1924715131}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.7</cx:f>
+              <cx:f>_xlchart.v1.10</cx:f>
               <cx:v>last_peak</cx:v>
             </cx:txData>
           </cx:tx>
@@ -33182,10 +33182,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD048DA-A8F8-478B-A13B-D6B68CC50DBC}">
-  <dimension ref="A1:M50"/>
+  <dimension ref="A1:M93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="M75" sqref="M75:M93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35240,6 +35240,1769 @@
         <v>3</v>
       </c>
     </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>-1</v>
+      </c>
+      <c r="E51">
+        <v>-1</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>-1</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="J51">
+        <v>-1</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="L51">
+        <v>0</v>
+      </c>
+      <c r="M51" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>-1</v>
+      </c>
+      <c r="E52">
+        <v>-1</v>
+      </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>-1</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+      <c r="J52">
+        <v>-1</v>
+      </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
+      <c r="L52">
+        <v>0</v>
+      </c>
+      <c r="M52" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>-1</v>
+      </c>
+      <c r="E53">
+        <v>-1</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>-1</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+      <c r="J53">
+        <v>-1</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+      <c r="M53" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>-1</v>
+      </c>
+      <c r="E54">
+        <v>-1</v>
+      </c>
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>-1</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+      <c r="J54">
+        <v>-1</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+      <c r="L54">
+        <v>0</v>
+      </c>
+      <c r="M54" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>1</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>-1</v>
+      </c>
+      <c r="E55">
+        <v>-1</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>-1</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>-1</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+      <c r="L55">
+        <v>0</v>
+      </c>
+      <c r="M55" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>0</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>-1</v>
+      </c>
+      <c r="E56">
+        <v>-1</v>
+      </c>
+      <c r="F56">
+        <v>1</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56">
+        <v>-1</v>
+      </c>
+      <c r="I56">
+        <v>1</v>
+      </c>
+      <c r="J56">
+        <v>-1</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="L56">
+        <v>0</v>
+      </c>
+      <c r="M56" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>1</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>-1</v>
+      </c>
+      <c r="E57">
+        <v>-1</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>-1</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
+      <c r="J57">
+        <v>-1</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+      <c r="L57">
+        <v>0</v>
+      </c>
+      <c r="M57" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>-1</v>
+      </c>
+      <c r="E58">
+        <v>-1</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>-1</v>
+      </c>
+      <c r="I58">
+        <v>1</v>
+      </c>
+      <c r="J58">
+        <v>-1</v>
+      </c>
+      <c r="K58">
+        <v>0</v>
+      </c>
+      <c r="L58">
+        <v>0</v>
+      </c>
+      <c r="M58" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>-1</v>
+      </c>
+      <c r="E59">
+        <v>-1</v>
+      </c>
+      <c r="F59">
+        <v>1</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>-1</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
+      </c>
+      <c r="J59">
+        <v>-1</v>
+      </c>
+      <c r="K59">
+        <v>0</v>
+      </c>
+      <c r="L59">
+        <v>0</v>
+      </c>
+      <c r="M59" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>1</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>-1</v>
+      </c>
+      <c r="E60">
+        <v>-1</v>
+      </c>
+      <c r="F60">
+        <v>1</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>-1</v>
+      </c>
+      <c r="I60">
+        <v>1</v>
+      </c>
+      <c r="J60">
+        <v>-1</v>
+      </c>
+      <c r="K60">
+        <v>0</v>
+      </c>
+      <c r="L60">
+        <v>0</v>
+      </c>
+      <c r="M60" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>1</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>-1</v>
+      </c>
+      <c r="E61">
+        <v>-1</v>
+      </c>
+      <c r="F61">
+        <v>1</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>-1</v>
+      </c>
+      <c r="I61">
+        <v>1</v>
+      </c>
+      <c r="J61">
+        <v>-1</v>
+      </c>
+      <c r="K61">
+        <v>0</v>
+      </c>
+      <c r="L61">
+        <v>0</v>
+      </c>
+      <c r="M61" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>-1</v>
+      </c>
+      <c r="E62">
+        <v>-1</v>
+      </c>
+      <c r="F62">
+        <v>1</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>-1</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>-1</v>
+      </c>
+      <c r="K62">
+        <v>0</v>
+      </c>
+      <c r="L62">
+        <v>0</v>
+      </c>
+      <c r="M62" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <v>-1</v>
+      </c>
+      <c r="E63">
+        <v>-1</v>
+      </c>
+      <c r="F63">
+        <v>1</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>-1</v>
+      </c>
+      <c r="I63">
+        <v>1</v>
+      </c>
+      <c r="J63">
+        <v>-1</v>
+      </c>
+      <c r="K63">
+        <v>0</v>
+      </c>
+      <c r="L63">
+        <v>0</v>
+      </c>
+      <c r="M63" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+      <c r="K64">
+        <v>1</v>
+      </c>
+      <c r="L64">
+        <v>0</v>
+      </c>
+      <c r="M64" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>1</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65">
+        <v>1</v>
+      </c>
+      <c r="K65">
+        <v>1</v>
+      </c>
+      <c r="L65">
+        <v>0</v>
+      </c>
+      <c r="M65" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>0</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66">
+        <v>1</v>
+      </c>
+      <c r="K66">
+        <v>1</v>
+      </c>
+      <c r="L66">
+        <v>0</v>
+      </c>
+      <c r="M66" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>1</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+      <c r="K67">
+        <v>1</v>
+      </c>
+      <c r="L67">
+        <v>0</v>
+      </c>
+      <c r="M67" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>1</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
+      </c>
+      <c r="J68">
+        <v>1</v>
+      </c>
+      <c r="K68">
+        <v>1</v>
+      </c>
+      <c r="L68">
+        <v>0</v>
+      </c>
+      <c r="M68" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>0</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+      <c r="J69">
+        <v>1</v>
+      </c>
+      <c r="K69">
+        <v>1</v>
+      </c>
+      <c r="L69">
+        <v>0</v>
+      </c>
+      <c r="M69" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>1</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70">
+        <v>1</v>
+      </c>
+      <c r="K70">
+        <v>1</v>
+      </c>
+      <c r="L70">
+        <v>0</v>
+      </c>
+      <c r="M70" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>1</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71">
+        <v>1</v>
+      </c>
+      <c r="K71">
+        <v>1</v>
+      </c>
+      <c r="L71">
+        <v>0</v>
+      </c>
+      <c r="M71" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>1</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="J72">
+        <v>1</v>
+      </c>
+      <c r="K72">
+        <v>1</v>
+      </c>
+      <c r="L72">
+        <v>0</v>
+      </c>
+      <c r="M72" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>1</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <v>1</v>
+      </c>
+      <c r="K73">
+        <v>1</v>
+      </c>
+      <c r="L73">
+        <v>0</v>
+      </c>
+      <c r="M73" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>-1</v>
+      </c>
+      <c r="B74">
+        <v>-1</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74">
+        <v>1</v>
+      </c>
+      <c r="G74">
+        <v>-1</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+      <c r="I74">
+        <v>-1</v>
+      </c>
+      <c r="J74">
+        <v>0</v>
+      </c>
+      <c r="K74">
+        <v>1</v>
+      </c>
+      <c r="L74">
+        <v>1</v>
+      </c>
+      <c r="M74" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>1</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>1</v>
+      </c>
+      <c r="F75">
+        <v>1</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>1</v>
+      </c>
+      <c r="I75">
+        <v>1</v>
+      </c>
+      <c r="J75">
+        <v>0</v>
+      </c>
+      <c r="K75">
+        <v>0</v>
+      </c>
+      <c r="L75">
+        <v>1</v>
+      </c>
+      <c r="M75" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>-1</v>
+      </c>
+      <c r="B76">
+        <v>-1</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>1</v>
+      </c>
+      <c r="G76">
+        <v>-1</v>
+      </c>
+      <c r="H76">
+        <v>1</v>
+      </c>
+      <c r="I76">
+        <v>-1</v>
+      </c>
+      <c r="J76">
+        <v>1</v>
+      </c>
+      <c r="K76">
+        <v>1</v>
+      </c>
+      <c r="L76">
+        <v>1</v>
+      </c>
+      <c r="M76" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>-1</v>
+      </c>
+      <c r="B77">
+        <v>-1</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <v>-1</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77">
+        <v>-1</v>
+      </c>
+      <c r="J77">
+        <v>1</v>
+      </c>
+      <c r="K77">
+        <v>1</v>
+      </c>
+      <c r="L77">
+        <v>1</v>
+      </c>
+      <c r="M77" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>-1</v>
+      </c>
+      <c r="B78">
+        <v>-1</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <v>-1</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
+      <c r="I78">
+        <v>-1</v>
+      </c>
+      <c r="J78">
+        <v>1</v>
+      </c>
+      <c r="K78">
+        <v>1</v>
+      </c>
+      <c r="L78">
+        <v>1</v>
+      </c>
+      <c r="M78" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>-1</v>
+      </c>
+      <c r="B79">
+        <v>-1</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
+      <c r="F79">
+        <v>1</v>
+      </c>
+      <c r="G79">
+        <v>-1</v>
+      </c>
+      <c r="H79">
+        <v>1</v>
+      </c>
+      <c r="I79">
+        <v>-1</v>
+      </c>
+      <c r="J79">
+        <v>1</v>
+      </c>
+      <c r="K79">
+        <v>1</v>
+      </c>
+      <c r="L79">
+        <v>1</v>
+      </c>
+      <c r="M79" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>-1</v>
+      </c>
+      <c r="B80">
+        <v>-1</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <v>1</v>
+      </c>
+      <c r="G80">
+        <v>-1</v>
+      </c>
+      <c r="H80">
+        <v>1</v>
+      </c>
+      <c r="I80">
+        <v>-1</v>
+      </c>
+      <c r="J80">
+        <v>1</v>
+      </c>
+      <c r="K80">
+        <v>1</v>
+      </c>
+      <c r="L80">
+        <v>1</v>
+      </c>
+      <c r="M80" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>1</v>
+      </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
+      </c>
+      <c r="E81">
+        <v>1</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+      <c r="I81">
+        <v>1</v>
+      </c>
+      <c r="J81">
+        <v>0</v>
+      </c>
+      <c r="K81">
+        <v>0</v>
+      </c>
+      <c r="L81">
+        <v>1</v>
+      </c>
+      <c r="M81" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>1</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="C82">
+        <v>1</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>1</v>
+      </c>
+      <c r="F82">
+        <v>1</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+      <c r="H82">
+        <v>1</v>
+      </c>
+      <c r="I82">
+        <v>1</v>
+      </c>
+      <c r="J82">
+        <v>0</v>
+      </c>
+      <c r="K82">
+        <v>0</v>
+      </c>
+      <c r="L82">
+        <v>1</v>
+      </c>
+      <c r="M82" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>1</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+      <c r="C83">
+        <v>1</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
+      <c r="F83">
+        <v>1</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+      <c r="H83">
+        <v>1</v>
+      </c>
+      <c r="I83">
+        <v>1</v>
+      </c>
+      <c r="J83">
+        <v>0</v>
+      </c>
+      <c r="K83">
+        <v>0</v>
+      </c>
+      <c r="L83">
+        <v>1</v>
+      </c>
+      <c r="M83" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>1</v>
+      </c>
+      <c r="B84">
+        <v>0</v>
+      </c>
+      <c r="C84">
+        <v>1</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="E84">
+        <v>1</v>
+      </c>
+      <c r="F84">
+        <v>1</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+      <c r="H84">
+        <v>1</v>
+      </c>
+      <c r="I84">
+        <v>1</v>
+      </c>
+      <c r="J84">
+        <v>0</v>
+      </c>
+      <c r="K84">
+        <v>0</v>
+      </c>
+      <c r="L84">
+        <v>1</v>
+      </c>
+      <c r="M84" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>1</v>
+      </c>
+      <c r="B85">
+        <v>0</v>
+      </c>
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>1</v>
+      </c>
+      <c r="F85">
+        <v>1</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+      <c r="H85">
+        <v>1</v>
+      </c>
+      <c r="I85">
+        <v>1</v>
+      </c>
+      <c r="J85">
+        <v>0</v>
+      </c>
+      <c r="K85">
+        <v>0</v>
+      </c>
+      <c r="L85">
+        <v>1</v>
+      </c>
+      <c r="M85" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>1</v>
+      </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
+      <c r="C86">
+        <v>1</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86">
+        <v>1</v>
+      </c>
+      <c r="F86">
+        <v>1</v>
+      </c>
+      <c r="G86">
+        <v>0</v>
+      </c>
+      <c r="H86">
+        <v>1</v>
+      </c>
+      <c r="I86">
+        <v>1</v>
+      </c>
+      <c r="J86">
+        <v>0</v>
+      </c>
+      <c r="K86">
+        <v>0</v>
+      </c>
+      <c r="L86">
+        <v>1</v>
+      </c>
+      <c r="M86" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>1</v>
+      </c>
+      <c r="B87">
+        <v>1</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="E87">
+        <v>1</v>
+      </c>
+      <c r="F87">
+        <v>1</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+      <c r="H87">
+        <v>1</v>
+      </c>
+      <c r="I87">
+        <v>0</v>
+      </c>
+      <c r="J87">
+        <v>0</v>
+      </c>
+      <c r="K87">
+        <v>0</v>
+      </c>
+      <c r="L87">
+        <v>1</v>
+      </c>
+      <c r="M87" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>-1</v>
+      </c>
+      <c r="B88">
+        <v>-1</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>1</v>
+      </c>
+      <c r="G88">
+        <v>-1</v>
+      </c>
+      <c r="H88">
+        <v>1</v>
+      </c>
+      <c r="I88">
+        <v>-1</v>
+      </c>
+      <c r="J88">
+        <v>1</v>
+      </c>
+      <c r="K88">
+        <v>1</v>
+      </c>
+      <c r="L88">
+        <v>1</v>
+      </c>
+      <c r="M88" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>-1</v>
+      </c>
+      <c r="B89">
+        <v>-1</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="E89">
+        <v>1</v>
+      </c>
+      <c r="F89">
+        <v>1</v>
+      </c>
+      <c r="G89">
+        <v>-1</v>
+      </c>
+      <c r="H89">
+        <v>1</v>
+      </c>
+      <c r="I89">
+        <v>-1</v>
+      </c>
+      <c r="J89">
+        <v>0</v>
+      </c>
+      <c r="K89">
+        <v>1</v>
+      </c>
+      <c r="L89">
+        <v>1</v>
+      </c>
+      <c r="M89" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>-1</v>
+      </c>
+      <c r="B90">
+        <v>-1</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="F90">
+        <v>1</v>
+      </c>
+      <c r="G90">
+        <v>-1</v>
+      </c>
+      <c r="H90">
+        <v>1</v>
+      </c>
+      <c r="I90">
+        <v>-1</v>
+      </c>
+      <c r="J90">
+        <v>1</v>
+      </c>
+      <c r="K90">
+        <v>1</v>
+      </c>
+      <c r="L90">
+        <v>1</v>
+      </c>
+      <c r="M90" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>1</v>
+      </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
+      <c r="C91">
+        <v>1</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="E91">
+        <v>1</v>
+      </c>
+      <c r="F91">
+        <v>1</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+      <c r="H91">
+        <v>1</v>
+      </c>
+      <c r="I91">
+        <v>1</v>
+      </c>
+      <c r="J91">
+        <v>0</v>
+      </c>
+      <c r="K91">
+        <v>0</v>
+      </c>
+      <c r="L91">
+        <v>1</v>
+      </c>
+      <c r="M91" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>1</v>
+      </c>
+      <c r="B92">
+        <v>0</v>
+      </c>
+      <c r="C92">
+        <v>1</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="E92">
+        <v>1</v>
+      </c>
+      <c r="F92">
+        <v>1</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+      <c r="H92">
+        <v>1</v>
+      </c>
+      <c r="I92">
+        <v>1</v>
+      </c>
+      <c r="J92">
+        <v>0</v>
+      </c>
+      <c r="K92">
+        <v>0</v>
+      </c>
+      <c r="L92">
+        <v>1</v>
+      </c>
+      <c r="M92" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>1</v>
+      </c>
+      <c r="B93">
+        <v>0</v>
+      </c>
+      <c r="C93">
+        <v>1</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>1</v>
+      </c>
+      <c r="F93">
+        <v>1</v>
+      </c>
+      <c r="G93">
+        <v>0</v>
+      </c>
+      <c r="H93">
+        <v>1</v>
+      </c>
+      <c r="I93">
+        <v>1</v>
+      </c>
+      <c r="J93">
+        <v>0</v>
+      </c>
+      <c r="K93">
+        <v>0</v>
+      </c>
+      <c r="L93">
+        <v>1</v>
+      </c>
+      <c r="M93" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
rtained new model, there where errors in some left predictions
</commit_message>
<xml_diff>
--- a/decision_data_new.xlsx
+++ b/decision_data_new.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/paul_kumar_mail_utoronto_ca/Documents/engineering_masters/thesis work/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="207" documentId="6_{F6B86153-F216-4926-93F2-3946DCDAA96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2B5CAC63-57CF-4522-9145-5026292BE9A6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="6_{8CD3D5B5-6988-49B2-8D51-5FAD4B2B7139}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,28 +23,28 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">wall_binary_2!$F$1:$F$182</definedName>
     <definedName name="_xlchart.v1.0" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">wall_mounted_data!$E$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">wall_mounted_data!$C$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">wall_mounted_data!$C$2:$C$320</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">wall_mounted_data!$B$1</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">wall_mounted_data!$F$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">wall_mounted_data!$F$2:$F$320</definedName>
     <definedName name="_xlchart.v1.12" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">wall_mounted_data!$D$1</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">wall_mounted_data!$D$2:$D$320</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">wall_mounted_data!$E$1</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">wall_mounted_data!$E$2:$E$320</definedName>
     <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$A$2:$A$150</definedName>
     <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$B$1</definedName>
     <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$B$2:$B$150</definedName>
     <definedName name="_xlchart.v1.18" hidden="1">adjusted_lens!$A$2:$A$41</definedName>
     <definedName name="_xlchart.v1.19" hidden="1">adjusted_lens!$D$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">wall_mounted_data!$E$2:$E$320</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">wall_mounted_data!$B$2:$B$320</definedName>
     <definedName name="_xlchart.v1.20" hidden="1">adjusted_lens!$D$2:$D$41</definedName>
     <definedName name="_xlchart.v1.21" hidden="1">adjusted_lens!$A$2:$A$41</definedName>
     <definedName name="_xlchart.v1.22" hidden="1">adjusted_lens!$G$1</definedName>
     <definedName name="_xlchart.v1.23" hidden="1">adjusted_lens!$G$2:$G$41</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">wall_mounted_data!$F$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">wall_mounted_data!$F$2:$F$320</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">wall_mounted_data!$C$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">wall_mounted_data!$C$2:$C$320</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">wall_mounted_data!$B$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">wall_mounted_data!$B$2:$B$320</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">wall_mounted_data!$D$1</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">wall_mounted_data!$D$2:$D$320</definedName>
     <definedName name="_xlchart.v1.9" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1242" uniqueCount="21">
   <si>
     <t>first_peak</t>
   </si>
@@ -663,10 +663,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -704,7 +704,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{24F89B28-D331-4BF4-97FC-98740A0DD325}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.7</cx:f>
+              <cx:f>_xlchart.v1.1</cx:f>
               <cx:v>first_peak</cx:v>
             </cx:txData>
           </cx:tx>
@@ -734,10 +734,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.11</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -775,7 +775,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{5A2C1765-A6AF-400C-A8FA-AC7260F1E1FC}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.10</cx:f>
+              <cx:f>_xlchart.v1.4</cx:f>
               <cx:v>second_peak</cx:v>
             </cx:txData>
           </cx:tx>
@@ -805,10 +805,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.12</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.14</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -846,7 +846,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{2E007EC1-CE09-47B1-A3E4-A95E48D1BADB}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.13</cx:f>
+              <cx:f>_xlchart.v1.7</cx:f>
               <cx:v>second_last_peak</cx:v>
             </cx:txData>
           </cx:tx>
@@ -876,10 +876,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.12</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.14</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -917,7 +917,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{28AFBDCB-EA5A-4D8B-B5F8-DF1924715131}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.1</cx:f>
+              <cx:f>_xlchart.v1.13</cx:f>
               <cx:v>last_peak</cx:v>
             </cx:txData>
           </cx:tx>
@@ -947,10 +947,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -988,7 +988,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{02F72712-9CA3-4436-A6ED-93C80B1901DF}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:f>_xlchart.v1.10</cx:f>
               <cx:v>Gradient_1</cx:v>
             </cx:txData>
           </cx:tx>
@@ -26893,10 +26893,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83B5E27E-8A64-4193-B44D-44B5D7422D12}">
-  <dimension ref="A1:M153"/>
+  <dimension ref="A1:M185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M153"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33174,6 +33174,1318 @@
         <v>20</v>
       </c>
     </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>1</v>
+      </c>
+      <c r="B154">
+        <v>1</v>
+      </c>
+      <c r="C154">
+        <v>-0.13738962267853999</v>
+      </c>
+      <c r="D154">
+        <v>0</v>
+      </c>
+      <c r="E154">
+        <v>1</v>
+      </c>
+      <c r="F154">
+        <v>0.51587703602726598</v>
+      </c>
+      <c r="G154">
+        <v>0</v>
+      </c>
+      <c r="H154">
+        <v>1</v>
+      </c>
+      <c r="I154">
+        <v>0</v>
+      </c>
+      <c r="J154">
+        <v>0</v>
+      </c>
+      <c r="K154">
+        <v>0</v>
+      </c>
+      <c r="L154">
+        <v>0</v>
+      </c>
+      <c r="M154" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>0</v>
+      </c>
+      <c r="B155">
+        <v>0</v>
+      </c>
+      <c r="C155">
+        <v>-3.9210615080581997E-2</v>
+      </c>
+      <c r="D155">
+        <v>1</v>
+      </c>
+      <c r="E155">
+        <v>0</v>
+      </c>
+      <c r="F155">
+        <v>-0.70358898427225403</v>
+      </c>
+      <c r="G155">
+        <v>1</v>
+      </c>
+      <c r="H155">
+        <v>0</v>
+      </c>
+      <c r="I155">
+        <v>1</v>
+      </c>
+      <c r="J155">
+        <v>1</v>
+      </c>
+      <c r="K155">
+        <v>1</v>
+      </c>
+      <c r="L155">
+        <v>0</v>
+      </c>
+      <c r="M155" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>1</v>
+      </c>
+      <c r="B156">
+        <v>1</v>
+      </c>
+      <c r="C156">
+        <v>-0.102619998531325</v>
+      </c>
+      <c r="D156">
+        <v>0</v>
+      </c>
+      <c r="E156">
+        <v>1</v>
+      </c>
+      <c r="F156">
+        <v>0.58974518722783797</v>
+      </c>
+      <c r="G156">
+        <v>0</v>
+      </c>
+      <c r="H156">
+        <v>1</v>
+      </c>
+      <c r="I156">
+        <v>0</v>
+      </c>
+      <c r="J156">
+        <v>0</v>
+      </c>
+      <c r="K156">
+        <v>0</v>
+      </c>
+      <c r="L156">
+        <v>0</v>
+      </c>
+      <c r="M156" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>1</v>
+      </c>
+      <c r="B157">
+        <v>1</v>
+      </c>
+      <c r="C157">
+        <v>0.206725430578036</v>
+      </c>
+      <c r="D157">
+        <v>1</v>
+      </c>
+      <c r="E157">
+        <v>0</v>
+      </c>
+      <c r="F157">
+        <v>-0.53174863780797899</v>
+      </c>
+      <c r="G157">
+        <v>0</v>
+      </c>
+      <c r="H157">
+        <v>0</v>
+      </c>
+      <c r="I157">
+        <v>0</v>
+      </c>
+      <c r="J157">
+        <v>1</v>
+      </c>
+      <c r="K157">
+        <v>1</v>
+      </c>
+      <c r="L157">
+        <v>1</v>
+      </c>
+      <c r="M157" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>1</v>
+      </c>
+      <c r="B158">
+        <v>0</v>
+      </c>
+      <c r="C158">
+        <v>0.48798652063946701</v>
+      </c>
+      <c r="D158">
+        <v>0</v>
+      </c>
+      <c r="E158">
+        <v>0</v>
+      </c>
+      <c r="F158">
+        <v>0.50624694473689502</v>
+      </c>
+      <c r="G158">
+        <v>0</v>
+      </c>
+      <c r="H158">
+        <v>1</v>
+      </c>
+      <c r="I158">
+        <v>1</v>
+      </c>
+      <c r="J158">
+        <v>1</v>
+      </c>
+      <c r="K158">
+        <v>0</v>
+      </c>
+      <c r="L158">
+        <v>0</v>
+      </c>
+      <c r="M158" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>0</v>
+      </c>
+      <c r="B159">
+        <v>1</v>
+      </c>
+      <c r="C159">
+        <v>-0.37806983269879302</v>
+      </c>
+      <c r="D159">
+        <v>1</v>
+      </c>
+      <c r="E159">
+        <v>0</v>
+      </c>
+      <c r="F159">
+        <v>-0.44788265580733</v>
+      </c>
+      <c r="G159">
+        <v>1</v>
+      </c>
+      <c r="H159">
+        <v>0</v>
+      </c>
+      <c r="I159">
+        <v>0</v>
+      </c>
+      <c r="J159">
+        <v>1</v>
+      </c>
+      <c r="K159">
+        <v>1</v>
+      </c>
+      <c r="L159">
+        <v>1</v>
+      </c>
+      <c r="M159" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>1</v>
+      </c>
+      <c r="B160">
+        <v>0</v>
+      </c>
+      <c r="C160">
+        <v>0.194314234221142</v>
+      </c>
+      <c r="D160">
+        <v>0</v>
+      </c>
+      <c r="E160">
+        <v>1</v>
+      </c>
+      <c r="F160">
+        <v>0.58985349585669</v>
+      </c>
+      <c r="G160">
+        <v>0</v>
+      </c>
+      <c r="H160">
+        <v>1</v>
+      </c>
+      <c r="I160">
+        <v>1</v>
+      </c>
+      <c r="J160">
+        <v>0</v>
+      </c>
+      <c r="K160">
+        <v>0</v>
+      </c>
+      <c r="L160">
+        <v>0</v>
+      </c>
+      <c r="M160" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>1</v>
+      </c>
+      <c r="B161">
+        <v>0</v>
+      </c>
+      <c r="C161">
+        <v>0.24350109352591601</v>
+      </c>
+      <c r="D161">
+        <v>1</v>
+      </c>
+      <c r="E161">
+        <v>1</v>
+      </c>
+      <c r="F161">
+        <v>-0.134318306610581</v>
+      </c>
+      <c r="G161">
+        <v>0</v>
+      </c>
+      <c r="H161">
+        <v>0</v>
+      </c>
+      <c r="I161">
+        <v>1</v>
+      </c>
+      <c r="J161">
+        <v>0</v>
+      </c>
+      <c r="K161">
+        <v>1</v>
+      </c>
+      <c r="L161">
+        <v>1</v>
+      </c>
+      <c r="M161" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>1</v>
+      </c>
+      <c r="B162">
+        <v>0</v>
+      </c>
+      <c r="C162">
+        <v>0.37594547062094302</v>
+      </c>
+      <c r="D162">
+        <v>0</v>
+      </c>
+      <c r="E162">
+        <v>1</v>
+      </c>
+      <c r="F162">
+        <v>0.568360709737739</v>
+      </c>
+      <c r="G162">
+        <v>0</v>
+      </c>
+      <c r="H162">
+        <v>1</v>
+      </c>
+      <c r="I162">
+        <v>1</v>
+      </c>
+      <c r="J162">
+        <v>1</v>
+      </c>
+      <c r="K162">
+        <v>0</v>
+      </c>
+      <c r="L162">
+        <v>0</v>
+      </c>
+      <c r="M162" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>1</v>
+      </c>
+      <c r="B163">
+        <v>1</v>
+      </c>
+      <c r="C163">
+        <v>4.5140250812914999E-2</v>
+      </c>
+      <c r="D163">
+        <v>1</v>
+      </c>
+      <c r="E163">
+        <v>1</v>
+      </c>
+      <c r="F163">
+        <v>-7.3240283100208997E-2</v>
+      </c>
+      <c r="G163">
+        <v>0</v>
+      </c>
+      <c r="H163">
+        <v>0</v>
+      </c>
+      <c r="I163">
+        <v>0</v>
+      </c>
+      <c r="J163">
+        <v>0</v>
+      </c>
+      <c r="K163">
+        <v>1</v>
+      </c>
+      <c r="L163">
+        <v>1</v>
+      </c>
+      <c r="M163" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>1</v>
+      </c>
+      <c r="B164">
+        <v>1</v>
+      </c>
+      <c r="C164">
+        <v>-0.16375735357659399</v>
+      </c>
+      <c r="D164">
+        <v>0</v>
+      </c>
+      <c r="E164">
+        <v>1</v>
+      </c>
+      <c r="F164">
+        <v>0.57558489305098903</v>
+      </c>
+      <c r="G164">
+        <v>0</v>
+      </c>
+      <c r="H164">
+        <v>1</v>
+      </c>
+      <c r="I164">
+        <v>0</v>
+      </c>
+      <c r="J164">
+        <v>0</v>
+      </c>
+      <c r="K164">
+        <v>0</v>
+      </c>
+      <c r="L164">
+        <v>0</v>
+      </c>
+      <c r="M164" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>1</v>
+      </c>
+      <c r="B165">
+        <v>1</v>
+      </c>
+      <c r="C165">
+        <v>-7.5502637399739003E-2</v>
+      </c>
+      <c r="D165">
+        <v>1</v>
+      </c>
+      <c r="E165">
+        <v>1</v>
+      </c>
+      <c r="F165">
+        <v>-0.152070072121571</v>
+      </c>
+      <c r="G165">
+        <v>0</v>
+      </c>
+      <c r="H165">
+        <v>0</v>
+      </c>
+      <c r="I165">
+        <v>0</v>
+      </c>
+      <c r="J165">
+        <v>0</v>
+      </c>
+      <c r="K165">
+        <v>1</v>
+      </c>
+      <c r="L165">
+        <v>1</v>
+      </c>
+      <c r="M165" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>1</v>
+      </c>
+      <c r="B166">
+        <v>0</v>
+      </c>
+      <c r="C166">
+        <v>0.21027304138696001</v>
+      </c>
+      <c r="D166">
+        <v>0</v>
+      </c>
+      <c r="E166">
+        <v>1</v>
+      </c>
+      <c r="F166">
+        <v>0.52947422451341197</v>
+      </c>
+      <c r="G166">
+        <v>0</v>
+      </c>
+      <c r="H166">
+        <v>1</v>
+      </c>
+      <c r="I166">
+        <v>1</v>
+      </c>
+      <c r="J166">
+        <v>1</v>
+      </c>
+      <c r="K166">
+        <v>0</v>
+      </c>
+      <c r="L166">
+        <v>0</v>
+      </c>
+      <c r="M166" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>1</v>
+      </c>
+      <c r="B167">
+        <v>0</v>
+      </c>
+      <c r="C167">
+        <v>0.21049130578338901</v>
+      </c>
+      <c r="D167">
+        <v>1</v>
+      </c>
+      <c r="E167">
+        <v>1</v>
+      </c>
+      <c r="F167">
+        <v>-0.107316276816038</v>
+      </c>
+      <c r="G167">
+        <v>0</v>
+      </c>
+      <c r="H167">
+        <v>0</v>
+      </c>
+      <c r="I167">
+        <v>1</v>
+      </c>
+      <c r="J167">
+        <v>0</v>
+      </c>
+      <c r="K167">
+        <v>1</v>
+      </c>
+      <c r="L167">
+        <v>1</v>
+      </c>
+      <c r="M167" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>1</v>
+      </c>
+      <c r="B168">
+        <v>0</v>
+      </c>
+      <c r="C168">
+        <v>0.156062314922704</v>
+      </c>
+      <c r="D168">
+        <v>0</v>
+      </c>
+      <c r="E168">
+        <v>1</v>
+      </c>
+      <c r="F168">
+        <v>0.57589516671274399</v>
+      </c>
+      <c r="G168">
+        <v>0</v>
+      </c>
+      <c r="H168">
+        <v>1</v>
+      </c>
+      <c r="I168">
+        <v>1</v>
+      </c>
+      <c r="J168">
+        <v>1</v>
+      </c>
+      <c r="K168">
+        <v>0</v>
+      </c>
+      <c r="L168">
+        <v>0</v>
+      </c>
+      <c r="M168" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>1</v>
+      </c>
+      <c r="B169">
+        <v>0</v>
+      </c>
+      <c r="C169">
+        <v>0.22530120363701001</v>
+      </c>
+      <c r="D169">
+        <v>1</v>
+      </c>
+      <c r="E169">
+        <v>1</v>
+      </c>
+      <c r="F169">
+        <v>-5.8773997350353997E-2</v>
+      </c>
+      <c r="G169">
+        <v>0</v>
+      </c>
+      <c r="H169">
+        <v>0</v>
+      </c>
+      <c r="I169">
+        <v>1</v>
+      </c>
+      <c r="J169">
+        <v>0</v>
+      </c>
+      <c r="K169">
+        <v>1</v>
+      </c>
+      <c r="L169">
+        <v>1</v>
+      </c>
+      <c r="M169" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>1</v>
+      </c>
+      <c r="B170">
+        <v>0</v>
+      </c>
+      <c r="C170">
+        <v>0.20975386895383999</v>
+      </c>
+      <c r="D170">
+        <v>0</v>
+      </c>
+      <c r="E170">
+        <v>1</v>
+      </c>
+      <c r="F170">
+        <v>0.59143480040240204</v>
+      </c>
+      <c r="G170">
+        <v>0</v>
+      </c>
+      <c r="H170">
+        <v>1</v>
+      </c>
+      <c r="I170">
+        <v>1</v>
+      </c>
+      <c r="J170">
+        <v>1</v>
+      </c>
+      <c r="K170">
+        <v>0</v>
+      </c>
+      <c r="L170">
+        <v>0</v>
+      </c>
+      <c r="M170" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>0</v>
+      </c>
+      <c r="B171">
+        <v>0</v>
+      </c>
+      <c r="C171">
+        <v>-5.3589796034666001E-2</v>
+      </c>
+      <c r="D171">
+        <v>1</v>
+      </c>
+      <c r="E171">
+        <v>0</v>
+      </c>
+      <c r="F171">
+        <v>-0.44116138640098101</v>
+      </c>
+      <c r="G171">
+        <v>1</v>
+      </c>
+      <c r="H171">
+        <v>0</v>
+      </c>
+      <c r="I171">
+        <v>1</v>
+      </c>
+      <c r="J171">
+        <v>1</v>
+      </c>
+      <c r="K171">
+        <v>1</v>
+      </c>
+      <c r="L171">
+        <v>1</v>
+      </c>
+      <c r="M171" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>1</v>
+      </c>
+      <c r="B172">
+        <v>0</v>
+      </c>
+      <c r="C172">
+        <v>0.118097000032258</v>
+      </c>
+      <c r="D172">
+        <v>0</v>
+      </c>
+      <c r="E172">
+        <v>1</v>
+      </c>
+      <c r="F172">
+        <v>0.58355679818873396</v>
+      </c>
+      <c r="G172">
+        <v>0</v>
+      </c>
+      <c r="H172">
+        <v>1</v>
+      </c>
+      <c r="I172">
+        <v>1</v>
+      </c>
+      <c r="J172">
+        <v>0</v>
+      </c>
+      <c r="K172">
+        <v>0</v>
+      </c>
+      <c r="L172">
+        <v>0</v>
+      </c>
+      <c r="M172" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>1</v>
+      </c>
+      <c r="B173">
+        <v>1</v>
+      </c>
+      <c r="C173">
+        <v>2.2126371731535002E-2</v>
+      </c>
+      <c r="D173">
+        <v>1</v>
+      </c>
+      <c r="E173">
+        <v>0</v>
+      </c>
+      <c r="F173">
+        <v>-0.43297523314370501</v>
+      </c>
+      <c r="G173">
+        <v>0</v>
+      </c>
+      <c r="H173">
+        <v>0</v>
+      </c>
+      <c r="I173">
+        <v>0</v>
+      </c>
+      <c r="J173">
+        <v>1</v>
+      </c>
+      <c r="K173">
+        <v>1</v>
+      </c>
+      <c r="L173">
+        <v>1</v>
+      </c>
+      <c r="M173" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>1</v>
+      </c>
+      <c r="B174">
+        <v>0</v>
+      </c>
+      <c r="C174">
+        <v>-7.8127783411249992E-3</v>
+      </c>
+      <c r="D174">
+        <v>0</v>
+      </c>
+      <c r="E174">
+        <v>1</v>
+      </c>
+      <c r="F174">
+        <v>0.57549723120140195</v>
+      </c>
+      <c r="G174">
+        <v>0</v>
+      </c>
+      <c r="H174">
+        <v>1</v>
+      </c>
+      <c r="I174">
+        <v>1</v>
+      </c>
+      <c r="J174">
+        <v>0</v>
+      </c>
+      <c r="K174">
+        <v>0</v>
+      </c>
+      <c r="L174">
+        <v>0</v>
+      </c>
+      <c r="M174" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>1</v>
+      </c>
+      <c r="B175">
+        <v>0</v>
+      </c>
+      <c r="C175">
+        <v>0.24714067545398299</v>
+      </c>
+      <c r="D175">
+        <v>1</v>
+      </c>
+      <c r="E175">
+        <v>1</v>
+      </c>
+      <c r="F175">
+        <v>-8.5041133398212995E-2</v>
+      </c>
+      <c r="G175">
+        <v>0</v>
+      </c>
+      <c r="H175">
+        <v>0</v>
+      </c>
+      <c r="I175">
+        <v>1</v>
+      </c>
+      <c r="J175">
+        <v>0</v>
+      </c>
+      <c r="K175">
+        <v>1</v>
+      </c>
+      <c r="L175">
+        <v>1</v>
+      </c>
+      <c r="M175" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>1</v>
+      </c>
+      <c r="B176">
+        <v>1</v>
+      </c>
+      <c r="C176">
+        <v>-3.6960445064643001E-2</v>
+      </c>
+      <c r="D176">
+        <v>0</v>
+      </c>
+      <c r="E176">
+        <v>1</v>
+      </c>
+      <c r="F176">
+        <v>0.51996780701656298</v>
+      </c>
+      <c r="G176">
+        <v>0</v>
+      </c>
+      <c r="H176">
+        <v>1</v>
+      </c>
+      <c r="I176">
+        <v>0</v>
+      </c>
+      <c r="J176">
+        <v>1</v>
+      </c>
+      <c r="K176">
+        <v>0</v>
+      </c>
+      <c r="L176">
+        <v>0</v>
+      </c>
+      <c r="M176" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>0</v>
+      </c>
+      <c r="B177">
+        <v>0</v>
+      </c>
+      <c r="C177">
+        <v>-3.1647155362772003E-2</v>
+      </c>
+      <c r="D177">
+        <v>1</v>
+      </c>
+      <c r="E177">
+        <v>1</v>
+      </c>
+      <c r="F177">
+        <v>-8.8591282741013994E-2</v>
+      </c>
+      <c r="G177">
+        <v>1</v>
+      </c>
+      <c r="H177">
+        <v>0</v>
+      </c>
+      <c r="I177">
+        <v>1</v>
+      </c>
+      <c r="J177">
+        <v>0</v>
+      </c>
+      <c r="K177">
+        <v>1</v>
+      </c>
+      <c r="L177">
+        <v>1</v>
+      </c>
+      <c r="M177" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>1</v>
+      </c>
+      <c r="B178">
+        <v>1</v>
+      </c>
+      <c r="C178">
+        <v>-0.113467651190855</v>
+      </c>
+      <c r="D178">
+        <v>0</v>
+      </c>
+      <c r="E178">
+        <v>1</v>
+      </c>
+      <c r="F178">
+        <v>0.59880642242594895</v>
+      </c>
+      <c r="G178">
+        <v>0</v>
+      </c>
+      <c r="H178">
+        <v>1</v>
+      </c>
+      <c r="I178">
+        <v>0</v>
+      </c>
+      <c r="J178">
+        <v>0</v>
+      </c>
+      <c r="K178">
+        <v>0</v>
+      </c>
+      <c r="L178">
+        <v>0</v>
+      </c>
+      <c r="M178" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>0</v>
+      </c>
+      <c r="B179">
+        <v>0</v>
+      </c>
+      <c r="C179">
+        <v>6.3032824387702996E-2</v>
+      </c>
+      <c r="D179">
+        <v>1</v>
+      </c>
+      <c r="E179">
+        <v>0</v>
+      </c>
+      <c r="F179">
+        <v>-0.45504249910063499</v>
+      </c>
+      <c r="G179">
+        <v>1</v>
+      </c>
+      <c r="H179">
+        <v>0</v>
+      </c>
+      <c r="I179">
+        <v>1</v>
+      </c>
+      <c r="J179">
+        <v>1</v>
+      </c>
+      <c r="K179">
+        <v>1</v>
+      </c>
+      <c r="L179">
+        <v>1</v>
+      </c>
+      <c r="M179" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>1</v>
+      </c>
+      <c r="B180">
+        <v>1</v>
+      </c>
+      <c r="C180">
+        <v>-0.13805112357704599</v>
+      </c>
+      <c r="D180">
+        <v>0</v>
+      </c>
+      <c r="E180">
+        <v>1</v>
+      </c>
+      <c r="F180">
+        <v>0.58491461213679996</v>
+      </c>
+      <c r="G180">
+        <v>0</v>
+      </c>
+      <c r="H180">
+        <v>1</v>
+      </c>
+      <c r="I180">
+        <v>0</v>
+      </c>
+      <c r="J180">
+        <v>1</v>
+      </c>
+      <c r="K180">
+        <v>0</v>
+      </c>
+      <c r="L180">
+        <v>0</v>
+      </c>
+      <c r="M180" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>0</v>
+      </c>
+      <c r="B181">
+        <v>0</v>
+      </c>
+      <c r="C181">
+        <v>2.5131818367733001E-2</v>
+      </c>
+      <c r="D181">
+        <v>1</v>
+      </c>
+      <c r="E181">
+        <v>0</v>
+      </c>
+      <c r="F181">
+        <v>-0.430603666451496</v>
+      </c>
+      <c r="G181">
+        <v>1</v>
+      </c>
+      <c r="H181">
+        <v>0</v>
+      </c>
+      <c r="I181">
+        <v>1</v>
+      </c>
+      <c r="J181">
+        <v>1</v>
+      </c>
+      <c r="K181">
+        <v>1</v>
+      </c>
+      <c r="L181">
+        <v>0</v>
+      </c>
+      <c r="M181" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>1</v>
+      </c>
+      <c r="B182">
+        <v>1</v>
+      </c>
+      <c r="C182">
+        <v>-4.6062546737821002E-2</v>
+      </c>
+      <c r="D182">
+        <v>0</v>
+      </c>
+      <c r="E182">
+        <v>1</v>
+      </c>
+      <c r="F182">
+        <v>0.55551737989622096</v>
+      </c>
+      <c r="G182">
+        <v>0</v>
+      </c>
+      <c r="H182">
+        <v>1</v>
+      </c>
+      <c r="I182">
+        <v>0</v>
+      </c>
+      <c r="J182">
+        <v>0</v>
+      </c>
+      <c r="K182">
+        <v>0</v>
+      </c>
+      <c r="L182">
+        <v>0</v>
+      </c>
+      <c r="M182" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>1</v>
+      </c>
+      <c r="B183">
+        <v>0</v>
+      </c>
+      <c r="C183">
+        <v>0.380606181479971</v>
+      </c>
+      <c r="D183">
+        <v>1</v>
+      </c>
+      <c r="E183">
+        <v>0</v>
+      </c>
+      <c r="F183">
+        <v>-0.588463870852306</v>
+      </c>
+      <c r="G183">
+        <v>0</v>
+      </c>
+      <c r="H183">
+        <v>0</v>
+      </c>
+      <c r="I183">
+        <v>1</v>
+      </c>
+      <c r="J183">
+        <v>1</v>
+      </c>
+      <c r="K183">
+        <v>1</v>
+      </c>
+      <c r="L183">
+        <v>0</v>
+      </c>
+      <c r="M183" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>1</v>
+      </c>
+      <c r="B184">
+        <v>0</v>
+      </c>
+      <c r="C184">
+        <v>0.21261656138578</v>
+      </c>
+      <c r="D184">
+        <v>0</v>
+      </c>
+      <c r="E184">
+        <v>1</v>
+      </c>
+      <c r="F184">
+        <v>0.55384132410582898</v>
+      </c>
+      <c r="G184">
+        <v>0</v>
+      </c>
+      <c r="H184">
+        <v>1</v>
+      </c>
+      <c r="I184">
+        <v>1</v>
+      </c>
+      <c r="J184">
+        <v>0</v>
+      </c>
+      <c r="K184">
+        <v>0</v>
+      </c>
+      <c r="L184">
+        <v>0</v>
+      </c>
+      <c r="M184" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>1</v>
+      </c>
+      <c r="B185">
+        <v>1</v>
+      </c>
+      <c r="C185">
+        <v>0.14534180474835701</v>
+      </c>
+      <c r="D185">
+        <v>1</v>
+      </c>
+      <c r="E185">
+        <v>1</v>
+      </c>
+      <c r="F185">
+        <v>-5.5894741287923003E-2</v>
+      </c>
+      <c r="G185">
+        <v>0</v>
+      </c>
+      <c r="H185">
+        <v>0</v>
+      </c>
+      <c r="I185">
+        <v>0</v>
+      </c>
+      <c r="J185">
+        <v>1</v>
+      </c>
+      <c r="K185">
+        <v>1</v>
+      </c>
+      <c r="L185">
+        <v>1</v>
+      </c>
+      <c r="M185" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
making chnages to data screening
</commit_message>
<xml_diff>
--- a/decision_data_new.xlsx
+++ b/decision_data_new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/paul_kumar_mail_utoronto_ca/Documents/engineering_masters/thesis work/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="215" documentId="6_{F6B86153-F216-4926-93F2-3946DCDAA96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{DB3DC674-4E5F-407F-AFB9-77F28321B448}"/>
+  <xr:revisionPtr revIDLastSave="223" documentId="6_{F6B86153-F216-4926-93F2-3946DCDAA96A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{B3CDF8E8-C533-4B54-8641-7921A04FBC2D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15480" yWindow="-120" windowWidth="15600" windowHeight="11160" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wall_mounted_data" sheetId="12" r:id="rId1"/>
@@ -22,14 +22,15 @@
     <sheet name="sys2" sheetId="25" r:id="rId7"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'sys2'!$M$2:$M$93</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">wall_binary_2!$F$1:$F$182</definedName>
     <definedName name="_xlchart.v1.0" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">wall_mounted_data!$B$1</definedName>
     <definedName name="_xlchart.v1.10" hidden="1">wall_mounted_data!$E$1</definedName>
     <definedName name="_xlchart.v1.11" hidden="1">wall_mounted_data!$E$2:$E$320</definedName>
     <definedName name="_xlchart.v1.12" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">wall_mounted_data!$F$1</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">wall_mounted_data!$F$2:$F$320</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">wall_mounted_data!$D$1</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">wall_mounted_data!$D$2:$D$320</definedName>
     <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$A$2:$A$150</definedName>
     <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$B$1</definedName>
     <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$B$2:$B$150</definedName>
@@ -44,11 +45,21 @@
     <definedName name="_xlchart.v1.4" hidden="1">wall_mounted_data!$C$1</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">wall_mounted_data!$C$2:$C$320</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">wall_mounted_data!$D$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">wall_mounted_data!$D$2:$D$320</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">wall_mounted_data!$F$1</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">wall_mounted_data!$F$2:$F$320</definedName>
     <definedName name="_xlchart.v1.9" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -806,10 +817,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.12</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.14</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -847,7 +858,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{2E007EC1-CE09-47B1-A3E4-A95E48D1BADB}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.7</cx:f>
+              <cx:f>_xlchart.v1.13</cx:f>
               <cx:v>second_last_peak</cx:v>
             </cx:txData>
           </cx:tx>
@@ -948,10 +959,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.12</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.14</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -989,7 +1000,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{02F72712-9CA3-4436-A6ED-93C80B1901DF}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.13</cx:f>
+              <cx:f>_xlchart.v1.7</cx:f>
               <cx:v>Gradient_1</cx:v>
             </cx:txData>
           </cx:tx>
@@ -33182,10 +33193,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD048DA-A8F8-478B-A13B-D6B68CC50DBC}">
-  <dimension ref="A1:M93"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:M94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="M75" sqref="M75:M93"/>
+    <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
+      <selection activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33272,7 +33284,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -33313,7 +33325,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -33354,7 +33366,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -33395,7 +33407,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -33436,7 +33448,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -33477,7 +33489,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -33518,7 +33530,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -33559,7 +33571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -33600,7 +33612,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -33641,7 +33653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -33682,7 +33694,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -33723,7 +33735,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -33764,7 +33776,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -33805,7 +33817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -33846,7 +33858,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -33887,7 +33899,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -33928,7 +33940,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -33969,7 +33981,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -34010,7 +34022,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -34051,7 +34063,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -34092,7 +34104,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -34133,7 +34145,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -34174,7 +34186,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -34215,7 +34227,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -34256,7 +34268,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -34297,7 +34309,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -34338,7 +34350,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -34379,7 +34391,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
@@ -34420,7 +34432,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1</v>
       </c>
@@ -34461,7 +34473,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -34502,7 +34514,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
@@ -34543,7 +34555,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1</v>
       </c>
@@ -34584,7 +34596,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1</v>
       </c>
@@ -34625,7 +34637,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
@@ -34666,7 +34678,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1</v>
       </c>
@@ -34707,7 +34719,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1</v>
       </c>
@@ -34748,7 +34760,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1</v>
       </c>
@@ -34789,7 +34801,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>0</v>
       </c>
@@ -34830,7 +34842,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1</v>
       </c>
@@ -34871,7 +34883,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1</v>
       </c>
@@ -34912,7 +34924,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1</v>
       </c>
@@ -34953,7 +34965,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1</v>
       </c>
@@ -34994,7 +35006,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1</v>
       </c>
@@ -35035,7 +35047,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1</v>
       </c>
@@ -35076,7 +35088,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1</v>
       </c>
@@ -35117,7 +35129,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1</v>
       </c>
@@ -35158,7 +35170,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1</v>
       </c>
@@ -35199,7 +35211,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1</v>
       </c>
@@ -36183,7 +36195,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>-1</v>
       </c>
@@ -36224,7 +36236,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>1</v>
       </c>
@@ -36265,7 +36277,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>-1</v>
       </c>
@@ -36306,7 +36318,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>-1</v>
       </c>
@@ -36347,7 +36359,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>-1</v>
       </c>
@@ -36388,7 +36400,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>-1</v>
       </c>
@@ -36429,7 +36441,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>-1</v>
       </c>
@@ -36470,7 +36482,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>1</v>
       </c>
@@ -36511,7 +36523,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>1</v>
       </c>
@@ -36552,7 +36564,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>1</v>
       </c>
@@ -36593,7 +36605,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>1</v>
       </c>
@@ -36634,7 +36646,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>1</v>
       </c>
@@ -36675,7 +36687,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>1</v>
       </c>
@@ -36716,7 +36728,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>1</v>
       </c>
@@ -36757,7 +36769,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>-1</v>
       </c>
@@ -36798,7 +36810,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>-1</v>
       </c>
@@ -36839,7 +36851,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>-1</v>
       </c>
@@ -36880,7 +36892,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>1</v>
       </c>
@@ -36921,7 +36933,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>1</v>
       </c>
@@ -36962,7 +36974,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>1</v>
       </c>
@@ -37003,7 +37015,64 @@
         <v>20</v>
       </c>
     </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <f>SUM(A51:A73)/COUNT(A51:A73)</f>
+        <v>0.86956521739130432</v>
+      </c>
+      <c r="B94">
+        <f t="shared" ref="B94:L94" si="0">SUM(B51:B73)/COUNT(B51:B73)</f>
+        <v>0.52173913043478259</v>
+      </c>
+      <c r="C94">
+        <f t="shared" si="0"/>
+        <v>0.78260869565217395</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="0"/>
+        <v>-0.17391304347826086</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="0"/>
+        <v>-0.47826086956521741</v>
+      </c>
+      <c r="F94">
+        <f t="shared" si="0"/>
+        <v>0.60869565217391308</v>
+      </c>
+      <c r="G94">
+        <f t="shared" si="0"/>
+        <v>0.13043478260869565</v>
+      </c>
+      <c r="H94">
+        <f>ABS(SUM(H51:H73))/COUNT(H51:H73)</f>
+        <v>0.52173913043478259</v>
+      </c>
+      <c r="I94">
+        <f t="shared" si="0"/>
+        <v>0.47826086956521741</v>
+      </c>
+      <c r="J94">
+        <f t="shared" si="0"/>
+        <v>-0.21739130434782608</v>
+      </c>
+      <c r="K94">
+        <f t="shared" si="0"/>
+        <v>0.43478260869565216</v>
+      </c>
+      <c r="L94">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="M2:M93" xr:uid="{741387AA-246E-42DC-BA1D-D20018C22044}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="No-left"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fucked up a merge again.....
</commit_message>
<xml_diff>
--- a/decision_data_new.xlsx
+++ b/decision_data_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/paul_kumar_mail_utoronto_ca/Documents/engineering_masters/thesis work/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="230" documentId="6_{F6B86153-F216-4926-93F2-3946DCDAA96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{EBBFBE73-3FFF-4053-851C-D23F618350FF}"/>
+  <xr:revisionPtr revIDLastSave="231" documentId="6_{F6B86153-F216-4926-93F2-3946DCDAA96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E11D7730-4475-4408-B43F-FD2D63EDE5D1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">wall_binary_2!$F$1:$F$182</definedName>
     <definedName name="_xlchart.v1.0" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">wall_mounted_data!$C$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">wall_mounted_data!$B$1</definedName>
     <definedName name="_xlchart.v1.10" hidden="1">wall_mounted_data!$E$1</definedName>
     <definedName name="_xlchart.v1.11" hidden="1">wall_mounted_data!$E$2:$E$320</definedName>
     <definedName name="_xlchart.v1.12" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
@@ -34,18 +34,18 @@
     <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$B$1</definedName>
     <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$B$2:$B$150</definedName>
     <definedName name="_xlchart.v1.18" hidden="1">adjusted_lens!$A$2:$A$41</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">adjusted_lens!$G$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">wall_mounted_data!$C$2:$C$320</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">adjusted_lens!$G$2:$G$41</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">adjusted_lens!$D$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">wall_mounted_data!$B$2:$B$320</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">adjusted_lens!$D$2:$D$41</definedName>
     <definedName name="_xlchart.v1.21" hidden="1">adjusted_lens!$A$2:$A$41</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">adjusted_lens!$D$1</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">adjusted_lens!$D$2:$D$41</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">adjusted_lens!$G$1</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">adjusted_lens!$G$2:$G$41</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">wall_mounted_data!$B$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">wall_mounted_data!$B$2:$B$320</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">wall_mounted_data!$D$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">wall_mounted_data!$D$2:$D$320</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">wall_mounted_data!$D$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">wall_mounted_data!$D$2:$D$320</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">wall_mounted_data!$C$1</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">wall_mounted_data!$C$2:$C$320</definedName>
     <definedName name="_xlchart.v1.9" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1323" uniqueCount="23">
   <si>
     <t>first_peak</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>no-left</t>
+  </si>
+  <si>
+    <t>no-right</t>
   </si>
 </sst>
 </file>
@@ -677,10 +680,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -718,7 +721,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{24F89B28-D331-4BF4-97FC-98740A0DD325}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:f>_xlchart.v1.1</cx:f>
               <cx:v>first_peak</cx:v>
             </cx:txData>
           </cx:tx>
@@ -748,10 +751,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -789,7 +792,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{5A2C1765-A6AF-400C-A8FA-AC7260F1E1FC}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.1</cx:f>
+              <cx:f>_xlchart.v1.7</cx:f>
               <cx:v>second_peak</cx:v>
             </cx:txData>
           </cx:tx>
@@ -819,10 +822,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -860,7 +863,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{2E007EC1-CE09-47B1-A3E4-A95E48D1BADB}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.7</cx:f>
+              <cx:f>_xlchart.v1.4</cx:f>
               <cx:v>second_last_peak</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1076,10 +1079,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.21</cx:f>
+        <cx:f>_xlchart.v1.18</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.23</cx:f>
+        <cx:f>_xlchart.v1.20</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1117,7 +1120,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{F817657A-853F-485F-B1CA-8304AC66361E}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.22</cx:f>
+              <cx:f>_xlchart.v1.19</cx:f>
               <cx:v>Gradient_1</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1147,10 +1150,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.18</cx:f>
+        <cx:f>_xlchart.v1.21</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.20</cx:f>
+        <cx:f>_xlchart.v1.23</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1188,7 +1191,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{54F07B9F-F54F-47A3-8629-153198983661}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.19</cx:f>
+              <cx:f>_xlchart.v1.22</cx:f>
               <cx:v>Gradient_2</cx:v>
             </cx:txData>
           </cx:tx>
@@ -33195,10 +33198,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD048DA-A8F8-478B-A13B-D6B68CC50DBC}">
-  <dimension ref="A1:M87"/>
+  <dimension ref="A1:M101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="79" workbookViewId="0">
-      <selection activeCell="Q52" sqref="Q52"/>
+    <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:M101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36090,7 +36093,7 @@
         <v>1</v>
       </c>
       <c r="F71">
-        <v>0.158721120739927</v>
+        <v>0.15872112099999999</v>
       </c>
       <c r="G71">
         <v>-1</v>
@@ -36131,7 +36134,7 @@
         <v>1</v>
       </c>
       <c r="F72">
-        <v>0.18191552477610901</v>
+        <v>0.18191552499999999</v>
       </c>
       <c r="G72">
         <v>-1</v>
@@ -36172,7 +36175,7 @@
         <v>1</v>
       </c>
       <c r="F73">
-        <v>0.221341393060977</v>
+        <v>0.221341393</v>
       </c>
       <c r="G73">
         <v>-1</v>
@@ -36213,7 +36216,7 @@
         <v>1</v>
       </c>
       <c r="F74">
-        <v>0.30920677886792203</v>
+        <v>0.30920677899999999</v>
       </c>
       <c r="G74">
         <v>-1</v>
@@ -36254,7 +36257,7 @@
         <v>1</v>
       </c>
       <c r="F75">
-        <v>0.203403415957013</v>
+        <v>0.203403416</v>
       </c>
       <c r="G75">
         <v>-1</v>
@@ -36286,7 +36289,7 @@
         <v>0</v>
       </c>
       <c r="C76">
-        <v>0.21532896699901999</v>
+        <v>0.21532896700000001</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -36295,7 +36298,7 @@
         <v>0</v>
       </c>
       <c r="F76">
-        <v>3.1419546199545102E-2</v>
+        <v>3.1419546E-2</v>
       </c>
       <c r="G76">
         <v>0</v>
@@ -36327,7 +36330,7 @@
         <v>0</v>
       </c>
       <c r="C77">
-        <v>0.212519197992143</v>
+        <v>0.21251919799999999</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -36336,7 +36339,7 @@
         <v>0</v>
       </c>
       <c r="F77">
-        <v>2.7188608142129599E-2</v>
+        <v>2.7188608E-2</v>
       </c>
       <c r="G77">
         <v>0</v>
@@ -36368,7 +36371,7 @@
         <v>0</v>
       </c>
       <c r="C78">
-        <v>0.17616757542603301</v>
+        <v>0.17616757499999999</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -36377,7 +36380,7 @@
         <v>0</v>
       </c>
       <c r="F78">
-        <v>-2.9476204920928301E-2</v>
+        <v>-2.9476204999999998E-2</v>
       </c>
       <c r="G78">
         <v>0</v>
@@ -36418,7 +36421,7 @@
         <v>1</v>
       </c>
       <c r="F79">
-        <v>0.27074920381032702</v>
+        <v>0.27074920400000002</v>
       </c>
       <c r="G79">
         <v>-1</v>
@@ -36459,7 +36462,7 @@
         <v>1</v>
       </c>
       <c r="F80">
-        <v>0.19316557970539799</v>
+        <v>0.19316558</v>
       </c>
       <c r="G80">
         <v>-1</v>
@@ -36491,7 +36494,7 @@
         <v>0</v>
       </c>
       <c r="C81">
-        <v>0.227924418521499</v>
+        <v>0.22792441899999999</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -36500,7 +36503,7 @@
         <v>1</v>
       </c>
       <c r="F81">
-        <v>7.6425388355727999E-2</v>
+        <v>7.6425387999999997E-2</v>
       </c>
       <c r="G81">
         <v>0</v>
@@ -36532,7 +36535,7 @@
         <v>0</v>
       </c>
       <c r="C82">
-        <v>0.23953720237033799</v>
+        <v>0.239537202</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -36541,7 +36544,7 @@
         <v>0</v>
       </c>
       <c r="F82">
-        <v>6.0881167641786298E-2</v>
+        <v>6.0881167999999999E-2</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -36573,7 +36576,7 @@
         <v>0</v>
       </c>
       <c r="C83">
-        <v>0.17100803368352799</v>
+        <v>0.171008034</v>
       </c>
       <c r="D83">
         <v>0</v>
@@ -36582,7 +36585,7 @@
         <v>0</v>
       </c>
       <c r="F83">
-        <v>2.3708579110901899E-2</v>
+        <v>2.3708579E-2</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -36614,7 +36617,7 @@
         <v>0</v>
       </c>
       <c r="C84">
-        <v>0.136519980011619</v>
+        <v>0.13651998000000001</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -36623,7 +36626,7 @@
         <v>0</v>
       </c>
       <c r="F84">
-        <v>-3.3333439078020698E-4</v>
+        <v>-3.3333400000000002E-4</v>
       </c>
       <c r="G84">
         <v>0</v>
@@ -36664,7 +36667,7 @@
         <v>1</v>
       </c>
       <c r="F85">
-        <v>0.15508593156676101</v>
+        <v>0.15508593200000001</v>
       </c>
       <c r="G85">
         <v>-1</v>
@@ -36705,7 +36708,7 @@
         <v>1</v>
       </c>
       <c r="F86">
-        <v>0.20784857718908201</v>
+        <v>0.20784857700000001</v>
       </c>
       <c r="G86">
         <v>-1</v>
@@ -36737,7 +36740,7 @@
         <v>0</v>
       </c>
       <c r="C87">
-        <v>2.6639978819621799E-2</v>
+        <v>2.6639979000000001E-2</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -36746,7 +36749,7 @@
         <v>0</v>
       </c>
       <c r="F87">
-        <v>2.31697094891338E-2</v>
+        <v>2.3169709E-2</v>
       </c>
       <c r="G87">
         <v>0</v>
@@ -36768,6 +36771,580 @@
       </c>
       <c r="M87" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>0</v>
+      </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
+      <c r="C88">
+        <v>8.2672049950766796E-2</v>
+      </c>
+      <c r="D88">
+        <v>-1</v>
+      </c>
+      <c r="E88">
+        <v>-1</v>
+      </c>
+      <c r="F88">
+        <v>9999</v>
+      </c>
+      <c r="G88">
+        <v>1</v>
+      </c>
+      <c r="H88">
+        <v>-1</v>
+      </c>
+      <c r="I88">
+        <v>1</v>
+      </c>
+      <c r="J88">
+        <v>-1</v>
+      </c>
+      <c r="K88">
+        <v>0</v>
+      </c>
+      <c r="L88">
+        <v>0</v>
+      </c>
+      <c r="M88" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>0</v>
+      </c>
+      <c r="B89">
+        <v>0</v>
+      </c>
+      <c r="C89">
+        <v>4.5515432948655898E-2</v>
+      </c>
+      <c r="D89">
+        <v>-1</v>
+      </c>
+      <c r="E89">
+        <v>-1</v>
+      </c>
+      <c r="F89">
+        <v>9999</v>
+      </c>
+      <c r="G89">
+        <v>1</v>
+      </c>
+      <c r="H89">
+        <v>-1</v>
+      </c>
+      <c r="I89">
+        <v>1</v>
+      </c>
+      <c r="J89">
+        <v>-1</v>
+      </c>
+      <c r="K89">
+        <v>0</v>
+      </c>
+      <c r="L89">
+        <v>0</v>
+      </c>
+      <c r="M89" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>0</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+      <c r="C90">
+        <v>4.1364132182983099E-2</v>
+      </c>
+      <c r="D90">
+        <v>-1</v>
+      </c>
+      <c r="E90">
+        <v>-1</v>
+      </c>
+      <c r="F90">
+        <v>9999</v>
+      </c>
+      <c r="G90">
+        <v>1</v>
+      </c>
+      <c r="H90">
+        <v>-1</v>
+      </c>
+      <c r="I90">
+        <v>1</v>
+      </c>
+      <c r="J90">
+        <v>-1</v>
+      </c>
+      <c r="K90">
+        <v>0</v>
+      </c>
+      <c r="L90">
+        <v>0</v>
+      </c>
+      <c r="M90" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>0</v>
+      </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
+      <c r="C91">
+        <v>5.1255657984232199E-2</v>
+      </c>
+      <c r="D91">
+        <v>1</v>
+      </c>
+      <c r="E91">
+        <v>1</v>
+      </c>
+      <c r="F91">
+        <v>5.4635583596662901E-2</v>
+      </c>
+      <c r="G91">
+        <v>1</v>
+      </c>
+      <c r="H91">
+        <v>0</v>
+      </c>
+      <c r="I91">
+        <v>1</v>
+      </c>
+      <c r="J91">
+        <v>0</v>
+      </c>
+      <c r="K91">
+        <v>1</v>
+      </c>
+      <c r="L91">
+        <v>0</v>
+      </c>
+      <c r="M91" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>0</v>
+      </c>
+      <c r="B92">
+        <v>1</v>
+      </c>
+      <c r="C92">
+        <v>-6.6458714224118795E-2</v>
+      </c>
+      <c r="D92">
+        <v>1</v>
+      </c>
+      <c r="E92">
+        <v>1</v>
+      </c>
+      <c r="F92">
+        <v>5.1641319988196301E-2</v>
+      </c>
+      <c r="G92">
+        <v>1</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
+      <c r="I92">
+        <v>0</v>
+      </c>
+      <c r="J92">
+        <v>0</v>
+      </c>
+      <c r="K92">
+        <v>1</v>
+      </c>
+      <c r="L92">
+        <v>0</v>
+      </c>
+      <c r="M92" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>0</v>
+      </c>
+      <c r="B93">
+        <v>1</v>
+      </c>
+      <c r="C93">
+        <v>-0.105687110478037</v>
+      </c>
+      <c r="D93">
+        <v>1</v>
+      </c>
+      <c r="E93">
+        <v>1</v>
+      </c>
+      <c r="F93">
+        <v>-1.6643453998222899E-2</v>
+      </c>
+      <c r="G93">
+        <v>1</v>
+      </c>
+      <c r="H93">
+        <v>0</v>
+      </c>
+      <c r="I93">
+        <v>0</v>
+      </c>
+      <c r="J93">
+        <v>0</v>
+      </c>
+      <c r="K93">
+        <v>1</v>
+      </c>
+      <c r="L93">
+        <v>0</v>
+      </c>
+      <c r="M93" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>0</v>
+      </c>
+      <c r="B94">
+        <v>1</v>
+      </c>
+      <c r="C94">
+        <v>-8.6765498850936096E-2</v>
+      </c>
+      <c r="D94">
+        <v>1</v>
+      </c>
+      <c r="E94">
+        <v>1</v>
+      </c>
+      <c r="F94">
+        <v>-1.6101218840755199E-2</v>
+      </c>
+      <c r="G94">
+        <v>1</v>
+      </c>
+      <c r="H94">
+        <v>0</v>
+      </c>
+      <c r="I94">
+        <v>0</v>
+      </c>
+      <c r="J94">
+        <v>0</v>
+      </c>
+      <c r="K94">
+        <v>1</v>
+      </c>
+      <c r="L94">
+        <v>0</v>
+      </c>
+      <c r="M94" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>0</v>
+      </c>
+      <c r="B95">
+        <v>1</v>
+      </c>
+      <c r="C95">
+        <v>-7.7654471799725996E-2</v>
+      </c>
+      <c r="D95">
+        <v>1</v>
+      </c>
+      <c r="E95">
+        <v>1</v>
+      </c>
+      <c r="F95">
+        <v>-1.1960002043694301E-2</v>
+      </c>
+      <c r="G95">
+        <v>1</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95">
+        <v>0</v>
+      </c>
+      <c r="J95">
+        <v>0</v>
+      </c>
+      <c r="K95">
+        <v>1</v>
+      </c>
+      <c r="L95">
+        <v>0</v>
+      </c>
+      <c r="M95" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>0</v>
+      </c>
+      <c r="B96">
+        <v>1</v>
+      </c>
+      <c r="C96">
+        <v>-0.11111810813152501</v>
+      </c>
+      <c r="D96">
+        <v>1</v>
+      </c>
+      <c r="E96">
+        <v>1</v>
+      </c>
+      <c r="F96">
+        <v>-1.1786787797992001E-2</v>
+      </c>
+      <c r="G96">
+        <v>1</v>
+      </c>
+      <c r="H96">
+        <v>0</v>
+      </c>
+      <c r="I96">
+        <v>0</v>
+      </c>
+      <c r="J96">
+        <v>0</v>
+      </c>
+      <c r="K96">
+        <v>1</v>
+      </c>
+      <c r="L96">
+        <v>0</v>
+      </c>
+      <c r="M96" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>0</v>
+      </c>
+      <c r="B97">
+        <v>1</v>
+      </c>
+      <c r="C97">
+        <v>-6.2132519105072302E-2</v>
+      </c>
+      <c r="D97">
+        <v>1</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97">
+        <v>-0.163323180890215</v>
+      </c>
+      <c r="G97">
+        <v>1</v>
+      </c>
+      <c r="H97">
+        <v>0</v>
+      </c>
+      <c r="I97">
+        <v>0</v>
+      </c>
+      <c r="J97">
+        <v>1</v>
+      </c>
+      <c r="K97">
+        <v>1</v>
+      </c>
+      <c r="L97">
+        <v>0</v>
+      </c>
+      <c r="M97" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>0</v>
+      </c>
+      <c r="B98">
+        <v>1</v>
+      </c>
+      <c r="C98">
+        <v>-8.0074348628915798E-2</v>
+      </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
+      <c r="E98">
+        <v>1</v>
+      </c>
+      <c r="F98">
+        <v>-2.44013273901998E-2</v>
+      </c>
+      <c r="G98">
+        <v>1</v>
+      </c>
+      <c r="H98">
+        <v>0</v>
+      </c>
+      <c r="I98">
+        <v>0</v>
+      </c>
+      <c r="J98">
+        <v>0</v>
+      </c>
+      <c r="K98">
+        <v>1</v>
+      </c>
+      <c r="L98">
+        <v>0</v>
+      </c>
+      <c r="M98" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>0</v>
+      </c>
+      <c r="B99">
+        <v>1</v>
+      </c>
+      <c r="C99">
+        <v>-8.5107871740544405E-2</v>
+      </c>
+      <c r="D99">
+        <v>1</v>
+      </c>
+      <c r="E99">
+        <v>1</v>
+      </c>
+      <c r="F99">
+        <v>-1.1141381518335301E-2</v>
+      </c>
+      <c r="G99">
+        <v>1</v>
+      </c>
+      <c r="H99">
+        <v>0</v>
+      </c>
+      <c r="I99">
+        <v>0</v>
+      </c>
+      <c r="J99">
+        <v>0</v>
+      </c>
+      <c r="K99">
+        <v>1</v>
+      </c>
+      <c r="L99">
+        <v>0</v>
+      </c>
+      <c r="M99" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>0</v>
+      </c>
+      <c r="B100">
+        <v>1</v>
+      </c>
+      <c r="C100">
+        <v>-8.6319377561982394E-2</v>
+      </c>
+      <c r="D100">
+        <v>1</v>
+      </c>
+      <c r="E100">
+        <v>1</v>
+      </c>
+      <c r="F100">
+        <v>-3.5547655473810801E-2</v>
+      </c>
+      <c r="G100">
+        <v>1</v>
+      </c>
+      <c r="H100">
+        <v>0</v>
+      </c>
+      <c r="I100">
+        <v>0</v>
+      </c>
+      <c r="J100">
+        <v>0</v>
+      </c>
+      <c r="K100">
+        <v>1</v>
+      </c>
+      <c r="L100">
+        <v>0</v>
+      </c>
+      <c r="M100" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>0</v>
+      </c>
+      <c r="B101">
+        <v>1</v>
+      </c>
+      <c r="C101">
+        <v>-6.8487588433220406E-2</v>
+      </c>
+      <c r="D101">
+        <v>1</v>
+      </c>
+      <c r="E101">
+        <v>1</v>
+      </c>
+      <c r="F101">
+        <v>-2.1448924428295699E-2</v>
+      </c>
+      <c r="G101">
+        <v>1</v>
+      </c>
+      <c r="H101">
+        <v>0</v>
+      </c>
+      <c r="I101">
+        <v>0</v>
+      </c>
+      <c r="J101">
+        <v>0</v>
+      </c>
+      <c r="K101">
+        <v>1</v>
+      </c>
+      <c r="L101">
+        <v>0</v>
+      </c>
+      <c r="M101" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made changes to mdoel data
</commit_message>
<xml_diff>
--- a/decision_data_new.xlsx
+++ b/decision_data_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/paul_kumar_mail_utoronto_ca/Documents/engineering_masters/thesis work/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="231" documentId="6_{F6B86153-F216-4926-93F2-3946DCDAA96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E11D7730-4475-4408-B43F-FD2D63EDE5D1}"/>
+  <xr:revisionPtr revIDLastSave="245" documentId="6_{F6B86153-F216-4926-93F2-3946DCDAA96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{860CA718-7AB1-4B1B-9CA4-70B0C8037C43}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,28 +24,28 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">wall_binary_2!$F$1:$F$182</definedName>
     <definedName name="_xlchart.v1.0" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">wall_mounted_data!$B$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">wall_mounted_data!$E$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">wall_mounted_data!$E$2:$E$320</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">wall_mounted_data!$F$1</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">wall_mounted_data!$B$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">wall_mounted_data!$B$2:$B$320</definedName>
     <definedName name="_xlchart.v1.12" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">wall_mounted_data!$F$1</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">wall_mounted_data!$F$2:$F$320</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">wall_mounted_data!$E$1</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">wall_mounted_data!$E$2:$E$320</definedName>
     <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$A$2:$A$150</definedName>
     <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$B$1</definedName>
     <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$B$2:$B$150</definedName>
     <definedName name="_xlchart.v1.18" hidden="1">adjusted_lens!$A$2:$A$41</definedName>
     <definedName name="_xlchart.v1.19" hidden="1">adjusted_lens!$D$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">wall_mounted_data!$B$2:$B$320</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">wall_mounted_data!$F$2:$F$320</definedName>
     <definedName name="_xlchart.v1.20" hidden="1">adjusted_lens!$D$2:$D$41</definedName>
     <definedName name="_xlchart.v1.21" hidden="1">adjusted_lens!$A$2:$A$41</definedName>
     <definedName name="_xlchart.v1.22" hidden="1">adjusted_lens!$G$1</definedName>
     <definedName name="_xlchart.v1.23" hidden="1">adjusted_lens!$G$2:$G$41</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">wall_mounted_data!$D$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">wall_mounted_data!$D$2:$D$320</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">wall_mounted_data!$C$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">wall_mounted_data!$C$2:$C$320</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">wall_mounted_data!$C$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">wall_mounted_data!$C$2:$C$320</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">wall_mounted_data!$D$1</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">wall_mounted_data!$D$2:$D$320</definedName>
     <definedName name="_xlchart.v1.9" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1323" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1340" uniqueCount="23">
   <si>
     <t>first_peak</t>
   </si>
@@ -680,10 +680,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -721,7 +721,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{24F89B28-D331-4BF4-97FC-98740A0DD325}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.1</cx:f>
+              <cx:f>_xlchart.v1.10</cx:f>
               <cx:v>first_peak</cx:v>
             </cx:txData>
           </cx:tx>
@@ -751,10 +751,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -792,7 +792,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{5A2C1765-A6AF-400C-A8FA-AC7260F1E1FC}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.7</cx:f>
+              <cx:f>_xlchart.v1.4</cx:f>
               <cx:v>second_peak</cx:v>
             </cx:txData>
           </cx:tx>
@@ -822,10 +822,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -863,7 +863,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{2E007EC1-CE09-47B1-A3E4-A95E48D1BADB}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:f>_xlchart.v1.7</cx:f>
               <cx:v>second_last_peak</cx:v>
             </cx:txData>
           </cx:tx>
@@ -893,10 +893,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.12</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.11</cx:f>
+        <cx:f>_xlchart.v1.14</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -934,7 +934,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{28AFBDCB-EA5A-4D8B-B5F8-DF1924715131}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.10</cx:f>
+              <cx:f>_xlchart.v1.13</cx:f>
               <cx:v>last_peak</cx:v>
             </cx:txData>
           </cx:tx>
@@ -964,10 +964,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.12</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.14</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1005,7 +1005,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{02F72712-9CA3-4436-A6ED-93C80B1901DF}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.13</cx:f>
+              <cx:f>_xlchart.v1.1</cx:f>
               <cx:v>Gradient_1</cx:v>
             </cx:txData>
           </cx:tx>
@@ -33198,10 +33198,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD048DA-A8F8-478B-A13B-D6B68CC50DBC}">
-  <dimension ref="A1:M101"/>
+  <dimension ref="A1:M118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:M101"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="79" workbookViewId="0">
+      <selection activeCell="M2" sqref="A1:M118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36781,7 +36781,7 @@
         <v>0</v>
       </c>
       <c r="C88">
-        <v>8.2672049950766796E-2</v>
+        <v>8.2672049999999997E-2</v>
       </c>
       <c r="D88">
         <v>-1</v>
@@ -36822,7 +36822,7 @@
         <v>0</v>
       </c>
       <c r="C89">
-        <v>4.5515432948655898E-2</v>
+        <v>4.5515433000000001E-2</v>
       </c>
       <c r="D89">
         <v>-1</v>
@@ -36863,7 +36863,7 @@
         <v>0</v>
       </c>
       <c r="C90">
-        <v>4.1364132182983099E-2</v>
+        <v>4.1364131999999998E-2</v>
       </c>
       <c r="D90">
         <v>-1</v>
@@ -36904,7 +36904,7 @@
         <v>0</v>
       </c>
       <c r="C91">
-        <v>5.1255657984232199E-2</v>
+        <v>5.1255658000000003E-2</v>
       </c>
       <c r="D91">
         <v>1</v>
@@ -36913,7 +36913,7 @@
         <v>1</v>
       </c>
       <c r="F91">
-        <v>5.4635583596662901E-2</v>
+        <v>5.4635584000000001E-2</v>
       </c>
       <c r="G91">
         <v>1</v>
@@ -36945,7 +36945,7 @@
         <v>1</v>
       </c>
       <c r="C92">
-        <v>-6.6458714224118795E-2</v>
+        <v>-6.6458714000000002E-2</v>
       </c>
       <c r="D92">
         <v>1</v>
@@ -36954,7 +36954,7 @@
         <v>1</v>
       </c>
       <c r="F92">
-        <v>5.1641319988196301E-2</v>
+        <v>5.1641319999999998E-2</v>
       </c>
       <c r="G92">
         <v>1</v>
@@ -36986,7 +36986,7 @@
         <v>1</v>
       </c>
       <c r="C93">
-        <v>-0.105687110478037</v>
+        <v>-0.10568711</v>
       </c>
       <c r="D93">
         <v>1</v>
@@ -36995,7 +36995,7 @@
         <v>1</v>
       </c>
       <c r="F93">
-        <v>-1.6643453998222899E-2</v>
+        <v>-1.6643453999999998E-2</v>
       </c>
       <c r="G93">
         <v>1</v>
@@ -37027,7 +37027,7 @@
         <v>1</v>
       </c>
       <c r="C94">
-        <v>-8.6765498850936096E-2</v>
+        <v>-8.6765498999999996E-2</v>
       </c>
       <c r="D94">
         <v>1</v>
@@ -37036,7 +37036,7 @@
         <v>1</v>
       </c>
       <c r="F94">
-        <v>-1.6101218840755199E-2</v>
+        <v>-1.6101219E-2</v>
       </c>
       <c r="G94">
         <v>1</v>
@@ -37068,7 +37068,7 @@
         <v>1</v>
       </c>
       <c r="C95">
-        <v>-7.7654471799725996E-2</v>
+        <v>-7.7654472000000002E-2</v>
       </c>
       <c r="D95">
         <v>1</v>
@@ -37077,7 +37077,7 @@
         <v>1</v>
       </c>
       <c r="F95">
-        <v>-1.1960002043694301E-2</v>
+        <v>-1.1960002000000001E-2</v>
       </c>
       <c r="G95">
         <v>1</v>
@@ -37109,7 +37109,7 @@
         <v>1</v>
       </c>
       <c r="C96">
-        <v>-0.11111810813152501</v>
+        <v>-0.11111810799999999</v>
       </c>
       <c r="D96">
         <v>1</v>
@@ -37118,7 +37118,7 @@
         <v>1</v>
       </c>
       <c r="F96">
-        <v>-1.1786787797992001E-2</v>
+        <v>-1.1786787999999999E-2</v>
       </c>
       <c r="G96">
         <v>1</v>
@@ -37150,7 +37150,7 @@
         <v>1</v>
       </c>
       <c r="C97">
-        <v>-6.2132519105072302E-2</v>
+        <v>-6.2132518999999997E-2</v>
       </c>
       <c r="D97">
         <v>1</v>
@@ -37159,7 +37159,7 @@
         <v>0</v>
       </c>
       <c r="F97">
-        <v>-0.163323180890215</v>
+        <v>-0.16332318100000001</v>
       </c>
       <c r="G97">
         <v>1</v>
@@ -37191,7 +37191,7 @@
         <v>1</v>
       </c>
       <c r="C98">
-        <v>-8.0074348628915798E-2</v>
+        <v>-8.0074349000000003E-2</v>
       </c>
       <c r="D98">
         <v>1</v>
@@ -37200,7 +37200,7 @@
         <v>1</v>
       </c>
       <c r="F98">
-        <v>-2.44013273901998E-2</v>
+        <v>-2.4401327E-2</v>
       </c>
       <c r="G98">
         <v>1</v>
@@ -37232,7 +37232,7 @@
         <v>1</v>
       </c>
       <c r="C99">
-        <v>-8.5107871740544405E-2</v>
+        <v>-8.5107872000000001E-2</v>
       </c>
       <c r="D99">
         <v>1</v>
@@ -37241,7 +37241,7 @@
         <v>1</v>
       </c>
       <c r="F99">
-        <v>-1.1141381518335301E-2</v>
+        <v>-1.1141382E-2</v>
       </c>
       <c r="G99">
         <v>1</v>
@@ -37273,7 +37273,7 @@
         <v>1</v>
       </c>
       <c r="C100">
-        <v>-8.6319377561982394E-2</v>
+        <v>-8.6319378000000002E-2</v>
       </c>
       <c r="D100">
         <v>1</v>
@@ -37282,7 +37282,7 @@
         <v>1</v>
       </c>
       <c r="F100">
-        <v>-3.5547655473810801E-2</v>
+        <v>-3.5547654999999997E-2</v>
       </c>
       <c r="G100">
         <v>1</v>
@@ -37314,7 +37314,7 @@
         <v>1</v>
       </c>
       <c r="C101">
-        <v>-6.8487588433220406E-2</v>
+        <v>-6.8487588000000002E-2</v>
       </c>
       <c r="D101">
         <v>1</v>
@@ -37323,7 +37323,7 @@
         <v>1</v>
       </c>
       <c r="F101">
-        <v>-2.1448924428295699E-2</v>
+        <v>-2.1448924000000001E-2</v>
       </c>
       <c r="G101">
         <v>1</v>
@@ -37345,6 +37345,703 @@
       </c>
       <c r="M101" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>0</v>
+      </c>
+      <c r="B102">
+        <v>1</v>
+      </c>
+      <c r="C102">
+        <v>6.5519599999999999E-3</v>
+      </c>
+      <c r="D102">
+        <v>-1</v>
+      </c>
+      <c r="E102">
+        <v>-1</v>
+      </c>
+      <c r="F102">
+        <v>9999</v>
+      </c>
+      <c r="G102">
+        <v>1</v>
+      </c>
+      <c r="H102">
+        <v>-1</v>
+      </c>
+      <c r="I102">
+        <v>0</v>
+      </c>
+      <c r="J102">
+        <v>-1</v>
+      </c>
+      <c r="K102">
+        <v>0</v>
+      </c>
+      <c r="L102">
+        <v>0</v>
+      </c>
+      <c r="M102" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>1</v>
+      </c>
+      <c r="B103">
+        <v>1</v>
+      </c>
+      <c r="C103">
+        <v>-1.2027858000000001E-2</v>
+      </c>
+      <c r="D103">
+        <v>-1</v>
+      </c>
+      <c r="E103">
+        <v>-1</v>
+      </c>
+      <c r="F103">
+        <v>9999</v>
+      </c>
+      <c r="G103">
+        <v>0</v>
+      </c>
+      <c r="H103">
+        <v>-1</v>
+      </c>
+      <c r="I103">
+        <v>0</v>
+      </c>
+      <c r="J103">
+        <v>-1</v>
+      </c>
+      <c r="K103">
+        <v>0</v>
+      </c>
+      <c r="L103">
+        <v>0</v>
+      </c>
+      <c r="M103" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>1</v>
+      </c>
+      <c r="B104">
+        <v>1</v>
+      </c>
+      <c r="C104">
+        <v>-1.7014052000000002E-2</v>
+      </c>
+      <c r="D104">
+        <v>-1</v>
+      </c>
+      <c r="E104">
+        <v>-1</v>
+      </c>
+      <c r="F104">
+        <v>9999</v>
+      </c>
+      <c r="G104">
+        <v>0</v>
+      </c>
+      <c r="H104">
+        <v>-1</v>
+      </c>
+      <c r="I104">
+        <v>0</v>
+      </c>
+      <c r="J104">
+        <v>-1</v>
+      </c>
+      <c r="K104">
+        <v>0</v>
+      </c>
+      <c r="L104">
+        <v>0</v>
+      </c>
+      <c r="M104" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>0</v>
+      </c>
+      <c r="B105">
+        <v>1</v>
+      </c>
+      <c r="C105">
+        <v>-0.17338121500000001</v>
+      </c>
+      <c r="D105">
+        <v>-1</v>
+      </c>
+      <c r="E105">
+        <v>-1</v>
+      </c>
+      <c r="F105">
+        <v>9999</v>
+      </c>
+      <c r="G105">
+        <v>1</v>
+      </c>
+      <c r="H105">
+        <v>-1</v>
+      </c>
+      <c r="I105">
+        <v>0</v>
+      </c>
+      <c r="J105">
+        <v>-1</v>
+      </c>
+      <c r="K105">
+        <v>0</v>
+      </c>
+      <c r="L105">
+        <v>0</v>
+      </c>
+      <c r="M105" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>0</v>
+      </c>
+      <c r="B106">
+        <v>0</v>
+      </c>
+      <c r="C106">
+        <v>-2.7724113000000002E-2</v>
+      </c>
+      <c r="D106">
+        <v>-1</v>
+      </c>
+      <c r="E106">
+        <v>-1</v>
+      </c>
+      <c r="F106">
+        <v>9999</v>
+      </c>
+      <c r="G106">
+        <v>1</v>
+      </c>
+      <c r="H106">
+        <v>-1</v>
+      </c>
+      <c r="I106">
+        <v>1</v>
+      </c>
+      <c r="J106">
+        <v>-1</v>
+      </c>
+      <c r="K106">
+        <v>0</v>
+      </c>
+      <c r="L106">
+        <v>0</v>
+      </c>
+      <c r="M106" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>0</v>
+      </c>
+      <c r="B107">
+        <v>1</v>
+      </c>
+      <c r="C107">
+        <v>-0.12497230300000001</v>
+      </c>
+      <c r="D107">
+        <v>-1</v>
+      </c>
+      <c r="E107">
+        <v>-1</v>
+      </c>
+      <c r="F107">
+        <v>9999</v>
+      </c>
+      <c r="G107">
+        <v>1</v>
+      </c>
+      <c r="H107">
+        <v>-1</v>
+      </c>
+      <c r="I107">
+        <v>0</v>
+      </c>
+      <c r="J107">
+        <v>-1</v>
+      </c>
+      <c r="K107">
+        <v>0</v>
+      </c>
+      <c r="L107">
+        <v>0</v>
+      </c>
+      <c r="M107" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>0</v>
+      </c>
+      <c r="B108">
+        <v>0</v>
+      </c>
+      <c r="C108">
+        <v>-3.7983230000000002E-3</v>
+      </c>
+      <c r="D108">
+        <v>-1</v>
+      </c>
+      <c r="E108">
+        <v>-1</v>
+      </c>
+      <c r="F108">
+        <v>9999</v>
+      </c>
+      <c r="G108">
+        <v>1</v>
+      </c>
+      <c r="H108">
+        <v>-1</v>
+      </c>
+      <c r="I108">
+        <v>1</v>
+      </c>
+      <c r="J108">
+        <v>-1</v>
+      </c>
+      <c r="K108">
+        <v>0</v>
+      </c>
+      <c r="L108">
+        <v>0</v>
+      </c>
+      <c r="M108" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>0</v>
+      </c>
+      <c r="B109">
+        <v>1</v>
+      </c>
+      <c r="C109">
+        <v>-1.5624499E-2</v>
+      </c>
+      <c r="D109">
+        <v>-1</v>
+      </c>
+      <c r="E109">
+        <v>-1</v>
+      </c>
+      <c r="F109">
+        <v>9999</v>
+      </c>
+      <c r="G109">
+        <v>1</v>
+      </c>
+      <c r="H109">
+        <v>-1</v>
+      </c>
+      <c r="I109">
+        <v>0</v>
+      </c>
+      <c r="J109">
+        <v>-1</v>
+      </c>
+      <c r="K109">
+        <v>0</v>
+      </c>
+      <c r="L109">
+        <v>0</v>
+      </c>
+      <c r="M109" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>0</v>
+      </c>
+      <c r="B110">
+        <v>0</v>
+      </c>
+      <c r="C110">
+        <v>3.3601687999999998E-2</v>
+      </c>
+      <c r="D110">
+        <v>-1</v>
+      </c>
+      <c r="E110">
+        <v>-1</v>
+      </c>
+      <c r="F110">
+        <v>9999</v>
+      </c>
+      <c r="G110">
+        <v>1</v>
+      </c>
+      <c r="H110">
+        <v>-1</v>
+      </c>
+      <c r="I110">
+        <v>1</v>
+      </c>
+      <c r="J110">
+        <v>-1</v>
+      </c>
+      <c r="K110">
+        <v>0</v>
+      </c>
+      <c r="L110">
+        <v>0</v>
+      </c>
+      <c r="M110" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>1</v>
+      </c>
+      <c r="B111">
+        <v>1</v>
+      </c>
+      <c r="C111">
+        <v>9.6192959999999994E-3</v>
+      </c>
+      <c r="D111">
+        <v>-1</v>
+      </c>
+      <c r="E111">
+        <v>-1</v>
+      </c>
+      <c r="F111">
+        <v>9999</v>
+      </c>
+      <c r="G111">
+        <v>0</v>
+      </c>
+      <c r="H111">
+        <v>-1</v>
+      </c>
+      <c r="I111">
+        <v>0</v>
+      </c>
+      <c r="J111">
+        <v>-1</v>
+      </c>
+      <c r="K111">
+        <v>0</v>
+      </c>
+      <c r="L111">
+        <v>0</v>
+      </c>
+      <c r="M111" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>0</v>
+      </c>
+      <c r="B112">
+        <v>1</v>
+      </c>
+      <c r="C112">
+        <v>-0.119221941</v>
+      </c>
+      <c r="D112">
+        <v>-1</v>
+      </c>
+      <c r="E112">
+        <v>-1</v>
+      </c>
+      <c r="F112">
+        <v>9999</v>
+      </c>
+      <c r="G112">
+        <v>1</v>
+      </c>
+      <c r="H112">
+        <v>-1</v>
+      </c>
+      <c r="I112">
+        <v>0</v>
+      </c>
+      <c r="J112">
+        <v>-1</v>
+      </c>
+      <c r="K112">
+        <v>0</v>
+      </c>
+      <c r="L112">
+        <v>0</v>
+      </c>
+      <c r="M112" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>0</v>
+      </c>
+      <c r="B113">
+        <v>0</v>
+      </c>
+      <c r="C113">
+        <v>0.12401332800000001</v>
+      </c>
+      <c r="D113">
+        <v>-1</v>
+      </c>
+      <c r="E113">
+        <v>-1</v>
+      </c>
+      <c r="F113">
+        <v>9999</v>
+      </c>
+      <c r="G113">
+        <v>1</v>
+      </c>
+      <c r="H113">
+        <v>-1</v>
+      </c>
+      <c r="I113">
+        <v>1</v>
+      </c>
+      <c r="J113">
+        <v>-1</v>
+      </c>
+      <c r="K113">
+        <v>0</v>
+      </c>
+      <c r="L113">
+        <v>0</v>
+      </c>
+      <c r="M113" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>1</v>
+      </c>
+      <c r="B114">
+        <v>1</v>
+      </c>
+      <c r="C114">
+        <v>9.0124937000000002E-2</v>
+      </c>
+      <c r="D114">
+        <v>-1</v>
+      </c>
+      <c r="E114">
+        <v>-1</v>
+      </c>
+      <c r="F114">
+        <v>9999</v>
+      </c>
+      <c r="G114">
+        <v>0</v>
+      </c>
+      <c r="H114">
+        <v>-1</v>
+      </c>
+      <c r="I114">
+        <v>0</v>
+      </c>
+      <c r="J114">
+        <v>-1</v>
+      </c>
+      <c r="K114">
+        <v>0</v>
+      </c>
+      <c r="L114">
+        <v>0</v>
+      </c>
+      <c r="M114" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>1</v>
+      </c>
+      <c r="B115">
+        <v>0</v>
+      </c>
+      <c r="C115">
+        <v>0.23252844975381701</v>
+      </c>
+      <c r="D115">
+        <v>0</v>
+      </c>
+      <c r="E115">
+        <v>1</v>
+      </c>
+      <c r="F115">
+        <v>0.36134678258824099</v>
+      </c>
+      <c r="G115">
+        <v>0</v>
+      </c>
+      <c r="H115">
+        <v>1</v>
+      </c>
+      <c r="I115">
+        <v>1</v>
+      </c>
+      <c r="J115">
+        <v>0</v>
+      </c>
+      <c r="K115">
+        <v>0</v>
+      </c>
+      <c r="L115">
+        <v>0</v>
+      </c>
+      <c r="M115" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>1</v>
+      </c>
+      <c r="B116">
+        <v>0</v>
+      </c>
+      <c r="C116">
+        <v>0.222120029249608</v>
+      </c>
+      <c r="D116">
+        <v>1</v>
+      </c>
+      <c r="E116">
+        <v>0</v>
+      </c>
+      <c r="F116">
+        <v>-0.27754046153136902</v>
+      </c>
+      <c r="G116">
+        <v>0</v>
+      </c>
+      <c r="H116">
+        <v>0</v>
+      </c>
+      <c r="I116">
+        <v>1</v>
+      </c>
+      <c r="J116">
+        <v>1</v>
+      </c>
+      <c r="K116">
+        <v>1</v>
+      </c>
+      <c r="L116">
+        <v>1</v>
+      </c>
+      <c r="M116" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>1</v>
+      </c>
+      <c r="B117">
+        <v>0</v>
+      </c>
+      <c r="C117">
+        <v>0.16193442831632299</v>
+      </c>
+      <c r="D117">
+        <v>0</v>
+      </c>
+      <c r="E117">
+        <v>1</v>
+      </c>
+      <c r="F117">
+        <v>0.35515758118115398</v>
+      </c>
+      <c r="G117">
+        <v>0</v>
+      </c>
+      <c r="H117">
+        <v>1</v>
+      </c>
+      <c r="I117">
+        <v>1</v>
+      </c>
+      <c r="J117">
+        <v>0</v>
+      </c>
+      <c r="K117">
+        <v>0</v>
+      </c>
+      <c r="L117">
+        <v>0</v>
+      </c>
+      <c r="M117" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>1</v>
+      </c>
+      <c r="B118">
+        <v>0</v>
+      </c>
+      <c r="C118">
+        <v>0.204694473401068</v>
+      </c>
+      <c r="D118">
+        <v>1</v>
+      </c>
+      <c r="E118">
+        <v>0</v>
+      </c>
+      <c r="F118">
+        <v>-0.27399005592427</v>
+      </c>
+      <c r="G118">
+        <v>0</v>
+      </c>
+      <c r="H118">
+        <v>0</v>
+      </c>
+      <c r="I118">
+        <v>1</v>
+      </c>
+      <c r="J118">
+        <v>1</v>
+      </c>
+      <c r="K118">
+        <v>1</v>
+      </c>
+      <c r="L118">
+        <v>1</v>
+      </c>
+      <c r="M118" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
committing new decision datas
</commit_message>
<xml_diff>
--- a/decision_data_new.xlsx
+++ b/decision_data_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/paul_kumar_mail_utoronto_ca/Documents/engineering_masters/thesis work/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="253" documentId="6_{F6B86153-F216-4926-93F2-3946DCDAA96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{02CE9511-7CED-4CCB-BC74-10470BCACD1F}"/>
+  <xr:revisionPtr revIDLastSave="258" documentId="6_{F6B86153-F216-4926-93F2-3946DCDAA96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{84E30572-575A-4611-8994-8AB72DAABD02}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wall_mounted_data" sheetId="12" r:id="rId1"/>
@@ -25,22 +25,22 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">wall_binary_2!$F$1:$F$182</definedName>
     <definedName name="_xlchart.v1.0" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">wall_mounted_data!$E$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">wall_mounted_data!$B$1</definedName>
     <definedName name="_xlchart.v1.10" hidden="1">wall_mounted_data!$D$1</definedName>
     <definedName name="_xlchart.v1.11" hidden="1">wall_mounted_data!$D$2:$D$320</definedName>
     <definedName name="_xlchart.v1.12" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">wall_mounted_data!$B$1</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">wall_mounted_data!$B$2:$B$320</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">wall_mounted_data!$E$1</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">wall_mounted_data!$E$2:$E$320</definedName>
     <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$A$2:$A$150</definedName>
     <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$B$1</definedName>
     <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$B$2:$B$150</definedName>
     <definedName name="_xlchart.v1.18" hidden="1">adjusted_lens!$A$2:$A$41</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">adjusted_lens!$D$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">wall_mounted_data!$E$2:$E$320</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">adjusted_lens!$D$2:$D$41</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">adjusted_lens!$G$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">wall_mounted_data!$B$2:$B$320</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">adjusted_lens!$G$2:$G$41</definedName>
     <definedName name="_xlchart.v1.21" hidden="1">adjusted_lens!$A$2:$A$41</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">adjusted_lens!$G$1</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">adjusted_lens!$G$2:$G$41</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">adjusted_lens!$D$1</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">adjusted_lens!$D$2:$D$41</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">wall_mounted_data!$A$2:$A$320</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">wall_mounted_data!$F$1</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">wall_mounted_data!$F$2:$F$320</definedName>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1541" uniqueCount="24">
   <si>
     <t>first_peak</t>
   </si>
@@ -684,10 +684,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.12</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.14</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -725,7 +725,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{24F89B28-D331-4BF4-97FC-98740A0DD325}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.13</cx:f>
+              <cx:f>_xlchart.v1.1</cx:f>
               <cx:v>first_peak</cx:v>
             </cx:txData>
           </cx:tx>
@@ -897,10 +897,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.12</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.14</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -938,7 +938,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{28AFBDCB-EA5A-4D8B-B5F8-DF1924715131}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.1</cx:f>
+              <cx:f>_xlchart.v1.13</cx:f>
               <cx:v>last_peak</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1083,10 +1083,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.18</cx:f>
+        <cx:f>_xlchart.v1.21</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.20</cx:f>
+        <cx:f>_xlchart.v1.23</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1124,7 +1124,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{F817657A-853F-485F-B1CA-8304AC66361E}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.19</cx:f>
+              <cx:f>_xlchart.v1.22</cx:f>
               <cx:v>Gradient_1</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1154,10 +1154,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.21</cx:f>
+        <cx:f>_xlchart.v1.18</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.23</cx:f>
+        <cx:f>_xlchart.v1.20</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1195,7 +1195,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{54F07B9F-F54F-47A3-8629-153198983661}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.22</cx:f>
+              <cx:f>_xlchart.v1.19</cx:f>
               <cx:v>Gradient_2</cx:v>
             </cx:txData>
           </cx:tx>
@@ -33202,10 +33202,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD048DA-A8F8-478B-A13B-D6B68CC50DBC}">
-  <dimension ref="A1:M130"/>
+  <dimension ref="A1:M157"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView zoomScale="79" workbookViewId="0">
+      <selection activeCell="M1" activeCellId="5" sqref="C1:C1048576 F1:F1048576 G1:G1048576 K1:K1048576 L1:L1048576 M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38543,6 +38543,1113 @@
         <v>21</v>
       </c>
     </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>1</v>
+      </c>
+      <c r="B131">
+        <v>1</v>
+      </c>
+      <c r="C131">
+        <v>-2.3021396615663402E-2</v>
+      </c>
+      <c r="D131">
+        <v>1</v>
+      </c>
+      <c r="E131">
+        <v>0</v>
+      </c>
+      <c r="F131">
+        <v>-0.14308251083017601</v>
+      </c>
+      <c r="G131">
+        <v>0</v>
+      </c>
+      <c r="H131">
+        <v>0</v>
+      </c>
+      <c r="I131">
+        <v>0</v>
+      </c>
+      <c r="J131">
+        <v>1</v>
+      </c>
+      <c r="K131">
+        <v>0</v>
+      </c>
+      <c r="L131">
+        <v>0</v>
+      </c>
+      <c r="M131" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>0</v>
+      </c>
+      <c r="B132">
+        <v>0</v>
+      </c>
+      <c r="C132">
+        <v>6.0738217814308201E-2</v>
+      </c>
+      <c r="D132">
+        <v>1</v>
+      </c>
+      <c r="E132">
+        <v>1</v>
+      </c>
+      <c r="F132">
+        <v>-0.104055189098392</v>
+      </c>
+      <c r="G132">
+        <v>1</v>
+      </c>
+      <c r="H132">
+        <v>0</v>
+      </c>
+      <c r="I132">
+        <v>1</v>
+      </c>
+      <c r="J132">
+        <v>0</v>
+      </c>
+      <c r="K132">
+        <v>1</v>
+      </c>
+      <c r="L132">
+        <v>1</v>
+      </c>
+      <c r="M132" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>0</v>
+      </c>
+      <c r="B133">
+        <v>1</v>
+      </c>
+      <c r="C133">
+        <v>-0.22789823849746699</v>
+      </c>
+      <c r="D133">
+        <v>0</v>
+      </c>
+      <c r="E133">
+        <v>0</v>
+      </c>
+      <c r="F133">
+        <v>-8.5016880706790705E-3</v>
+      </c>
+      <c r="G133">
+        <v>1</v>
+      </c>
+      <c r="H133">
+        <v>1</v>
+      </c>
+      <c r="I133">
+        <v>0</v>
+      </c>
+      <c r="J133">
+        <v>1</v>
+      </c>
+      <c r="K133">
+        <v>0</v>
+      </c>
+      <c r="L133">
+        <v>0</v>
+      </c>
+      <c r="M133" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>0</v>
+      </c>
+      <c r="B134">
+        <v>0</v>
+      </c>
+      <c r="C134">
+        <v>-3.8013183504730999E-2</v>
+      </c>
+      <c r="D134">
+        <v>1</v>
+      </c>
+      <c r="E134">
+        <v>1</v>
+      </c>
+      <c r="F134">
+        <v>-7.7462887875195702E-2</v>
+      </c>
+      <c r="G134">
+        <v>1</v>
+      </c>
+      <c r="H134">
+        <v>0</v>
+      </c>
+      <c r="I134">
+        <v>1</v>
+      </c>
+      <c r="J134">
+        <v>0</v>
+      </c>
+      <c r="K134">
+        <v>1</v>
+      </c>
+      <c r="L134">
+        <v>1</v>
+      </c>
+      <c r="M134" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>1</v>
+      </c>
+      <c r="B135">
+        <v>1</v>
+      </c>
+      <c r="C135">
+        <v>-5.3364465595300802E-2</v>
+      </c>
+      <c r="D135">
+        <v>0</v>
+      </c>
+      <c r="E135">
+        <v>0</v>
+      </c>
+      <c r="F135">
+        <v>-5.1054128281936796E-3</v>
+      </c>
+      <c r="G135">
+        <v>0</v>
+      </c>
+      <c r="H135">
+        <v>1</v>
+      </c>
+      <c r="I135">
+        <v>0</v>
+      </c>
+      <c r="J135">
+        <v>1</v>
+      </c>
+      <c r="K135">
+        <v>0</v>
+      </c>
+      <c r="L135">
+        <v>0</v>
+      </c>
+      <c r="M135" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>0</v>
+      </c>
+      <c r="B136">
+        <v>0</v>
+      </c>
+      <c r="C136">
+        <v>6.0156846920413502E-2</v>
+      </c>
+      <c r="D136">
+        <v>1</v>
+      </c>
+      <c r="E136">
+        <v>1</v>
+      </c>
+      <c r="F136">
+        <v>-9.7380944572685701E-2</v>
+      </c>
+      <c r="G136">
+        <v>1</v>
+      </c>
+      <c r="H136">
+        <v>0</v>
+      </c>
+      <c r="I136">
+        <v>1</v>
+      </c>
+      <c r="J136">
+        <v>0</v>
+      </c>
+      <c r="K136">
+        <v>1</v>
+      </c>
+      <c r="L136">
+        <v>1</v>
+      </c>
+      <c r="M136" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>0</v>
+      </c>
+      <c r="B137">
+        <v>1</v>
+      </c>
+      <c r="C137">
+        <v>-0.21314620281322399</v>
+      </c>
+      <c r="D137">
+        <v>0</v>
+      </c>
+      <c r="E137">
+        <v>0</v>
+      </c>
+      <c r="F137">
+        <v>5.0115291735105302E-2</v>
+      </c>
+      <c r="G137">
+        <v>1</v>
+      </c>
+      <c r="H137">
+        <v>1</v>
+      </c>
+      <c r="I137">
+        <v>0</v>
+      </c>
+      <c r="J137">
+        <v>1</v>
+      </c>
+      <c r="K137">
+        <v>0</v>
+      </c>
+      <c r="L137">
+        <v>0</v>
+      </c>
+      <c r="M137" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>0</v>
+      </c>
+      <c r="B138">
+        <v>0</v>
+      </c>
+      <c r="C138">
+        <v>9.1723723851644304E-2</v>
+      </c>
+      <c r="D138">
+        <v>1</v>
+      </c>
+      <c r="E138">
+        <v>1</v>
+      </c>
+      <c r="F138">
+        <v>-7.2693457748126605E-2</v>
+      </c>
+      <c r="G138">
+        <v>1</v>
+      </c>
+      <c r="H138">
+        <v>0</v>
+      </c>
+      <c r="I138">
+        <v>1</v>
+      </c>
+      <c r="J138">
+        <v>0</v>
+      </c>
+      <c r="K138">
+        <v>1</v>
+      </c>
+      <c r="L138">
+        <v>1</v>
+      </c>
+      <c r="M138" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>1</v>
+      </c>
+      <c r="B139">
+        <v>1</v>
+      </c>
+      <c r="C139">
+        <v>-3.2169778198787198E-2</v>
+      </c>
+      <c r="D139">
+        <v>0</v>
+      </c>
+      <c r="E139">
+        <v>0</v>
+      </c>
+      <c r="F139">
+        <v>-2.7072716051931298E-3</v>
+      </c>
+      <c r="G139">
+        <v>0</v>
+      </c>
+      <c r="H139">
+        <v>1</v>
+      </c>
+      <c r="I139">
+        <v>0</v>
+      </c>
+      <c r="J139">
+        <v>1</v>
+      </c>
+      <c r="K139">
+        <v>0</v>
+      </c>
+      <c r="L139">
+        <v>0</v>
+      </c>
+      <c r="M139" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>0</v>
+      </c>
+      <c r="B140">
+        <v>0</v>
+      </c>
+      <c r="C140">
+        <v>6.1722051235653497E-2</v>
+      </c>
+      <c r="D140">
+        <v>1</v>
+      </c>
+      <c r="E140">
+        <v>1</v>
+      </c>
+      <c r="F140">
+        <v>-0.10005958715931799</v>
+      </c>
+      <c r="G140">
+        <v>1</v>
+      </c>
+      <c r="H140">
+        <v>0</v>
+      </c>
+      <c r="I140">
+        <v>1</v>
+      </c>
+      <c r="J140">
+        <v>0</v>
+      </c>
+      <c r="K140">
+        <v>1</v>
+      </c>
+      <c r="L140">
+        <v>1</v>
+      </c>
+      <c r="M140" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>1</v>
+      </c>
+      <c r="B141">
+        <v>1</v>
+      </c>
+      <c r="C141">
+        <v>-2.66094643094196E-2</v>
+      </c>
+      <c r="D141">
+        <v>1</v>
+      </c>
+      <c r="E141">
+        <v>0</v>
+      </c>
+      <c r="F141">
+        <v>-0.14829029022474799</v>
+      </c>
+      <c r="G141">
+        <v>0</v>
+      </c>
+      <c r="H141">
+        <v>0</v>
+      </c>
+      <c r="I141">
+        <v>0</v>
+      </c>
+      <c r="J141">
+        <v>1</v>
+      </c>
+      <c r="K141">
+        <v>0</v>
+      </c>
+      <c r="L141">
+        <v>0</v>
+      </c>
+      <c r="M141" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>0</v>
+      </c>
+      <c r="B142">
+        <v>0</v>
+      </c>
+      <c r="C142">
+        <v>0.17433709262962199</v>
+      </c>
+      <c r="D142">
+        <v>1</v>
+      </c>
+      <c r="E142">
+        <v>1</v>
+      </c>
+      <c r="F142">
+        <v>-8.4066444941509194E-2</v>
+      </c>
+      <c r="G142">
+        <v>1</v>
+      </c>
+      <c r="H142">
+        <v>0</v>
+      </c>
+      <c r="I142">
+        <v>1</v>
+      </c>
+      <c r="J142">
+        <v>0</v>
+      </c>
+      <c r="K142">
+        <v>1</v>
+      </c>
+      <c r="L142">
+        <v>1</v>
+      </c>
+      <c r="M142" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>1</v>
+      </c>
+      <c r="B143">
+        <v>0</v>
+      </c>
+      <c r="C143">
+        <v>0.15558560892728601</v>
+      </c>
+      <c r="D143">
+        <v>0</v>
+      </c>
+      <c r="E143">
+        <v>0</v>
+      </c>
+      <c r="F143">
+        <v>-5.2135169105877503E-2</v>
+      </c>
+      <c r="G143">
+        <v>0</v>
+      </c>
+      <c r="H143">
+        <v>1</v>
+      </c>
+      <c r="I143">
+        <v>1</v>
+      </c>
+      <c r="J143">
+        <v>1</v>
+      </c>
+      <c r="K143">
+        <v>0</v>
+      </c>
+      <c r="L143">
+        <v>0</v>
+      </c>
+      <c r="M143" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>0</v>
+      </c>
+      <c r="B144">
+        <v>0</v>
+      </c>
+      <c r="C144">
+        <v>0.13966176000059</v>
+      </c>
+      <c r="D144">
+        <v>1</v>
+      </c>
+      <c r="E144">
+        <v>1</v>
+      </c>
+      <c r="F144">
+        <v>-5.8320479464493202E-2</v>
+      </c>
+      <c r="G144">
+        <v>1</v>
+      </c>
+      <c r="H144">
+        <v>0</v>
+      </c>
+      <c r="I144">
+        <v>1</v>
+      </c>
+      <c r="J144">
+        <v>0</v>
+      </c>
+      <c r="K144">
+        <v>1</v>
+      </c>
+      <c r="L144">
+        <v>1</v>
+      </c>
+      <c r="M144" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>1</v>
+      </c>
+      <c r="B145">
+        <v>1</v>
+      </c>
+      <c r="C145">
+        <v>-6.2948081545613696E-2</v>
+      </c>
+      <c r="D145">
+        <v>0</v>
+      </c>
+      <c r="E145">
+        <v>0</v>
+      </c>
+      <c r="F145">
+        <v>6.2765628564072806E-2</v>
+      </c>
+      <c r="G145">
+        <v>0</v>
+      </c>
+      <c r="H145">
+        <v>1</v>
+      </c>
+      <c r="I145">
+        <v>0</v>
+      </c>
+      <c r="J145">
+        <v>1</v>
+      </c>
+      <c r="K145">
+        <v>0</v>
+      </c>
+      <c r="L145">
+        <v>0</v>
+      </c>
+      <c r="M145" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>0</v>
+      </c>
+      <c r="B146">
+        <v>0</v>
+      </c>
+      <c r="C146">
+        <v>7.6136379406990903E-2</v>
+      </c>
+      <c r="D146">
+        <v>1</v>
+      </c>
+      <c r="E146">
+        <v>0</v>
+      </c>
+      <c r="F146">
+        <v>-0.18402015867107799</v>
+      </c>
+      <c r="G146">
+        <v>1</v>
+      </c>
+      <c r="H146">
+        <v>0</v>
+      </c>
+      <c r="I146">
+        <v>1</v>
+      </c>
+      <c r="J146">
+        <v>1</v>
+      </c>
+      <c r="K146">
+        <v>1</v>
+      </c>
+      <c r="L146">
+        <v>1</v>
+      </c>
+      <c r="M146" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>0</v>
+      </c>
+      <c r="B147">
+        <v>1</v>
+      </c>
+      <c r="C147">
+        <v>-0.238421736776155</v>
+      </c>
+      <c r="D147">
+        <v>0</v>
+      </c>
+      <c r="E147">
+        <v>0</v>
+      </c>
+      <c r="F147">
+        <v>0.10910741960003199</v>
+      </c>
+      <c r="G147">
+        <v>1</v>
+      </c>
+      <c r="H147">
+        <v>1</v>
+      </c>
+      <c r="I147">
+        <v>0</v>
+      </c>
+      <c r="J147">
+        <v>1</v>
+      </c>
+      <c r="K147">
+        <v>0</v>
+      </c>
+      <c r="L147">
+        <v>0</v>
+      </c>
+      <c r="M147" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>0</v>
+      </c>
+      <c r="B148">
+        <v>0</v>
+      </c>
+      <c r="C148">
+        <v>3.3508016505704799E-2</v>
+      </c>
+      <c r="D148">
+        <v>1</v>
+      </c>
+      <c r="E148">
+        <v>1</v>
+      </c>
+      <c r="F148">
+        <v>-8.43721776385392E-2</v>
+      </c>
+      <c r="G148">
+        <v>1</v>
+      </c>
+      <c r="H148">
+        <v>0</v>
+      </c>
+      <c r="I148">
+        <v>1</v>
+      </c>
+      <c r="J148">
+        <v>0</v>
+      </c>
+      <c r="K148">
+        <v>1</v>
+      </c>
+      <c r="L148">
+        <v>1</v>
+      </c>
+      <c r="M148" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>0</v>
+      </c>
+      <c r="B149">
+        <v>1</v>
+      </c>
+      <c r="C149">
+        <v>-0.23516440047833001</v>
+      </c>
+      <c r="D149">
+        <v>0</v>
+      </c>
+      <c r="E149">
+        <v>0</v>
+      </c>
+      <c r="F149">
+        <v>9.2530885586807596E-2</v>
+      </c>
+      <c r="G149">
+        <v>1</v>
+      </c>
+      <c r="H149">
+        <v>1</v>
+      </c>
+      <c r="I149">
+        <v>0</v>
+      </c>
+      <c r="J149">
+        <v>1</v>
+      </c>
+      <c r="K149">
+        <v>0</v>
+      </c>
+      <c r="L149">
+        <v>0</v>
+      </c>
+      <c r="M149" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>0</v>
+      </c>
+      <c r="B150">
+        <v>0</v>
+      </c>
+      <c r="C150">
+        <v>0.101548157707196</v>
+      </c>
+      <c r="D150">
+        <v>1</v>
+      </c>
+      <c r="E150">
+        <v>1</v>
+      </c>
+      <c r="F150">
+        <v>-0.107914633432386</v>
+      </c>
+      <c r="G150">
+        <v>1</v>
+      </c>
+      <c r="H150">
+        <v>0</v>
+      </c>
+      <c r="I150">
+        <v>1</v>
+      </c>
+      <c r="J150">
+        <v>0</v>
+      </c>
+      <c r="K150">
+        <v>1</v>
+      </c>
+      <c r="L150">
+        <v>1</v>
+      </c>
+      <c r="M150" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>1</v>
+      </c>
+      <c r="B151">
+        <v>1</v>
+      </c>
+      <c r="C151">
+        <v>-3.3522390965087898E-2</v>
+      </c>
+      <c r="D151">
+        <v>0</v>
+      </c>
+      <c r="E151">
+        <v>0</v>
+      </c>
+      <c r="F151">
+        <v>0.12868435928835401</v>
+      </c>
+      <c r="G151">
+        <v>0</v>
+      </c>
+      <c r="H151">
+        <v>1</v>
+      </c>
+      <c r="I151">
+        <v>0</v>
+      </c>
+      <c r="J151">
+        <v>1</v>
+      </c>
+      <c r="K151">
+        <v>0</v>
+      </c>
+      <c r="L151">
+        <v>0</v>
+      </c>
+      <c r="M151" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>0</v>
+      </c>
+      <c r="B152">
+        <v>0</v>
+      </c>
+      <c r="C152">
+        <v>2.90110895196236E-3</v>
+      </c>
+      <c r="D152">
+        <v>1</v>
+      </c>
+      <c r="E152">
+        <v>1</v>
+      </c>
+      <c r="F152">
+        <v>-0.105256093171753</v>
+      </c>
+      <c r="G152">
+        <v>1</v>
+      </c>
+      <c r="H152">
+        <v>0</v>
+      </c>
+      <c r="I152">
+        <v>1</v>
+      </c>
+      <c r="J152">
+        <v>0</v>
+      </c>
+      <c r="K152">
+        <v>1</v>
+      </c>
+      <c r="L152">
+        <v>1</v>
+      </c>
+      <c r="M152" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>0</v>
+      </c>
+      <c r="B153">
+        <v>1</v>
+      </c>
+      <c r="C153">
+        <v>-0.25344565376419098</v>
+      </c>
+      <c r="D153">
+        <v>0</v>
+      </c>
+      <c r="E153">
+        <v>0</v>
+      </c>
+      <c r="F153">
+        <v>9.1724783296486104E-2</v>
+      </c>
+      <c r="G153">
+        <v>1</v>
+      </c>
+      <c r="H153">
+        <v>1</v>
+      </c>
+      <c r="I153">
+        <v>0</v>
+      </c>
+      <c r="J153">
+        <v>1</v>
+      </c>
+      <c r="K153">
+        <v>0</v>
+      </c>
+      <c r="L153">
+        <v>0</v>
+      </c>
+      <c r="M153" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>0</v>
+      </c>
+      <c r="B154">
+        <v>0</v>
+      </c>
+      <c r="C154">
+        <v>7.4495432813834098E-2</v>
+      </c>
+      <c r="D154">
+        <v>1</v>
+      </c>
+      <c r="E154">
+        <v>1</v>
+      </c>
+      <c r="F154">
+        <v>-9.06559894852417E-2</v>
+      </c>
+      <c r="G154">
+        <v>1</v>
+      </c>
+      <c r="H154">
+        <v>0</v>
+      </c>
+      <c r="I154">
+        <v>1</v>
+      </c>
+      <c r="J154">
+        <v>0</v>
+      </c>
+      <c r="K154">
+        <v>1</v>
+      </c>
+      <c r="L154">
+        <v>1</v>
+      </c>
+      <c r="M154" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>0</v>
+      </c>
+      <c r="B155">
+        <v>1</v>
+      </c>
+      <c r="C155">
+        <v>-0.25189166772856703</v>
+      </c>
+      <c r="D155">
+        <v>1</v>
+      </c>
+      <c r="E155">
+        <v>0</v>
+      </c>
+      <c r="F155">
+        <v>-0.11693544356935499</v>
+      </c>
+      <c r="G155">
+        <v>1</v>
+      </c>
+      <c r="H155">
+        <v>0</v>
+      </c>
+      <c r="I155">
+        <v>0</v>
+      </c>
+      <c r="J155">
+        <v>1</v>
+      </c>
+      <c r="K155">
+        <v>0</v>
+      </c>
+      <c r="L155">
+        <v>0</v>
+      </c>
+      <c r="M155" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>0</v>
+      </c>
+      <c r="B156">
+        <v>0</v>
+      </c>
+      <c r="C156">
+        <v>6.47154504782054E-2</v>
+      </c>
+      <c r="D156">
+        <v>1</v>
+      </c>
+      <c r="E156">
+        <v>1</v>
+      </c>
+      <c r="F156">
+        <v>-9.1701864558186297E-2</v>
+      </c>
+      <c r="G156">
+        <v>1</v>
+      </c>
+      <c r="H156">
+        <v>0</v>
+      </c>
+      <c r="I156">
+        <v>1</v>
+      </c>
+      <c r="J156">
+        <v>0</v>
+      </c>
+      <c r="K156">
+        <v>1</v>
+      </c>
+      <c r="L156">
+        <v>1</v>
+      </c>
+      <c r="M156" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>1</v>
+      </c>
+      <c r="B157">
+        <v>1</v>
+      </c>
+      <c r="C157">
+        <v>-5.5094762879053502E-2</v>
+      </c>
+      <c r="D157">
+        <v>0</v>
+      </c>
+      <c r="E157">
+        <v>0</v>
+      </c>
+      <c r="F157">
+        <v>5.4971607092529899E-2</v>
+      </c>
+      <c r="G157">
+        <v>0</v>
+      </c>
+      <c r="H157">
+        <v>1</v>
+      </c>
+      <c r="I157">
+        <v>0</v>
+      </c>
+      <c r="J157">
+        <v>1</v>
+      </c>
+      <c r="K157">
+        <v>0</v>
+      </c>
+      <c r="L157">
+        <v>0</v>
+      </c>
+      <c r="M157" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -38551,10 +39658,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A75373D6-3132-4BE4-A918-2B1BB3855FDC}">
-  <dimension ref="A1:F130"/>
+  <dimension ref="A1:F157"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41159,6 +42266,546 @@
         <v>21</v>
       </c>
     </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>-2.3021396615663402E-2</v>
+      </c>
+      <c r="B131">
+        <v>-0.14308251083017601</v>
+      </c>
+      <c r="C131">
+        <v>0</v>
+      </c>
+      <c r="D131">
+        <v>0</v>
+      </c>
+      <c r="E131">
+        <v>0</v>
+      </c>
+      <c r="F131" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>6.0738217814308201E-2</v>
+      </c>
+      <c r="B132">
+        <v>-0.104055189098392</v>
+      </c>
+      <c r="C132">
+        <v>1</v>
+      </c>
+      <c r="D132">
+        <v>1</v>
+      </c>
+      <c r="E132">
+        <v>1</v>
+      </c>
+      <c r="F132" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>-0.22789823849746699</v>
+      </c>
+      <c r="B133">
+        <v>-8.5016880706790705E-3</v>
+      </c>
+      <c r="C133">
+        <v>1</v>
+      </c>
+      <c r="D133">
+        <v>0</v>
+      </c>
+      <c r="E133">
+        <v>0</v>
+      </c>
+      <c r="F133" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>-3.8013183504730999E-2</v>
+      </c>
+      <c r="B134">
+        <v>-7.7462887875195702E-2</v>
+      </c>
+      <c r="C134">
+        <v>1</v>
+      </c>
+      <c r="D134">
+        <v>1</v>
+      </c>
+      <c r="E134">
+        <v>1</v>
+      </c>
+      <c r="F134" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>-5.3364465595300802E-2</v>
+      </c>
+      <c r="B135">
+        <v>-5.1054128281936796E-3</v>
+      </c>
+      <c r="C135">
+        <v>0</v>
+      </c>
+      <c r="D135">
+        <v>0</v>
+      </c>
+      <c r="E135">
+        <v>0</v>
+      </c>
+      <c r="F135" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>6.0156846920413502E-2</v>
+      </c>
+      <c r="B136">
+        <v>-9.7380944572685701E-2</v>
+      </c>
+      <c r="C136">
+        <v>1</v>
+      </c>
+      <c r="D136">
+        <v>1</v>
+      </c>
+      <c r="E136">
+        <v>1</v>
+      </c>
+      <c r="F136" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>-0.21314620281322399</v>
+      </c>
+      <c r="B137">
+        <v>5.0115291735105302E-2</v>
+      </c>
+      <c r="C137">
+        <v>1</v>
+      </c>
+      <c r="D137">
+        <v>0</v>
+      </c>
+      <c r="E137">
+        <v>0</v>
+      </c>
+      <c r="F137" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>9.1723723851644304E-2</v>
+      </c>
+      <c r="B138">
+        <v>-7.2693457748126605E-2</v>
+      </c>
+      <c r="C138">
+        <v>1</v>
+      </c>
+      <c r="D138">
+        <v>1</v>
+      </c>
+      <c r="E138">
+        <v>1</v>
+      </c>
+      <c r="F138" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>-3.2169778198787198E-2</v>
+      </c>
+      <c r="B139">
+        <v>-2.7072716051931298E-3</v>
+      </c>
+      <c r="C139">
+        <v>0</v>
+      </c>
+      <c r="D139">
+        <v>0</v>
+      </c>
+      <c r="E139">
+        <v>0</v>
+      </c>
+      <c r="F139" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>6.1722051235653497E-2</v>
+      </c>
+      <c r="B140">
+        <v>-0.10005958715931799</v>
+      </c>
+      <c r="C140">
+        <v>1</v>
+      </c>
+      <c r="D140">
+        <v>1</v>
+      </c>
+      <c r="E140">
+        <v>1</v>
+      </c>
+      <c r="F140" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>-2.66094643094196E-2</v>
+      </c>
+      <c r="B141">
+        <v>-0.14829029022474799</v>
+      </c>
+      <c r="C141">
+        <v>0</v>
+      </c>
+      <c r="D141">
+        <v>0</v>
+      </c>
+      <c r="E141">
+        <v>0</v>
+      </c>
+      <c r="F141" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>0.17433709262962199</v>
+      </c>
+      <c r="B142">
+        <v>-8.4066444941509194E-2</v>
+      </c>
+      <c r="C142">
+        <v>1</v>
+      </c>
+      <c r="D142">
+        <v>1</v>
+      </c>
+      <c r="E142">
+        <v>1</v>
+      </c>
+      <c r="F142" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>0.15558560892728601</v>
+      </c>
+      <c r="B143">
+        <v>-5.2135169105877503E-2</v>
+      </c>
+      <c r="C143">
+        <v>0</v>
+      </c>
+      <c r="D143">
+        <v>0</v>
+      </c>
+      <c r="E143">
+        <v>0</v>
+      </c>
+      <c r="F143" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>0.13966176000059</v>
+      </c>
+      <c r="B144">
+        <v>-5.8320479464493202E-2</v>
+      </c>
+      <c r="C144">
+        <v>1</v>
+      </c>
+      <c r="D144">
+        <v>1</v>
+      </c>
+      <c r="E144">
+        <v>1</v>
+      </c>
+      <c r="F144" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>-6.2948081545613696E-2</v>
+      </c>
+      <c r="B145">
+        <v>6.2765628564072806E-2</v>
+      </c>
+      <c r="C145">
+        <v>0</v>
+      </c>
+      <c r="D145">
+        <v>0</v>
+      </c>
+      <c r="E145">
+        <v>0</v>
+      </c>
+      <c r="F145" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>7.6136379406990903E-2</v>
+      </c>
+      <c r="B146">
+        <v>-0.18402015867107799</v>
+      </c>
+      <c r="C146">
+        <v>1</v>
+      </c>
+      <c r="D146">
+        <v>1</v>
+      </c>
+      <c r="E146">
+        <v>1</v>
+      </c>
+      <c r="F146" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>-0.238421736776155</v>
+      </c>
+      <c r="B147">
+        <v>0.10910741960003199</v>
+      </c>
+      <c r="C147">
+        <v>1</v>
+      </c>
+      <c r="D147">
+        <v>0</v>
+      </c>
+      <c r="E147">
+        <v>0</v>
+      </c>
+      <c r="F147" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>3.3508016505704799E-2</v>
+      </c>
+      <c r="B148">
+        <v>-8.43721776385392E-2</v>
+      </c>
+      <c r="C148">
+        <v>1</v>
+      </c>
+      <c r="D148">
+        <v>1</v>
+      </c>
+      <c r="E148">
+        <v>1</v>
+      </c>
+      <c r="F148" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>-0.23516440047833001</v>
+      </c>
+      <c r="B149">
+        <v>9.2530885586807596E-2</v>
+      </c>
+      <c r="C149">
+        <v>1</v>
+      </c>
+      <c r="D149">
+        <v>0</v>
+      </c>
+      <c r="E149">
+        <v>0</v>
+      </c>
+      <c r="F149" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>0.101548157707196</v>
+      </c>
+      <c r="B150">
+        <v>-0.107914633432386</v>
+      </c>
+      <c r="C150">
+        <v>1</v>
+      </c>
+      <c r="D150">
+        <v>1</v>
+      </c>
+      <c r="E150">
+        <v>1</v>
+      </c>
+      <c r="F150" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>-3.3522390965087898E-2</v>
+      </c>
+      <c r="B151">
+        <v>0.12868435928835401</v>
+      </c>
+      <c r="C151">
+        <v>0</v>
+      </c>
+      <c r="D151">
+        <v>0</v>
+      </c>
+      <c r="E151">
+        <v>0</v>
+      </c>
+      <c r="F151" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>2.90110895196236E-3</v>
+      </c>
+      <c r="B152">
+        <v>-0.105256093171753</v>
+      </c>
+      <c r="C152">
+        <v>1</v>
+      </c>
+      <c r="D152">
+        <v>1</v>
+      </c>
+      <c r="E152">
+        <v>1</v>
+      </c>
+      <c r="F152" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>-0.25344565376419098</v>
+      </c>
+      <c r="B153">
+        <v>9.1724783296486104E-2</v>
+      </c>
+      <c r="C153">
+        <v>1</v>
+      </c>
+      <c r="D153">
+        <v>0</v>
+      </c>
+      <c r="E153">
+        <v>0</v>
+      </c>
+      <c r="F153" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>7.4495432813834098E-2</v>
+      </c>
+      <c r="B154">
+        <v>-9.06559894852417E-2</v>
+      </c>
+      <c r="C154">
+        <v>1</v>
+      </c>
+      <c r="D154">
+        <v>1</v>
+      </c>
+      <c r="E154">
+        <v>1</v>
+      </c>
+      <c r="F154" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>-0.25189166772856703</v>
+      </c>
+      <c r="B155">
+        <v>-0.11693544356935499</v>
+      </c>
+      <c r="C155">
+        <v>1</v>
+      </c>
+      <c r="D155">
+        <v>0</v>
+      </c>
+      <c r="E155">
+        <v>0</v>
+      </c>
+      <c r="F155" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>6.47154504782054E-2</v>
+      </c>
+      <c r="B156">
+        <v>-9.1701864558186297E-2</v>
+      </c>
+      <c r="C156">
+        <v>1</v>
+      </c>
+      <c r="D156">
+        <v>1</v>
+      </c>
+      <c r="E156">
+        <v>1</v>
+      </c>
+      <c r="F156" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>-5.5094762879053502E-2</v>
+      </c>
+      <c r="B157">
+        <v>5.4971607092529899E-2</v>
+      </c>
+      <c r="C157">
+        <v>0</v>
+      </c>
+      <c r="D157">
+        <v>0</v>
+      </c>
+      <c r="E157">
+        <v>0</v>
+      </c>
+      <c r="F157" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>